<commit_message>
Move zero 1st gen biofuel import year to 2025
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_Temporary_Fixes.xlsx
+++ b/SuppXLS/Scen_B_Temporary_Fixes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A7053A-52BD-457A-B706-AB5E3D0DEC18}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F49803A-243C-4746-834D-A87E61166701}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3233" yWindow="8002" windowWidth="20716" windowHeight="13276" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="15" r:id="rId1"/>
@@ -2631,7 +2631,7 @@
   <dimension ref="B3:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2696,7 +2696,7 @@
         <v>229</v>
       </c>
       <c r="E5">
-        <v>2018</v>
+        <v>2025</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -3007,8 +3007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{209CF89D-3AC9-4E2E-BCF6-79A710F8BD8A}">
   <dimension ref="A1:S173"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6235,7 +6235,7 @@
   <dimension ref="B3:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Disallow import of hydrogen in temporary fixes
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_Temporary_Fixes.xlsx
+++ b/SuppXLS/Scen_B_Temporary_Fixes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F49803A-243C-4746-834D-A87E61166701}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E547AB09-6FEC-43E5-BFAB-68469CB2085F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -123,7 +123,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1736" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1739" uniqueCount="236">
   <si>
     <t>UC_N</t>
   </si>
@@ -848,6 +848,9 @@
   </si>
   <si>
     <t>IMPBIO*1G*2,IMPBIO*1G*3,IMPBIO*1G*4</t>
+  </si>
+  <si>
+    <t>IMPH2G</t>
   </si>
 </sst>
 </file>
@@ -2628,10 +2631,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B3:L14"/>
+  <dimension ref="B3:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2801,7 +2804,7 @@
         <v>UP</v>
       </c>
       <c r="D14" t="str">
-        <f t="shared" ref="D14" si="1">D13</f>
+        <f t="shared" ref="D14:D16" si="1">D13</f>
         <v>ACT_BND</v>
       </c>
       <c r="E14">
@@ -2820,6 +2823,51 @@
       <c r="I14" t="str">
         <f>I13</f>
         <v>*GRID*</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>83</v>
+      </c>
+      <c r="D15" t="s">
+        <v>229</v>
+      </c>
+      <c r="E15">
+        <v>2030</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <f>F15</f>
+        <v>0</v>
+      </c>
+      <c r="I15" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C16" t="str">
+        <f>C15</f>
+        <v>UP</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="1"/>
+        <v>ACT_BND</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>5</v>
+      </c>
+      <c r="G16">
+        <f>F16</f>
+        <v>5</v>
+      </c>
+      <c r="I16" t="str">
+        <f>I15</f>
+        <v>IMPH2G</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Move START of wave and tidal to 2035
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_Temporary_Fixes.xlsx
+++ b/SuppXLS/Scen_B_Temporary_Fixes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E547AB09-6FEC-43E5-BFAB-68469CB2085F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A76F4CAD-B9F2-4C06-B2DF-DC2EE4854950}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="15" r:id="rId1"/>
@@ -123,7 +123,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1739" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1749" uniqueCount="237">
   <si>
     <t>UC_N</t>
   </si>
@@ -851,6 +851,9 @@
   </si>
   <si>
     <t>IMPH2G</t>
+  </si>
+  <si>
+    <t>P*OCE*</t>
   </si>
 </sst>
 </file>
@@ -2476,15 +2479,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE79BAD-EA44-47F0-A194-320DE6C9FB50}">
-  <dimension ref="B2:M11"/>
+  <dimension ref="B2:M15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2622,6 +2625,57 @@
       </c>
       <c r="I11" t="s">
         <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B13" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" s="11" t="str">
+        <f>IF(Regions!C$3&lt;&gt;"",Regions!C$3,"*")</f>
+        <v>IE</v>
+      </c>
+      <c r="G14" s="11" t="str">
+        <f>IF(Regions!D$3&lt;&gt;"",Regions!D$3,"*")</f>
+        <v>National</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>79</v>
+      </c>
+      <c r="F15">
+        <v>2035</v>
+      </c>
+      <c r="G15">
+        <f>F15</f>
+        <v>2035</v>
+      </c>
+      <c r="I15" t="s">
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -2633,7 +2687,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
SRV: Limit AFA of some HPs (temp fix)
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_Temporary_Fixes.xlsx
+++ b/SuppXLS/Scen_B_Temporary_Fixes.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HannahD\Documents\GitHub\Irish-TIMES-model\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C7559A6-E99A-4541-ADCD-F359C7E3A430}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{816AC58D-57D5-41C5-95C4-318FB35D770C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4530" yWindow="16050" windowWidth="19650" windowHeight="11070" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="15" r:id="rId1"/>
     <sheet name="PWR" sheetId="19" r:id="rId2"/>
     <sheet name="SUP" sheetId="11" r:id="rId3"/>
     <sheet name="SUP_biogas" sheetId="1" r:id="rId4"/>
-    <sheet name="RSD" sheetId="22" r:id="rId5"/>
-    <sheet name="DataFill" sheetId="23" r:id="rId6"/>
-    <sheet name="RSDAFC" sheetId="25" r:id="rId7"/>
-    <sheet name="RSDAFA" sheetId="24" r:id="rId8"/>
+    <sheet name="SRV" sheetId="26" r:id="rId5"/>
+    <sheet name="RSD" sheetId="22" r:id="rId6"/>
+    <sheet name="DataFill" sheetId="23" r:id="rId7"/>
+    <sheet name="RSDAFC" sheetId="25" r:id="rId8"/>
+    <sheet name="RSDAFA" sheetId="24" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="__123Graph_AEUMILKPN" hidden="1">#REF!</definedName>
@@ -136,7 +137,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1767" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1798" uniqueCount="246">
   <si>
     <t>UC_N</t>
   </si>
@@ -870,6 +871,30 @@
   </si>
   <si>
     <t>FT-RSDCOA</t>
+  </si>
+  <si>
+    <t>S-SH-CS_ELC_N1</t>
+  </si>
+  <si>
+    <t>S-SH-CS_ELC_N2</t>
+  </si>
+  <si>
+    <t>S-SH-CS_ELC_N4</t>
+  </si>
+  <si>
+    <t>S-SH-CS_ELC_N7</t>
+  </si>
+  <si>
+    <t>S-SH-PU_ELC_N1</t>
+  </si>
+  <si>
+    <t>S-SH-PU_ELC_N2</t>
+  </si>
+  <si>
+    <t>S-SH-PU_ELC_N4</t>
+  </si>
+  <si>
+    <t>S-SH-PU_ELC_N7</t>
   </si>
 </sst>
 </file>
@@ -2704,7 +2729,7 @@
   <dimension ref="B3:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="B11" sqref="B11:I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2950,7 +2975,7 @@
   <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14:L16"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3122,10 +3147,232 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F532AC2E-E047-4124-A56C-AD8CA9B97A1E}">
+  <dimension ref="B3:I12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+    </row>
+    <row r="4" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="11" t="str">
+        <f>IF(Regions!C$3&lt;&gt;"",Regions!C$3,"*")</f>
+        <v>IE</v>
+      </c>
+      <c r="G4" s="11" t="str">
+        <f>IF(Regions!C$3&lt;&gt;"",Regions!D$3,"*")</f>
+        <v>National</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D5" t="s">
+        <v>110</v>
+      </c>
+      <c r="E5">
+        <v>2018</v>
+      </c>
+      <c r="F5">
+        <v>0.115</v>
+      </c>
+      <c r="G5">
+        <f>F5</f>
+        <v>0.115</v>
+      </c>
+      <c r="I5" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" t="s">
+        <v>110</v>
+      </c>
+      <c r="E6">
+        <v>2018</v>
+      </c>
+      <c r="F6">
+        <v>0.115</v>
+      </c>
+      <c r="G6">
+        <f t="shared" ref="G6:G12" si="0">F6</f>
+        <v>0.115</v>
+      </c>
+      <c r="I6" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" t="s">
+        <v>110</v>
+      </c>
+      <c r="E7">
+        <v>2018</v>
+      </c>
+      <c r="F7">
+        <v>0.115</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>0.115</v>
+      </c>
+      <c r="I7" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" t="s">
+        <v>110</v>
+      </c>
+      <c r="E8">
+        <v>2018</v>
+      </c>
+      <c r="F8">
+        <v>0.115</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>0.115</v>
+      </c>
+      <c r="I8" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D9" t="s">
+        <v>110</v>
+      </c>
+      <c r="E9">
+        <v>2018</v>
+      </c>
+      <c r="F9">
+        <v>0.115</v>
+      </c>
+      <c r="G9">
+        <f>F9</f>
+        <v>0.115</v>
+      </c>
+      <c r="I9" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D10" t="s">
+        <v>110</v>
+      </c>
+      <c r="E10">
+        <v>2018</v>
+      </c>
+      <c r="F10">
+        <v>0.115</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>0.115</v>
+      </c>
+      <c r="I10" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" t="s">
+        <v>110</v>
+      </c>
+      <c r="E11">
+        <v>2018</v>
+      </c>
+      <c r="F11">
+        <v>0.115</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>0.115</v>
+      </c>
+      <c r="I11" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" t="s">
+        <v>110</v>
+      </c>
+      <c r="E12">
+        <v>2018</v>
+      </c>
+      <c r="F12">
+        <v>0.115</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>0.115</v>
+      </c>
+      <c r="I12" t="s">
+        <v>245</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{209CF89D-3AC9-4E2E-BCF6-79A710F8BD8A}">
   <dimension ref="A1:S182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
@@ -6469,7 +6716,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB6377ED-B160-4F16-923E-B56DAAEBF3A1}">
   <dimension ref="B3:I9"/>
   <sheetViews>
@@ -6597,7 +6844,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2A6683C-C57D-4A33-B9D9-D05BA0CBEA1C}">
   <dimension ref="A1:M93"/>
   <sheetViews>
@@ -10431,7 +10678,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D772440E-5AFD-47E0-A6C0-EF255248451F}">
   <dimension ref="A1:M31"/>
   <sheetViews>

</xml_diff>

<commit_message>
Limit peat in RSD to 2018 values
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_Temporary_Fixes.xlsx
+++ b/SuppXLS/Scen_B_Temporary_Fixes.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HannahD\Documents\GitHub\Irish-TIMES-model\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C7559A6-E99A-4541-ADCD-F359C7E3A430}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FEF21E0-C74D-4E7E-89B4-409302323446}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4530" yWindow="16050" windowWidth="19650" windowHeight="11070" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="15" r:id="rId1"/>
     <sheet name="PWR" sheetId="19" r:id="rId2"/>
     <sheet name="SUP" sheetId="11" r:id="rId3"/>
     <sheet name="SUP_biogas" sheetId="1" r:id="rId4"/>
-    <sheet name="RSD" sheetId="22" r:id="rId5"/>
-    <sheet name="DataFill" sheetId="23" r:id="rId6"/>
-    <sheet name="RSDAFC" sheetId="25" r:id="rId7"/>
-    <sheet name="RSDAFA" sheetId="24" r:id="rId8"/>
+    <sheet name="SRV" sheetId="26" r:id="rId5"/>
+    <sheet name="RSD" sheetId="22" r:id="rId6"/>
+    <sheet name="DataFill" sheetId="23" r:id="rId7"/>
+    <sheet name="RSDAFC" sheetId="25" r:id="rId8"/>
+    <sheet name="RSDAFA" sheetId="24" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="__123Graph_AEUMILKPN" hidden="1">#REF!</definedName>
@@ -96,7 +97,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I32" authorId="0" shapeId="0" xr:uid="{9FF5C6AC-B75C-4529-857A-E9C78B6E0755}">
+    <comment ref="I33" authorId="0" shapeId="0" xr:uid="{9FF5C6AC-B75C-4529-857A-E9C78B6E0755}">
       <text>
         <r>
           <rPr>
@@ -136,7 +137,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1767" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1807" uniqueCount="247">
   <si>
     <t>UC_N</t>
   </si>
@@ -870,6 +871,33 @@
   </si>
   <si>
     <t>FT-RSDCOA</t>
+  </si>
+  <si>
+    <t>S-SH-CS_ELC_N1</t>
+  </si>
+  <si>
+    <t>S-SH-CS_ELC_N2</t>
+  </si>
+  <si>
+    <t>S-SH-CS_ELC_N4</t>
+  </si>
+  <si>
+    <t>S-SH-CS_ELC_N7</t>
+  </si>
+  <si>
+    <t>S-SH-PU_ELC_N1</t>
+  </si>
+  <si>
+    <t>S-SH-PU_ELC_N2</t>
+  </si>
+  <si>
+    <t>S-SH-PU_ELC_N4</t>
+  </si>
+  <si>
+    <t>S-SH-PU_ELC_N7</t>
+  </si>
+  <si>
+    <t>FT-RSDPEA</t>
   </si>
 </sst>
 </file>
@@ -2704,7 +2732,7 @@
   <dimension ref="B3:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="B11" sqref="B11:I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2950,7 +2978,7 @@
   <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14:L16"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3122,11 +3150,233 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F532AC2E-E047-4124-A56C-AD8CA9B97A1E}">
+  <dimension ref="B3:I12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+    </row>
+    <row r="4" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="11" t="str">
+        <f>IF(Regions!C$3&lt;&gt;"",Regions!C$3,"*")</f>
+        <v>IE</v>
+      </c>
+      <c r="G4" s="11" t="str">
+        <f>IF(Regions!C$3&lt;&gt;"",Regions!D$3,"*")</f>
+        <v>National</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D5" t="s">
+        <v>110</v>
+      </c>
+      <c r="E5">
+        <v>2018</v>
+      </c>
+      <c r="F5">
+        <v>0.115</v>
+      </c>
+      <c r="G5">
+        <f>F5</f>
+        <v>0.115</v>
+      </c>
+      <c r="I5" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" t="s">
+        <v>110</v>
+      </c>
+      <c r="E6">
+        <v>2018</v>
+      </c>
+      <c r="F6">
+        <v>0.115</v>
+      </c>
+      <c r="G6">
+        <f t="shared" ref="G6:G12" si="0">F6</f>
+        <v>0.115</v>
+      </c>
+      <c r="I6" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" t="s">
+        <v>110</v>
+      </c>
+      <c r="E7">
+        <v>2018</v>
+      </c>
+      <c r="F7">
+        <v>0.115</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>0.115</v>
+      </c>
+      <c r="I7" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" t="s">
+        <v>110</v>
+      </c>
+      <c r="E8">
+        <v>2018</v>
+      </c>
+      <c r="F8">
+        <v>0.115</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>0.115</v>
+      </c>
+      <c r="I8" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D9" t="s">
+        <v>110</v>
+      </c>
+      <c r="E9">
+        <v>2018</v>
+      </c>
+      <c r="F9">
+        <v>0.115</v>
+      </c>
+      <c r="G9">
+        <f>F9</f>
+        <v>0.115</v>
+      </c>
+      <c r="I9" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D10" t="s">
+        <v>110</v>
+      </c>
+      <c r="E10">
+        <v>2018</v>
+      </c>
+      <c r="F10">
+        <v>0.115</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>0.115</v>
+      </c>
+      <c r="I10" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" t="s">
+        <v>110</v>
+      </c>
+      <c r="E11">
+        <v>2018</v>
+      </c>
+      <c r="F11">
+        <v>0.115</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>0.115</v>
+      </c>
+      <c r="I11" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" t="s">
+        <v>110</v>
+      </c>
+      <c r="E12">
+        <v>2018</v>
+      </c>
+      <c r="F12">
+        <v>0.115</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>0.115</v>
+      </c>
+      <c r="I12" t="s">
+        <v>245</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{209CF89D-3AC9-4E2E-BCF6-79A710F8BD8A}">
-  <dimension ref="A1:S182"/>
+  <dimension ref="A1:S183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L44" sqref="L44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3649,84 +3899,113 @@
       </c>
     </row>
     <row r="28" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="H28" s="26"/>
-      <c r="I28" s="26"/>
+      <c r="C28" t="s">
+        <v>83</v>
+      </c>
+      <c r="D28" t="s">
+        <v>229</v>
+      </c>
+      <c r="E28">
+        <v>2020</v>
+      </c>
+      <c r="H28">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="I28">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="K28" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="29" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
+      <c r="C29" t="s">
+        <v>83</v>
+      </c>
+      <c r="D29" t="s">
+        <v>229</v>
+      </c>
+      <c r="E29">
+        <v>2030</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="K29" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="30" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="H30" s="26"/>
-      <c r="I30" s="26"/>
+      <c r="C30" t="s">
+        <v>83</v>
+      </c>
+      <c r="D30" t="s">
+        <v>229</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>5</v>
+      </c>
+      <c r="I30">
+        <v>5</v>
+      </c>
+      <c r="K30" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="31" spans="2:19" x14ac:dyDescent="0.25">
       <c r="H31" s="26"/>
       <c r="I31" s="26"/>
     </row>
     <row r="32" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B32" s="7" t="s">
+      <c r="H32" s="26"/>
+      <c r="I32" s="26"/>
+    </row>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B33" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="I32" s="8"/>
-      <c r="J32" s="9"/>
-      <c r="K32" s="9"/>
-    </row>
-    <row r="33" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="10" t="s">
+      <c r="I33" s="8"/>
+      <c r="J33" s="9"/>
+      <c r="K33" s="9"/>
+    </row>
+    <row r="34" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C34" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D33" s="10" t="s">
+      <c r="D34" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E33" s="10" t="s">
+      <c r="E34" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F33" s="10" t="s">
+      <c r="F34" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G33" s="10" t="s">
+      <c r="G34" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="H33" s="11" t="str">
+      <c r="H34" s="11" t="str">
         <f>IF(Regions!C$3&lt;&gt;"",Regions!C$3,"*")</f>
         <v>IE</v>
       </c>
-      <c r="I33" s="11" t="str">
+      <c r="I34" s="11" t="str">
         <f>IF(Regions!D$3&lt;&gt;"",Regions!D$3,"*")</f>
         <v>National</v>
       </c>
-      <c r="J33" s="12" t="s">
+      <c r="J34" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="K33" s="12" t="s">
+      <c r="K34" s="12" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C34" t="s">
-        <v>208</v>
-      </c>
-      <c r="D34" t="s">
-        <v>110</v>
-      </c>
-      <c r="H34">
-        <v>5</v>
-      </c>
-      <c r="I34">
-        <v>5</v>
-      </c>
-      <c r="J34" t="s">
-        <v>109</v>
-      </c>
-      <c r="K34" t="s">
-        <v>108</v>
-      </c>
-      <c r="M34" s="25">
-        <v>0.5</v>
       </c>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.25">
@@ -3736,1182 +4015,1180 @@
       <c r="D35" t="s">
         <v>110</v>
       </c>
-      <c r="H35" s="26">
-        <f>RSDAFC!L2*$M$34</f>
+      <c r="H35">
+        <v>5</v>
+      </c>
+      <c r="I35">
+        <v>5</v>
+      </c>
+      <c r="J35" t="s">
+        <v>109</v>
+      </c>
+      <c r="K35" t="s">
+        <v>108</v>
+      </c>
+      <c r="M35" s="25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>208</v>
+      </c>
+      <c r="D36" t="s">
+        <v>110</v>
+      </c>
+      <c r="H36" s="26">
+        <f>RSDAFC!L2*$M$35</f>
         <v>1.2406827591965401E-2</v>
       </c>
-      <c r="I35" s="26">
-        <f>RSDAFC!M2*$M$34</f>
+      <c r="I36" s="26">
+        <f>RSDAFC!M2*$M$35</f>
         <v>1.2406827591965401E-2</v>
       </c>
-      <c r="K35" t="str">
+      <c r="K36" t="str">
         <f>RSDAFC!C2</f>
         <v>R-HC_Apt_ELC_HPN1</v>
       </c>
     </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
-        <v>208</v>
-      </c>
-      <c r="D36" t="s">
-        <v>110</v>
-      </c>
-      <c r="H36" s="26">
-        <f>RSDAFC!L3*$M$34</f>
+    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>208</v>
+      </c>
+      <c r="D37" t="s">
+        <v>110</v>
+      </c>
+      <c r="H37" s="26">
+        <f>RSDAFC!L3*$M$35</f>
         <v>1.2406827591965401E-2</v>
       </c>
-      <c r="I36" s="26">
-        <f>RSDAFC!M3*$M$34</f>
+      <c r="I37" s="26">
+        <f>RSDAFC!M3*$M$35</f>
         <v>1.2406827591965401E-2</v>
       </c>
-      <c r="K36" t="str">
+      <c r="K37" t="str">
         <f>RSDAFC!C3</f>
         <v>R-HC_Apt_ELC_HPN1</v>
       </c>
     </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C37" t="s">
-        <v>208</v>
-      </c>
-      <c r="D37" t="s">
-        <v>110</v>
-      </c>
-      <c r="H37" s="26">
-        <f>RSDAFC!L4*$M$34</f>
+    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>208</v>
+      </c>
+      <c r="D38" t="s">
+        <v>110</v>
+      </c>
+      <c r="H38" s="26">
+        <f>RSDAFC!L4*$M$35</f>
         <v>1.2406827591965401E-2</v>
       </c>
-      <c r="I37" s="26">
-        <f>RSDAFC!M4*$M$34</f>
+      <c r="I38" s="26">
+        <f>RSDAFC!M4*$M$35</f>
         <v>1.2406827591965401E-2</v>
       </c>
-      <c r="K37" t="str">
+      <c r="K38" t="str">
         <f>RSDAFC!C4</f>
         <v>R-HC_Apt_ELC_HPN2</v>
       </c>
     </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C38" t="s">
-        <v>208</v>
-      </c>
-      <c r="D38" t="s">
-        <v>110</v>
-      </c>
-      <c r="H38" s="26">
-        <f>RSDAFC!L5*$M$34</f>
+    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>208</v>
+      </c>
+      <c r="D39" t="s">
+        <v>110</v>
+      </c>
+      <c r="H39" s="26">
+        <f>RSDAFC!L5*$M$35</f>
         <v>1.2406827591965401E-2</v>
       </c>
-      <c r="I38" s="26">
-        <f>RSDAFC!M5*$M$34</f>
+      <c r="I39" s="26">
+        <f>RSDAFC!M5*$M$35</f>
         <v>1.2406827591965401E-2</v>
       </c>
-      <c r="K38" t="str">
+      <c r="K39" t="str">
         <f>RSDAFC!C5</f>
         <v>R-HC_Apt_ELC_HPN2</v>
       </c>
     </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C39" t="s">
-        <v>208</v>
-      </c>
-      <c r="D39" t="s">
-        <v>110</v>
-      </c>
-      <c r="H39" s="26">
-        <f>RSDAFC!L6*$M$34</f>
+    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>208</v>
+      </c>
+      <c r="D40" t="s">
+        <v>110</v>
+      </c>
+      <c r="H40" s="26">
+        <f>RSDAFC!L6*$M$35</f>
         <v>8.6842891028111498E-3</v>
       </c>
-      <c r="I39" s="26">
-        <f>RSDAFC!M6*$M$34</f>
+      <c r="I40" s="26">
+        <f>RSDAFC!M6*$M$35</f>
         <v>8.6842891028111498E-3</v>
       </c>
-      <c r="K39" t="str">
+      <c r="K40" t="str">
         <f>RSDAFC!C6</f>
         <v>R-HC_Att_ELC_HPN1</v>
       </c>
     </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C40" t="s">
-        <v>208</v>
-      </c>
-      <c r="D40" t="s">
-        <v>110</v>
-      </c>
-      <c r="H40" s="26">
-        <f>RSDAFC!L7*$M$34</f>
+    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>208</v>
+      </c>
+      <c r="D41" t="s">
+        <v>110</v>
+      </c>
+      <c r="H41" s="26">
+        <f>RSDAFC!L7*$M$35</f>
         <v>8.6842891028111498E-3</v>
       </c>
-      <c r="I40" s="26">
-        <f>RSDAFC!M7*$M$34</f>
+      <c r="I41" s="26">
+        <f>RSDAFC!M7*$M$35</f>
         <v>8.6842891028111498E-3</v>
       </c>
-      <c r="K40" t="str">
+      <c r="K41" t="str">
         <f>RSDAFC!C7</f>
         <v>R-HC_Att_ELC_HPN1</v>
       </c>
     </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
-        <v>208</v>
-      </c>
-      <c r="D41" t="s">
-        <v>110</v>
-      </c>
-      <c r="H41" s="26">
-        <f>RSDAFC!L8*$M$34</f>
+    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>208</v>
+      </c>
+      <c r="D42" t="s">
+        <v>110</v>
+      </c>
+      <c r="H42" s="26">
+        <f>RSDAFC!L8*$M$35</f>
         <v>8.6842891028111498E-3</v>
       </c>
-      <c r="I41" s="26">
-        <f>RSDAFC!M8*$M$34</f>
+      <c r="I42" s="26">
+        <f>RSDAFC!M8*$M$35</f>
         <v>8.6842891028111498E-3</v>
       </c>
-      <c r="K41" t="str">
+      <c r="K42" t="str">
         <f>RSDAFC!C8</f>
         <v>R-HC_Att_ELC_HPN2</v>
       </c>
     </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C42" t="s">
-        <v>208</v>
-      </c>
-      <c r="D42" t="s">
-        <v>110</v>
-      </c>
-      <c r="H42" s="26">
-        <f>RSDAFC!L9*$M$34</f>
+    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>208</v>
+      </c>
+      <c r="D43" t="s">
+        <v>110</v>
+      </c>
+      <c r="H43" s="26">
+        <f>RSDAFC!L9*$M$35</f>
         <v>8.6842891028111498E-3</v>
       </c>
-      <c r="I42" s="26">
-        <f>RSDAFC!M9*$M$34</f>
+      <c r="I43" s="26">
+        <f>RSDAFC!M9*$M$35</f>
         <v>8.6842891028111498E-3</v>
       </c>
-      <c r="K42" t="str">
+      <c r="K43" t="str">
         <f>RSDAFC!C9</f>
         <v>R-HC_Att_ELC_HPN2</v>
       </c>
     </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C43" t="s">
-        <v>208</v>
-      </c>
-      <c r="D43" t="s">
-        <v>110</v>
-      </c>
-      <c r="H43" s="26">
-        <f>RSDAFC!L10*$M$34</f>
+    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>208</v>
+      </c>
+      <c r="D44" t="s">
+        <v>110</v>
+      </c>
+      <c r="H44" s="26">
+        <f>RSDAFC!L10*$M$35</f>
         <v>1.58935057836939E-2</v>
       </c>
-      <c r="I43" s="26">
-        <f>RSDAFC!M10*$M$34</f>
+      <c r="I44" s="26">
+        <f>RSDAFC!M10*$M$35</f>
         <v>1.58935057836939E-2</v>
       </c>
-      <c r="K43" t="str">
+      <c r="K44" t="str">
         <f>RSDAFC!C10</f>
         <v>R-HC_Det_ELC_HPN1</v>
       </c>
     </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C44" t="s">
-        <v>208</v>
-      </c>
-      <c r="D44" t="s">
-        <v>110</v>
-      </c>
-      <c r="H44" s="26">
-        <f>RSDAFC!L11*$M$34</f>
+    <row r="45" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>208</v>
+      </c>
+      <c r="D45" t="s">
+        <v>110</v>
+      </c>
+      <c r="H45" s="26">
+        <f>RSDAFC!L11*$M$35</f>
         <v>1.58935057836939E-2</v>
       </c>
-      <c r="I44" s="26">
-        <f>RSDAFC!M11*$M$34</f>
+      <c r="I45" s="26">
+        <f>RSDAFC!M11*$M$35</f>
         <v>1.58935057836939E-2</v>
       </c>
-      <c r="K44" t="str">
+      <c r="K45" t="str">
         <f>RSDAFC!C11</f>
         <v>R-HC_Det_ELC_HPN1</v>
       </c>
     </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C45" t="s">
-        <v>208</v>
-      </c>
-      <c r="D45" t="s">
-        <v>110</v>
-      </c>
-      <c r="H45" s="26">
-        <f>RSDAFC!L12*$M$34</f>
+    <row r="46" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>208</v>
+      </c>
+      <c r="D46" t="s">
+        <v>110</v>
+      </c>
+      <c r="H46" s="26">
+        <f>RSDAFC!L12*$M$35</f>
         <v>1.58935057836939E-2</v>
       </c>
-      <c r="I45" s="26">
-        <f>RSDAFC!M12*$M$34</f>
+      <c r="I46" s="26">
+        <f>RSDAFC!M12*$M$35</f>
         <v>1.58935057836939E-2</v>
       </c>
-      <c r="K45" t="str">
+      <c r="K46" t="str">
         <f>RSDAFC!C12</f>
         <v>R-HC_Det_ELC_HPN2</v>
       </c>
     </row>
-    <row r="46" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C46" t="s">
-        <v>208</v>
-      </c>
-      <c r="D46" t="s">
-        <v>110</v>
-      </c>
-      <c r="H46" s="26">
-        <f>RSDAFC!L13*$M$34</f>
+    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>208</v>
+      </c>
+      <c r="D47" t="s">
+        <v>110</v>
+      </c>
+      <c r="H47" s="26">
+        <f>RSDAFC!L13*$M$35</f>
         <v>1.58935057836939E-2</v>
       </c>
-      <c r="I46" s="26">
-        <f>RSDAFC!M13*$M$34</f>
+      <c r="I47" s="26">
+        <f>RSDAFC!M13*$M$35</f>
         <v>1.58935057836939E-2</v>
       </c>
-      <c r="K46" t="str">
+      <c r="K47" t="str">
         <f>RSDAFC!C13</f>
         <v>R-HC_Det_ELC_HPN2</v>
       </c>
     </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C47" t="s">
-        <v>208</v>
-      </c>
-      <c r="D47" t="s">
-        <v>110</v>
-      </c>
-      <c r="H47" s="26">
-        <f>RSDAFC!L14*$M$34</f>
+    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>208</v>
+      </c>
+      <c r="D48" t="s">
+        <v>110</v>
+      </c>
+      <c r="H48" s="26">
+        <f>RSDAFC!L14*$M$35</f>
         <v>1.04804159170382E-2</v>
       </c>
-      <c r="I47" s="26">
-        <f>RSDAFC!M14*$M$34</f>
+      <c r="I48" s="26">
+        <f>RSDAFC!M14*$M$35</f>
         <v>1.04804159170382E-2</v>
       </c>
-      <c r="K47" t="str">
+      <c r="K48" t="str">
         <f>RSDAFC!C14</f>
         <v>R-SW_Apt_ELC_HPN1</v>
       </c>
     </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C48" t="s">
-        <v>208</v>
-      </c>
-      <c r="D48" t="s">
-        <v>110</v>
-      </c>
-      <c r="H48" s="26">
-        <f>RSDAFC!L15*$M$34</f>
+    <row r="49" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>208</v>
+      </c>
+      <c r="D49" t="s">
+        <v>110</v>
+      </c>
+      <c r="H49" s="26">
+        <f>RSDAFC!L15*$M$35</f>
         <v>1.04804159170382E-2</v>
       </c>
-      <c r="I48" s="26">
-        <f>RSDAFC!M15*$M$34</f>
+      <c r="I49" s="26">
+        <f>RSDAFC!M15*$M$35</f>
         <v>1.04804159170382E-2</v>
       </c>
-      <c r="K48" t="str">
+      <c r="K49" t="str">
         <f>RSDAFC!C15</f>
         <v>R-SW_Apt_ELC_HPN1</v>
       </c>
     </row>
-    <row r="49" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C49" t="s">
-        <v>208</v>
-      </c>
-      <c r="D49" t="s">
-        <v>110</v>
-      </c>
-      <c r="H49" s="26">
-        <f>RSDAFC!L16*$M$34</f>
+    <row r="50" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>208</v>
+      </c>
+      <c r="D50" t="s">
+        <v>110</v>
+      </c>
+      <c r="H50" s="26">
+        <f>RSDAFC!L16*$M$35</f>
         <v>4.7397506033708351E-3</v>
       </c>
-      <c r="I49" s="26">
-        <f>RSDAFC!M16*$M$34</f>
+      <c r="I50" s="26">
+        <f>RSDAFC!M16*$M$35</f>
         <v>4.7397506033708351E-3</v>
       </c>
-      <c r="K49" t="str">
+      <c r="K50" t="str">
         <f>RSDAFC!C16</f>
         <v>R-SW_Apt_GAS_HHPN1</v>
       </c>
     </row>
-    <row r="50" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C50" t="s">
-        <v>208</v>
-      </c>
-      <c r="D50" t="s">
-        <v>110</v>
-      </c>
-      <c r="H50" s="26">
-        <f>RSDAFC!L17*$M$34</f>
+    <row r="51" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>208</v>
+      </c>
+      <c r="D51" t="s">
+        <v>110</v>
+      </c>
+      <c r="H51" s="26">
+        <f>RSDAFC!L17*$M$35</f>
         <v>4.7397506033708351E-3</v>
       </c>
-      <c r="I50" s="26">
-        <f>RSDAFC!M17*$M$34</f>
+      <c r="I51" s="26">
+        <f>RSDAFC!M17*$M$35</f>
         <v>4.7397506033708351E-3</v>
       </c>
-      <c r="K50" t="str">
+      <c r="K51" t="str">
         <f>RSDAFC!C17</f>
         <v>R-SW_Apt_GAS_HHPN1</v>
       </c>
     </row>
-    <row r="51" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C51" t="s">
-        <v>208</v>
-      </c>
-      <c r="D51" t="s">
-        <v>110</v>
-      </c>
-      <c r="H51" s="26">
-        <f>RSDAFC!L18*$M$34</f>
+    <row r="52" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>208</v>
+      </c>
+      <c r="D52" t="s">
+        <v>110</v>
+      </c>
+      <c r="H52" s="26">
+        <f>RSDAFC!L18*$M$35</f>
         <v>4.7397506033708351E-3</v>
       </c>
-      <c r="I51" s="26">
-        <f>RSDAFC!M18*$M$34</f>
+      <c r="I52" s="26">
+        <f>RSDAFC!M18*$M$35</f>
         <v>4.7397506033708351E-3</v>
       </c>
-      <c r="K51" t="str">
+      <c r="K52" t="str">
         <f>RSDAFC!C18</f>
         <v>R-SW_Apt_GAS_HPN1</v>
       </c>
     </row>
-    <row r="52" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C52" t="s">
-        <v>208</v>
-      </c>
-      <c r="D52" t="s">
-        <v>110</v>
-      </c>
-      <c r="H52" s="26">
-        <f>RSDAFC!L19*$M$34</f>
+    <row r="53" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>208</v>
+      </c>
+      <c r="D53" t="s">
+        <v>110</v>
+      </c>
+      <c r="H53" s="26">
+        <f>RSDAFC!L19*$M$35</f>
         <v>4.7397506033708351E-3</v>
       </c>
-      <c r="I52" s="26">
-        <f>RSDAFC!M19*$M$34</f>
+      <c r="I53" s="26">
+        <f>RSDAFC!M19*$M$35</f>
         <v>4.7397506033708351E-3</v>
       </c>
-      <c r="K52" t="str">
+      <c r="K53" t="str">
         <f>RSDAFC!C19</f>
         <v>R-SW_Apt_GAS_HPN1</v>
       </c>
     </row>
-    <row r="53" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C53" t="s">
-        <v>208</v>
-      </c>
-      <c r="D53" t="s">
-        <v>110</v>
-      </c>
-      <c r="H53" s="26">
-        <f>RSDAFC!L20*$M$34</f>
+    <row r="54" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>208</v>
+      </c>
+      <c r="D54" t="s">
+        <v>110</v>
+      </c>
+      <c r="H54" s="26">
+        <f>RSDAFC!L20*$M$35</f>
         <v>4.7397506033708351E-3</v>
       </c>
-      <c r="I53" s="26">
-        <f>RSDAFC!M20*$M$34</f>
+      <c r="I54" s="26">
+        <f>RSDAFC!M20*$M$35</f>
         <v>4.7397506033708351E-3</v>
       </c>
-      <c r="K53" t="str">
+      <c r="K54" t="str">
         <f>RSDAFC!C20</f>
         <v>R-SW_Apt_GAS_HPN2</v>
       </c>
     </row>
-    <row r="54" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C54" t="s">
-        <v>208</v>
-      </c>
-      <c r="D54" t="s">
-        <v>110</v>
-      </c>
-      <c r="H54" s="26">
-        <f>RSDAFC!L21*$M$34</f>
+    <row r="55" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>208</v>
+      </c>
+      <c r="D55" t="s">
+        <v>110</v>
+      </c>
+      <c r="H55" s="26">
+        <f>RSDAFC!L21*$M$35</f>
         <v>4.7397506033708351E-3</v>
       </c>
-      <c r="I54" s="26">
-        <f>RSDAFC!M21*$M$34</f>
+      <c r="I55" s="26">
+        <f>RSDAFC!M21*$M$35</f>
         <v>4.7397506033708351E-3</v>
       </c>
-      <c r="K54" t="str">
+      <c r="K55" t="str">
         <f>RSDAFC!C21</f>
         <v>R-SW_Apt_GAS_HPN2</v>
       </c>
     </row>
-    <row r="55" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C55" t="s">
-        <v>208</v>
-      </c>
-      <c r="D55" t="s">
-        <v>110</v>
-      </c>
-      <c r="H55" s="26">
-        <f>RSDAFC!L22*$M$34</f>
+    <row r="56" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>208</v>
+      </c>
+      <c r="D56" t="s">
+        <v>110</v>
+      </c>
+      <c r="H56" s="26">
+        <f>RSDAFC!L22*$M$35</f>
         <v>4.7397506033708351E-3</v>
       </c>
-      <c r="I55" s="26">
-        <f>RSDAFC!M22*$M$34</f>
+      <c r="I56" s="26">
+        <f>RSDAFC!M22*$M$35</f>
         <v>4.7397506033708351E-3</v>
       </c>
-      <c r="K55" t="str">
+      <c r="K56" t="str">
         <f>RSDAFC!C22</f>
         <v>R-SW_Apt_GAS_N1</v>
       </c>
     </row>
-    <row r="56" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C56" t="s">
-        <v>208</v>
-      </c>
-      <c r="D56" t="s">
-        <v>110</v>
-      </c>
-      <c r="H56" s="26">
-        <f>RSDAFC!L23*$M$34</f>
+    <row r="57" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
+        <v>208</v>
+      </c>
+      <c r="D57" t="s">
+        <v>110</v>
+      </c>
+      <c r="H57" s="26">
+        <f>RSDAFC!L23*$M$35</f>
         <v>4.7397506033708351E-3</v>
       </c>
-      <c r="I56" s="26">
-        <f>RSDAFC!M23*$M$34</f>
+      <c r="I57" s="26">
+        <f>RSDAFC!M23*$M$35</f>
         <v>4.7397506033708351E-3</v>
       </c>
-      <c r="K56" t="str">
+      <c r="K57" t="str">
         <f>RSDAFC!C23</f>
         <v>R-SW_Apt_GAS_N1</v>
       </c>
     </row>
-    <row r="57" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C57" t="s">
-        <v>208</v>
-      </c>
-      <c r="D57" t="s">
-        <v>110</v>
-      </c>
-      <c r="H57" s="26">
-        <f>RSDAFC!L24*$M$34</f>
+    <row r="58" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>208</v>
+      </c>
+      <c r="D58" t="s">
+        <v>110</v>
+      </c>
+      <c r="H58" s="26">
+        <f>RSDAFC!L24*$M$35</f>
         <v>3.5434891836400251E-4</v>
       </c>
-      <c r="I57" s="26">
-        <f>RSDAFC!M24*$M$34</f>
+      <c r="I58" s="26">
+        <f>RSDAFC!M24*$M$35</f>
         <v>3.5434891836400251E-4</v>
       </c>
-      <c r="K57" t="str">
+      <c r="K58" t="str">
         <f>RSDAFC!C24</f>
         <v>R-SW_Apt_HET_N1</v>
       </c>
     </row>
-    <row r="58" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C58" t="s">
-        <v>208</v>
-      </c>
-      <c r="D58" t="s">
-        <v>110</v>
-      </c>
-      <c r="H58" s="26">
-        <f>RSDAFC!L25*$M$34</f>
+    <row r="59" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
+        <v>208</v>
+      </c>
+      <c r="D59" t="s">
+        <v>110</v>
+      </c>
+      <c r="H59" s="26">
+        <f>RSDAFC!L25*$M$35</f>
         <v>3.5434891836400251E-4</v>
       </c>
-      <c r="I58" s="26">
-        <f>RSDAFC!M25*$M$34</f>
+      <c r="I59" s="26">
+        <f>RSDAFC!M25*$M$35</f>
         <v>3.5434891836400251E-4</v>
       </c>
-      <c r="K58" t="str">
+      <c r="K59" t="str">
         <f>RSDAFC!C25</f>
         <v>R-SW_Apt_HET_N1</v>
       </c>
     </row>
-    <row r="59" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C59" t="s">
-        <v>208</v>
-      </c>
-      <c r="D59" t="s">
-        <v>110</v>
-      </c>
-      <c r="H59" s="26">
-        <f>RSDAFC!L26*$M$34</f>
+    <row r="60" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>208</v>
+      </c>
+      <c r="D60" t="s">
+        <v>110</v>
+      </c>
+      <c r="H60" s="26">
+        <f>RSDAFC!L26*$M$35</f>
         <v>3.5434891836400251E-4</v>
       </c>
-      <c r="I59" s="26">
-        <f>RSDAFC!M26*$M$34</f>
+      <c r="I60" s="26">
+        <f>RSDAFC!M26*$M$35</f>
         <v>3.5434891836400251E-4</v>
       </c>
-      <c r="K59" t="str">
+      <c r="K60" t="str">
         <f>RSDAFC!C26</f>
         <v>R-SW_Apt_HET_N2</v>
       </c>
     </row>
-    <row r="60" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C60" t="s">
-        <v>208</v>
-      </c>
-      <c r="D60" t="s">
-        <v>110</v>
-      </c>
-      <c r="H60" s="26">
-        <f>RSDAFC!L27*$M$34</f>
+    <row r="61" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C61" t="s">
+        <v>208</v>
+      </c>
+      <c r="D61" t="s">
+        <v>110</v>
+      </c>
+      <c r="H61" s="26">
+        <f>RSDAFC!L27*$M$35</f>
         <v>3.5434891836400251E-4</v>
       </c>
-      <c r="I60" s="26">
-        <f>RSDAFC!M27*$M$34</f>
+      <c r="I61" s="26">
+        <f>RSDAFC!M27*$M$35</f>
         <v>3.5434891836400251E-4</v>
       </c>
-      <c r="K60" t="str">
+      <c r="K61" t="str">
         <f>RSDAFC!C27</f>
         <v>R-SW_Apt_HET_N2</v>
       </c>
     </row>
-    <row r="61" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C61" t="s">
-        <v>208</v>
-      </c>
-      <c r="D61" t="s">
-        <v>110</v>
-      </c>
-      <c r="H61" s="26">
-        <f>RSDAFC!L28*$M$34</f>
+    <row r="62" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
+        <v>208</v>
+      </c>
+      <c r="D62" t="s">
+        <v>110</v>
+      </c>
+      <c r="H62" s="26">
+        <f>RSDAFC!L28*$M$35</f>
         <v>1.199300219050925E-2</v>
       </c>
-      <c r="I61" s="26">
-        <f>RSDAFC!M28*$M$34</f>
+      <c r="I62" s="26">
+        <f>RSDAFC!M28*$M$35</f>
         <v>1.199300219050925E-2</v>
       </c>
-      <c r="K61" t="str">
+      <c r="K62" t="str">
         <f>RSDAFC!C28</f>
         <v>R-SW_Apt_KER_N1</v>
       </c>
     </row>
-    <row r="62" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C62" t="s">
-        <v>208</v>
-      </c>
-      <c r="D62" t="s">
-        <v>110</v>
-      </c>
-      <c r="H62" s="26">
-        <f>RSDAFC!L29*$M$34</f>
+    <row r="63" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C63" t="s">
+        <v>208</v>
+      </c>
+      <c r="D63" t="s">
+        <v>110</v>
+      </c>
+      <c r="H63" s="26">
+        <f>RSDAFC!L29*$M$35</f>
         <v>1.199300219050925E-2</v>
       </c>
-      <c r="I62" s="26">
-        <f>RSDAFC!M29*$M$34</f>
+      <c r="I63" s="26">
+        <f>RSDAFC!M29*$M$35</f>
         <v>1.199300219050925E-2</v>
       </c>
-      <c r="K62" t="str">
+      <c r="K63" t="str">
         <f>RSDAFC!C29</f>
         <v>R-SW_Apt_KER_N1</v>
       </c>
     </row>
-    <row r="63" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C63" t="s">
-        <v>208</v>
-      </c>
-      <c r="D63" t="s">
-        <v>110</v>
-      </c>
-      <c r="H63" s="26">
-        <f>RSDAFC!L30*$M$34</f>
+    <row r="64" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C64" t="s">
+        <v>208</v>
+      </c>
+      <c r="D64" t="s">
+        <v>110</v>
+      </c>
+      <c r="H64" s="26">
+        <f>RSDAFC!L30*$M$35</f>
         <v>8.90395563099655E-3</v>
       </c>
-      <c r="I63" s="26">
-        <f>RSDAFC!M30*$M$34</f>
+      <c r="I64" s="26">
+        <f>RSDAFC!M30*$M$35</f>
         <v>8.90395563099655E-3</v>
       </c>
-      <c r="K63" t="str">
+      <c r="K64" t="str">
         <f>RSDAFC!C30</f>
         <v>R-SW_Apt_LPG_N1</v>
       </c>
     </row>
-    <row r="64" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C64" t="s">
-        <v>208</v>
-      </c>
-      <c r="D64" t="s">
-        <v>110</v>
-      </c>
-      <c r="H64" s="26">
-        <f>RSDAFC!L31*$M$34</f>
+    <row r="65" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C65" t="s">
+        <v>208</v>
+      </c>
+      <c r="D65" t="s">
+        <v>110</v>
+      </c>
+      <c r="H65" s="26">
+        <f>RSDAFC!L31*$M$35</f>
         <v>8.90395563099655E-3</v>
       </c>
-      <c r="I64" s="26">
-        <f>RSDAFC!M31*$M$34</f>
+      <c r="I65" s="26">
+        <f>RSDAFC!M31*$M$35</f>
         <v>8.90395563099655E-3</v>
       </c>
-      <c r="K64" t="str">
+      <c r="K65" t="str">
         <f>RSDAFC!C31</f>
         <v>R-SW_Apt_LPG_N1</v>
       </c>
     </row>
-    <row r="65" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C65" t="s">
-        <v>208</v>
-      </c>
-      <c r="D65" t="s">
-        <v>110</v>
-      </c>
-      <c r="H65" s="26">
-        <f>RSDAFC!L32*$M$34</f>
+    <row r="66" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C66" t="s">
+        <v>208</v>
+      </c>
+      <c r="D66" t="s">
+        <v>110</v>
+      </c>
+      <c r="H66" s="26">
+        <f>RSDAFC!L32*$M$35</f>
         <v>6.8519450639461001E-3</v>
       </c>
-      <c r="I65" s="26">
-        <f>RSDAFC!M32*$M$34</f>
+      <c r="I66" s="26">
+        <f>RSDAFC!M32*$M$35</f>
         <v>6.8519450639461001E-3</v>
       </c>
-      <c r="K65" t="str">
+      <c r="K66" t="str">
         <f>RSDAFC!C32</f>
         <v>R-SW_Apt_WOO_N1</v>
       </c>
     </row>
-    <row r="66" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C66" t="s">
-        <v>208</v>
-      </c>
-      <c r="D66" t="s">
-        <v>110</v>
-      </c>
-      <c r="H66" s="26">
-        <f>RSDAFC!L33*$M$34</f>
+    <row r="67" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C67" t="s">
+        <v>208</v>
+      </c>
+      <c r="D67" t="s">
+        <v>110</v>
+      </c>
+      <c r="H67" s="26">
+        <f>RSDAFC!L33*$M$35</f>
         <v>6.8519450639461001E-3</v>
       </c>
-      <c r="I66" s="26">
-        <f>RSDAFC!M33*$M$34</f>
+      <c r="I67" s="26">
+        <f>RSDAFC!M33*$M$35</f>
         <v>6.8519450639461001E-3</v>
       </c>
-      <c r="K66" t="str">
+      <c r="K67" t="str">
         <f>RSDAFC!C33</f>
         <v>R-SW_Apt_WOO_N1</v>
       </c>
     </row>
-    <row r="67" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C67" t="s">
-        <v>208</v>
-      </c>
-      <c r="D67" t="s">
-        <v>110</v>
-      </c>
-      <c r="H67" s="26">
-        <f>RSDAFC!L34*$M$34</f>
+    <row r="68" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C68" t="s">
+        <v>208</v>
+      </c>
+      <c r="D68" t="s">
+        <v>110</v>
+      </c>
+      <c r="H68" s="26">
+        <f>RSDAFC!L34*$M$35</f>
         <v>9.3952077625382002E-3</v>
       </c>
-      <c r="I67" s="26">
-        <f>RSDAFC!M34*$M$34</f>
+      <c r="I68" s="26">
+        <f>RSDAFC!M34*$M$35</f>
         <v>9.3952077625382002E-3</v>
       </c>
-      <c r="K67" t="str">
+      <c r="K68" t="str">
         <f>RSDAFC!C34</f>
         <v>R-SW_Att_ELC_HPN1</v>
       </c>
     </row>
-    <row r="68" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C68" t="s">
-        <v>208</v>
-      </c>
-      <c r="D68" t="s">
-        <v>110</v>
-      </c>
-      <c r="H68" s="26">
-        <f>RSDAFC!L35*$M$34</f>
+    <row r="69" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C69" t="s">
+        <v>208</v>
+      </c>
+      <c r="D69" t="s">
+        <v>110</v>
+      </c>
+      <c r="H69" s="26">
+        <f>RSDAFC!L35*$M$35</f>
         <v>9.3952077625382002E-3</v>
       </c>
-      <c r="I68" s="26">
-        <f>RSDAFC!M35*$M$34</f>
+      <c r="I69" s="26">
+        <f>RSDAFC!M35*$M$35</f>
         <v>9.3952077625382002E-3</v>
       </c>
-      <c r="K68" t="str">
+      <c r="K69" t="str">
         <f>RSDAFC!C35</f>
         <v>R-SW_Att_ELC_HPN1</v>
       </c>
     </row>
-    <row r="69" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C69" t="s">
-        <v>208</v>
-      </c>
-      <c r="D69" t="s">
-        <v>110</v>
-      </c>
-      <c r="H69" s="26">
-        <f>RSDAFC!L36*$M$34</f>
+    <row r="70" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C70" t="s">
+        <v>208</v>
+      </c>
+      <c r="D70" t="s">
+        <v>110</v>
+      </c>
+      <c r="H70" s="26">
+        <f>RSDAFC!L36*$M$35</f>
         <v>9.3952077625382002E-3</v>
       </c>
-      <c r="I69" s="26">
-        <f>RSDAFC!M36*$M$34</f>
+      <c r="I70" s="26">
+        <f>RSDAFC!M36*$M$35</f>
         <v>9.3952077625382002E-3</v>
       </c>
-      <c r="K69" t="str">
+      <c r="K70" t="str">
         <f>RSDAFC!C36</f>
         <v>R-SW_Att_ELC_HPN2</v>
       </c>
     </row>
-    <row r="70" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C70" t="s">
-        <v>208</v>
-      </c>
-      <c r="D70" t="s">
-        <v>110</v>
-      </c>
-      <c r="H70" s="26">
-        <f>RSDAFC!L37*$M$34</f>
+    <row r="71" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C71" t="s">
+        <v>208</v>
+      </c>
+      <c r="D71" t="s">
+        <v>110</v>
+      </c>
+      <c r="H71" s="26">
+        <f>RSDAFC!L37*$M$35</f>
         <v>9.3952077625382002E-3</v>
       </c>
-      <c r="I70" s="26">
-        <f>RSDAFC!M37*$M$34</f>
+      <c r="I71" s="26">
+        <f>RSDAFC!M37*$M$35</f>
         <v>9.3952077625382002E-3</v>
       </c>
-      <c r="K70" t="str">
+      <c r="K71" t="str">
         <f>RSDAFC!C37</f>
         <v>R-SW_Att_ELC_HPN2</v>
       </c>
     </row>
-    <row r="71" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C71" t="s">
-        <v>208</v>
-      </c>
-      <c r="D71" t="s">
-        <v>110</v>
-      </c>
-      <c r="H71" s="26">
-        <f>RSDAFC!L38*$M$34</f>
+    <row r="72" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C72" t="s">
+        <v>208</v>
+      </c>
+      <c r="D72" t="s">
+        <v>110</v>
+      </c>
+      <c r="H72" s="26">
+        <f>RSDAFC!L38*$M$35</f>
         <v>7.8256501810713003E-3</v>
       </c>
-      <c r="I71" s="26">
-        <f>RSDAFC!M38*$M$34</f>
+      <c r="I72" s="26">
+        <f>RSDAFC!M38*$M$35</f>
         <v>7.8256501810713003E-3</v>
       </c>
-      <c r="K71" t="str">
+      <c r="K72" t="str">
         <f>RSDAFC!C38</f>
         <v>R-SW_Att_GAS_HHPN1</v>
       </c>
     </row>
-    <row r="72" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C72" t="s">
-        <v>208</v>
-      </c>
-      <c r="D72" t="s">
-        <v>110</v>
-      </c>
-      <c r="H72" s="26">
-        <f>RSDAFC!L39*$M$34</f>
+    <row r="73" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C73" t="s">
+        <v>208</v>
+      </c>
+      <c r="D73" t="s">
+        <v>110</v>
+      </c>
+      <c r="H73" s="26">
+        <f>RSDAFC!L39*$M$35</f>
         <v>7.8256501810713003E-3</v>
       </c>
-      <c r="I72" s="26">
-        <f>RSDAFC!M39*$M$34</f>
+      <c r="I73" s="26">
+        <f>RSDAFC!M39*$M$35</f>
         <v>7.8256501810713003E-3</v>
       </c>
-      <c r="K72" t="str">
+      <c r="K73" t="str">
         <f>RSDAFC!C39</f>
         <v>R-SW_Att_GAS_HHPN1</v>
       </c>
     </row>
-    <row r="73" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C73" t="s">
-        <v>208</v>
-      </c>
-      <c r="D73" t="s">
-        <v>110</v>
-      </c>
-      <c r="H73" s="26">
-        <f>RSDAFC!L40*$M$34</f>
+    <row r="74" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C74" t="s">
+        <v>208</v>
+      </c>
+      <c r="D74" t="s">
+        <v>110</v>
+      </c>
+      <c r="H74" s="26">
+        <f>RSDAFC!L40*$M$35</f>
         <v>7.8256501810713003E-3</v>
       </c>
-      <c r="I73" s="26">
-        <f>RSDAFC!M40*$M$34</f>
+      <c r="I74" s="26">
+        <f>RSDAFC!M40*$M$35</f>
         <v>7.8256501810713003E-3</v>
       </c>
-      <c r="K73" t="str">
+      <c r="K74" t="str">
         <f>RSDAFC!C40</f>
         <v>R-SW_Att_GAS_HPN1</v>
       </c>
     </row>
-    <row r="74" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C74" t="s">
-        <v>208</v>
-      </c>
-      <c r="D74" t="s">
-        <v>110</v>
-      </c>
-      <c r="H74" s="26">
-        <f>RSDAFC!L41*$M$34</f>
+    <row r="75" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C75" t="s">
+        <v>208</v>
+      </c>
+      <c r="D75" t="s">
+        <v>110</v>
+      </c>
+      <c r="H75" s="26">
+        <f>RSDAFC!L41*$M$35</f>
         <v>7.8256501810713003E-3</v>
       </c>
-      <c r="I74" s="26">
-        <f>RSDAFC!M41*$M$34</f>
+      <c r="I75" s="26">
+        <f>RSDAFC!M41*$M$35</f>
         <v>7.8256501810713003E-3</v>
       </c>
-      <c r="K74" t="str">
+      <c r="K75" t="str">
         <f>RSDAFC!C41</f>
         <v>R-SW_Att_GAS_HPN1</v>
       </c>
     </row>
-    <row r="75" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C75" t="s">
-        <v>208</v>
-      </c>
-      <c r="D75" t="s">
-        <v>110</v>
-      </c>
-      <c r="H75" s="26">
-        <f>RSDAFC!L42*$M$34</f>
+    <row r="76" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C76" t="s">
+        <v>208</v>
+      </c>
+      <c r="D76" t="s">
+        <v>110</v>
+      </c>
+      <c r="H76" s="26">
+        <f>RSDAFC!L42*$M$35</f>
         <v>7.8256501810713003E-3</v>
       </c>
-      <c r="I75" s="26">
-        <f>RSDAFC!M42*$M$34</f>
+      <c r="I76" s="26">
+        <f>RSDAFC!M42*$M$35</f>
         <v>7.8256501810713003E-3</v>
       </c>
-      <c r="K75" t="str">
+      <c r="K76" t="str">
         <f>RSDAFC!C42</f>
         <v>R-SW_Att_GAS_HPN2</v>
       </c>
     </row>
-    <row r="76" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C76" t="s">
-        <v>208</v>
-      </c>
-      <c r="D76" t="s">
-        <v>110</v>
-      </c>
-      <c r="H76" s="26">
-        <f>RSDAFC!L43*$M$34</f>
+    <row r="77" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C77" t="s">
+        <v>208</v>
+      </c>
+      <c r="D77" t="s">
+        <v>110</v>
+      </c>
+      <c r="H77" s="26">
+        <f>RSDAFC!L43*$M$35</f>
         <v>7.8256501810713003E-3</v>
       </c>
-      <c r="I76" s="26">
-        <f>RSDAFC!M43*$M$34</f>
+      <c r="I77" s="26">
+        <f>RSDAFC!M43*$M$35</f>
         <v>7.8256501810713003E-3</v>
       </c>
-      <c r="K76" t="str">
+      <c r="K77" t="str">
         <f>RSDAFC!C43</f>
         <v>R-SW_Att_GAS_HPN2</v>
       </c>
     </row>
-    <row r="77" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C77" t="s">
-        <v>208</v>
-      </c>
-      <c r="D77" t="s">
-        <v>110</v>
-      </c>
-      <c r="H77" s="26">
-        <f>RSDAFC!L44*$M$34</f>
+    <row r="78" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C78" t="s">
+        <v>208</v>
+      </c>
+      <c r="D78" t="s">
+        <v>110</v>
+      </c>
+      <c r="H78" s="26">
+        <f>RSDAFC!L44*$M$35</f>
         <v>7.8256501810713003E-3</v>
       </c>
-      <c r="I77" s="26">
-        <f>RSDAFC!M44*$M$34</f>
+      <c r="I78" s="26">
+        <f>RSDAFC!M44*$M$35</f>
         <v>7.8256501810713003E-3</v>
       </c>
-      <c r="K77" t="str">
+      <c r="K78" t="str">
         <f>RSDAFC!C44</f>
         <v>R-SW_Att_GAS_N1</v>
       </c>
     </row>
-    <row r="78" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C78" t="s">
-        <v>208</v>
-      </c>
-      <c r="D78" t="s">
-        <v>110</v>
-      </c>
-      <c r="H78" s="26">
-        <f>RSDAFC!L45*$M$34</f>
+    <row r="79" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C79" t="s">
+        <v>208</v>
+      </c>
+      <c r="D79" t="s">
+        <v>110</v>
+      </c>
+      <c r="H79" s="26">
+        <f>RSDAFC!L45*$M$35</f>
         <v>7.8256501810713003E-3</v>
       </c>
-      <c r="I78" s="26">
-        <f>RSDAFC!M45*$M$34</f>
+      <c r="I79" s="26">
+        <f>RSDAFC!M45*$M$35</f>
         <v>7.8256501810713003E-3</v>
       </c>
-      <c r="K78" t="str">
+      <c r="K79" t="str">
         <f>RSDAFC!C45</f>
         <v>R-SW_Att_GAS_N1</v>
       </c>
     </row>
-    <row r="79" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C79" t="s">
-        <v>208</v>
-      </c>
-      <c r="D79" t="s">
-        <v>110</v>
-      </c>
-      <c r="H79" s="26">
-        <f>RSDAFC!L46*$M$34</f>
+    <row r="80" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C80" t="s">
+        <v>208</v>
+      </c>
+      <c r="D80" t="s">
+        <v>110</v>
+      </c>
+      <c r="H80" s="26">
+        <f>RSDAFC!L46*$M$35</f>
         <v>7.8256501810713003E-3</v>
       </c>
-      <c r="I79" s="26">
-        <f>RSDAFC!M46*$M$34</f>
+      <c r="I80" s="26">
+        <f>RSDAFC!M46*$M$35</f>
         <v>7.8256501810713003E-3</v>
       </c>
-      <c r="K79" t="str">
+      <c r="K80" t="str">
         <f>RSDAFC!C46</f>
         <v>R-SW_Att_GAS_N2</v>
       </c>
     </row>
-    <row r="80" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C80" t="s">
-        <v>208</v>
-      </c>
-      <c r="D80" t="s">
-        <v>110</v>
-      </c>
-      <c r="H80" s="26">
-        <f>RSDAFC!L47*$M$34</f>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C81" t="s">
+        <v>208</v>
+      </c>
+      <c r="D81" t="s">
+        <v>110</v>
+      </c>
+      <c r="H81" s="26">
+        <f>RSDAFC!L47*$M$35</f>
         <v>7.8256501810713003E-3</v>
       </c>
-      <c r="I80" s="26">
-        <f>RSDAFC!M47*$M$34</f>
+      <c r="I81" s="26">
+        <f>RSDAFC!M47*$M$35</f>
         <v>7.8256501810713003E-3</v>
       </c>
-      <c r="K80" t="str">
+      <c r="K81" t="str">
         <f>RSDAFC!C47</f>
         <v>R-SW_Att_GAS_N2</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C81" t="s">
-        <v>208</v>
-      </c>
-      <c r="D81" t="s">
-        <v>110</v>
-      </c>
-      <c r="H81" s="26">
-        <f>RSDAFC!L48*$M$34</f>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C82" t="s">
+        <v>208</v>
+      </c>
+      <c r="D82" t="s">
+        <v>110</v>
+      </c>
+      <c r="H82" s="26">
+        <f>RSDAFC!L48*$M$35</f>
         <v>7.8256501810713003E-3</v>
       </c>
-      <c r="I81" s="26">
-        <f>RSDAFC!M48*$M$34</f>
+      <c r="I82" s="26">
+        <f>RSDAFC!M48*$M$35</f>
         <v>7.8256501810713003E-3</v>
       </c>
-      <c r="K81" t="str">
+      <c r="K82" t="str">
         <f>RSDAFC!C48</f>
         <v>R-SW_Att_GAS_N3</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C82" t="s">
-        <v>208</v>
-      </c>
-      <c r="D82" t="s">
-        <v>110</v>
-      </c>
-      <c r="H82" s="26">
-        <f>RSDAFC!L49*$M$34</f>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C83" t="s">
+        <v>208</v>
+      </c>
+      <c r="D83" t="s">
+        <v>110</v>
+      </c>
+      <c r="H83" s="26">
+        <f>RSDAFC!L49*$M$35</f>
         <v>7.8256501810713003E-3</v>
       </c>
-      <c r="I82" s="26">
-        <f>RSDAFC!M49*$M$34</f>
+      <c r="I83" s="26">
+        <f>RSDAFC!M49*$M$35</f>
         <v>7.8256501810713003E-3</v>
       </c>
-      <c r="K82" t="str">
+      <c r="K83" t="str">
         <f>RSDAFC!C49</f>
         <v>R-SW_Att_GAS_N3</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C83" t="s">
-        <v>208</v>
-      </c>
-      <c r="D83" t="s">
-        <v>110</v>
-      </c>
-      <c r="H83" s="26">
-        <f>RSDAFC!L50*$M$34</f>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C84" t="s">
+        <v>208</v>
+      </c>
+      <c r="D84" t="s">
+        <v>110</v>
+      </c>
+      <c r="H84" s="26">
+        <f>RSDAFC!L50*$M$35</f>
         <v>3.7989460522007048E-3</v>
       </c>
-      <c r="I83" s="26">
-        <f>RSDAFC!M50*$M$34</f>
+      <c r="I84" s="26">
+        <f>RSDAFC!M50*$M$35</f>
         <v>3.7989460522007048E-3</v>
       </c>
-      <c r="K83" t="str">
+      <c r="K84" t="str">
         <f>RSDAFC!C50</f>
         <v>R-SW_Att_HET_N1</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C84" t="s">
-        <v>208</v>
-      </c>
-      <c r="D84" t="s">
-        <v>110</v>
-      </c>
-      <c r="H84" s="26">
-        <f>RSDAFC!L51*$M$34</f>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C85" t="s">
+        <v>208</v>
+      </c>
+      <c r="D85" t="s">
+        <v>110</v>
+      </c>
+      <c r="H85" s="26">
+        <f>RSDAFC!L51*$M$35</f>
         <v>3.7989460522007048E-3</v>
       </c>
-      <c r="I84" s="26">
-        <f>RSDAFC!M51*$M$34</f>
+      <c r="I85" s="26">
+        <f>RSDAFC!M51*$M$35</f>
         <v>3.7989460522007048E-3</v>
       </c>
-      <c r="K84" t="str">
+      <c r="K85" t="str">
         <f>RSDAFC!C51</f>
         <v>R-SW_Att_HET_N1</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C85" t="s">
-        <v>208</v>
-      </c>
-      <c r="D85" t="s">
-        <v>110</v>
-      </c>
-      <c r="H85" s="26">
-        <f>RSDAFC!L52*$M$34</f>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C86" t="s">
+        <v>208</v>
+      </c>
+      <c r="D86" t="s">
+        <v>110</v>
+      </c>
+      <c r="H86" s="26">
+        <f>RSDAFC!L52*$M$35</f>
         <v>3.7989460522007048E-3</v>
       </c>
-      <c r="I85" s="26">
-        <f>RSDAFC!M52*$M$34</f>
+      <c r="I86" s="26">
+        <f>RSDAFC!M52*$M$35</f>
         <v>3.7989460522007048E-3</v>
       </c>
-      <c r="K85" t="str">
+      <c r="K86" t="str">
         <f>RSDAFC!C52</f>
         <v>R-SW_Att_HET_N2</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C86" t="s">
-        <v>208</v>
-      </c>
-      <c r="D86" t="s">
-        <v>110</v>
-      </c>
-      <c r="H86" s="26">
-        <f>RSDAFC!L53*$M$34</f>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C87" t="s">
+        <v>208</v>
+      </c>
+      <c r="D87" t="s">
+        <v>110</v>
+      </c>
+      <c r="H87" s="26">
+        <f>RSDAFC!L53*$M$35</f>
         <v>3.7989460522007048E-3</v>
       </c>
-      <c r="I86" s="26">
-        <f>RSDAFC!M53*$M$34</f>
+      <c r="I87" s="26">
+        <f>RSDAFC!M53*$M$35</f>
         <v>3.7989460522007048E-3</v>
       </c>
-      <c r="K86" t="str">
+      <c r="K87" t="str">
         <f>RSDAFC!C53</f>
         <v>R-SW_Att_HET_N2</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C87" t="s">
-        <v>208</v>
-      </c>
-      <c r="D87" t="s">
-        <v>110</v>
-      </c>
-      <c r="H87" s="26">
-        <f>RSDAFC!L54*$M$34</f>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C88" t="s">
+        <v>208</v>
+      </c>
+      <c r="D88" t="s">
+        <v>110</v>
+      </c>
+      <c r="H88" s="26">
+        <f>RSDAFC!L54*$M$35</f>
         <v>9.8399724094370006E-3</v>
       </c>
-      <c r="I87" s="26">
-        <f>RSDAFC!M54*$M$34</f>
+      <c r="I88" s="26">
+        <f>RSDAFC!M54*$M$35</f>
         <v>9.8399724094370006E-3</v>
       </c>
-      <c r="K87" t="str">
+      <c r="K88" t="str">
         <f>RSDAFC!C54</f>
         <v>R-SW_Att_KER_N1</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C88" t="s">
-        <v>208</v>
-      </c>
-      <c r="D88" t="s">
-        <v>110</v>
-      </c>
-      <c r="H88" s="26">
-        <f>RSDAFC!L55*$M$34</f>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C89" t="s">
+        <v>208</v>
+      </c>
+      <c r="D89" t="s">
+        <v>110</v>
+      </c>
+      <c r="H89" s="26">
+        <f>RSDAFC!L55*$M$35</f>
         <v>9.8399724094370006E-3</v>
       </c>
-      <c r="I88" s="26">
-        <f>RSDAFC!M55*$M$34</f>
+      <c r="I89" s="26">
+        <f>RSDAFC!M55*$M$35</f>
         <v>9.8399724094370006E-3</v>
       </c>
-      <c r="K88" t="str">
+      <c r="K89" t="str">
         <f>RSDAFC!C55</f>
         <v>R-SW_Att_KER_N1</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C89" t="s">
-        <v>208</v>
-      </c>
-      <c r="D89" t="s">
-        <v>110</v>
-      </c>
-      <c r="H89" s="26">
-        <f>RSDAFC!L56*$M$34</f>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C90" t="s">
+        <v>208</v>
+      </c>
+      <c r="D90" t="s">
+        <v>110</v>
+      </c>
+      <c r="H90" s="26">
+        <f>RSDAFC!L56*$M$35</f>
         <v>9.8399724094370006E-3</v>
       </c>
-      <c r="I89" s="26">
-        <f>RSDAFC!M56*$M$34</f>
+      <c r="I90" s="26">
+        <f>RSDAFC!M56*$M$35</f>
         <v>9.8399724094370006E-3</v>
       </c>
-      <c r="K89" t="str">
+      <c r="K90" t="str">
         <f>RSDAFC!C56</f>
         <v>R-SW_Att_KER_N2</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C90" t="s">
-        <v>208</v>
-      </c>
-      <c r="D90" t="s">
-        <v>110</v>
-      </c>
-      <c r="H90" s="26">
-        <f>RSDAFC!L57*$M$34</f>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C91" t="s">
+        <v>208</v>
+      </c>
+      <c r="D91" t="s">
+        <v>110</v>
+      </c>
+      <c r="H91" s="26">
+        <f>RSDAFC!L57*$M$35</f>
         <v>9.8399724094370006E-3</v>
       </c>
-      <c r="I90" s="26">
-        <f>RSDAFC!M57*$M$34</f>
+      <c r="I91" s="26">
+        <f>RSDAFC!M57*$M$35</f>
         <v>9.8399724094370006E-3</v>
       </c>
-      <c r="K90" t="str">
+      <c r="K91" t="str">
         <f>RSDAFC!C57</f>
         <v>R-SW_Att_KER_N2</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C91" t="s">
-        <v>208</v>
-      </c>
-      <c r="D91" t="s">
-        <v>110</v>
-      </c>
-      <c r="H91" s="26">
-        <f>RSDAFC!L58*$M$34</f>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C92" t="s">
+        <v>208</v>
+      </c>
+      <c r="D92" t="s">
+        <v>110</v>
+      </c>
+      <c r="H92" s="26">
+        <f>RSDAFC!L58*$M$35</f>
         <v>9.8399724094370006E-3</v>
       </c>
-      <c r="I91" s="26">
-        <f>RSDAFC!M58*$M$34</f>
+      <c r="I92" s="26">
+        <f>RSDAFC!M58*$M$35</f>
         <v>9.8399724094370006E-3</v>
       </c>
-      <c r="K91" t="str">
+      <c r="K92" t="str">
         <f>RSDAFC!C58</f>
         <v>R-SW_Att_KER_N3</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C92" t="s">
-        <v>208</v>
-      </c>
-      <c r="D92" t="s">
-        <v>110</v>
-      </c>
-      <c r="H92" s="26">
-        <f>RSDAFC!L59*$M$34</f>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C93" t="s">
+        <v>208</v>
+      </c>
+      <c r="D93" t="s">
+        <v>110</v>
+      </c>
+      <c r="H93" s="26">
+        <f>RSDAFC!L59*$M$35</f>
         <v>9.8399724094370006E-3</v>
       </c>
-      <c r="I92" s="26">
-        <f>RSDAFC!M59*$M$34</f>
+      <c r="I93" s="26">
+        <f>RSDAFC!M59*$M$35</f>
         <v>9.8399724094370006E-3</v>
       </c>
-      <c r="K92" t="str">
+      <c r="K93" t="str">
         <f>RSDAFC!C59</f>
         <v>R-SW_Att_KER_N3</v>
-      </c>
-    </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A93" s="39"/>
-      <c r="B93" s="39"/>
-      <c r="C93" s="39" t="s">
-        <v>208</v>
-      </c>
-      <c r="D93" s="39" t="s">
-        <v>110</v>
-      </c>
-      <c r="E93" s="39"/>
-      <c r="F93" s="39"/>
-      <c r="G93" s="39"/>
-      <c r="H93" s="40">
-        <f>H99</f>
-        <v>2.14779508723714E-2</v>
-      </c>
-      <c r="I93" s="40">
-        <f>I99</f>
-        <v>2.14779508723714E-2</v>
-      </c>
-      <c r="J93" s="39"/>
-      <c r="K93" s="39" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
@@ -4936,7 +5213,7 @@
       </c>
       <c r="J94" s="39"/>
       <c r="K94" s="39" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
@@ -4952,16 +5229,16 @@
       <c r="F95" s="39"/>
       <c r="G95" s="39"/>
       <c r="H95" s="40">
-        <f>H92</f>
-        <v>9.8399724094370006E-3</v>
+        <f>H101</f>
+        <v>2.14779508723714E-2</v>
       </c>
       <c r="I95" s="40">
-        <f>I92</f>
-        <v>9.8399724094370006E-3</v>
+        <f>I101</f>
+        <v>2.14779508723714E-2</v>
       </c>
       <c r="J95" s="39"/>
       <c r="K95" s="39" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
@@ -4977,641 +5254,641 @@
       <c r="F96" s="39"/>
       <c r="G96" s="39"/>
       <c r="H96" s="40">
-        <f>H95</f>
+        <f>H93</f>
         <v>9.8399724094370006E-3</v>
       </c>
       <c r="I96" s="40">
-        <f>I95</f>
+        <f>I93</f>
         <v>9.8399724094370006E-3</v>
       </c>
       <c r="J96" s="39"/>
       <c r="K96" s="39" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A97" s="39"/>
+      <c r="B97" s="39"/>
+      <c r="C97" s="39" t="s">
+        <v>208</v>
+      </c>
+      <c r="D97" s="39" t="s">
+        <v>110</v>
+      </c>
+      <c r="E97" s="39"/>
+      <c r="F97" s="39"/>
+      <c r="G97" s="39"/>
+      <c r="H97" s="40">
+        <f>H96</f>
+        <v>9.8399724094370006E-3</v>
+      </c>
+      <c r="I97" s="40">
+        <f>I96</f>
+        <v>9.8399724094370006E-3</v>
+      </c>
+      <c r="J97" s="39"/>
+      <c r="K97" s="39" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="97" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C97" t="s">
-        <v>208</v>
-      </c>
-      <c r="D97" t="s">
-        <v>110</v>
-      </c>
-      <c r="H97" s="26">
-        <f>RSDAFC!L60*$M$34</f>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C98" t="s">
+        <v>208</v>
+      </c>
+      <c r="D98" t="s">
+        <v>110</v>
+      </c>
+      <c r="H98" s="26">
+        <f>RSDAFC!L60*$M$35</f>
         <v>1.1698585866472801E-2</v>
       </c>
-      <c r="I97" s="26">
-        <f>RSDAFC!M60*$M$34</f>
+      <c r="I98" s="26">
+        <f>RSDAFC!M60*$M$35</f>
         <v>1.1698585866472801E-2</v>
       </c>
-      <c r="K97" t="str">
+      <c r="K98" t="str">
         <f>RSDAFC!C60</f>
         <v>R-SW_Att_LPG_N1</v>
       </c>
     </row>
-    <row r="98" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C98" t="s">
-        <v>208</v>
-      </c>
-      <c r="D98" t="s">
-        <v>110</v>
-      </c>
-      <c r="H98" s="26">
-        <f>RSDAFC!L61*$M$34</f>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C99" t="s">
+        <v>208</v>
+      </c>
+      <c r="D99" t="s">
+        <v>110</v>
+      </c>
+      <c r="H99" s="26">
+        <f>RSDAFC!L61*$M$35</f>
         <v>1.1698585866472801E-2</v>
       </c>
-      <c r="I98" s="26">
-        <f>RSDAFC!M61*$M$34</f>
+      <c r="I99" s="26">
+        <f>RSDAFC!M61*$M$35</f>
         <v>1.1698585866472801E-2</v>
       </c>
-      <c r="K98" t="str">
+      <c r="K99" t="str">
         <f>RSDAFC!C61</f>
         <v>R-SW_Att_LPG_N1</v>
       </c>
     </row>
-    <row r="99" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C99" t="s">
-        <v>208</v>
-      </c>
-      <c r="D99" t="s">
-        <v>110</v>
-      </c>
-      <c r="H99" s="26">
-        <f>RSDAFC!L62*$M$34</f>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C100" t="s">
+        <v>208</v>
+      </c>
+      <c r="D100" t="s">
+        <v>110</v>
+      </c>
+      <c r="H100" s="26">
+        <f>RSDAFC!L62*$M$35</f>
         <v>2.14779508723714E-2</v>
       </c>
-      <c r="I99" s="26">
-        <f>RSDAFC!M62*$M$34</f>
+      <c r="I100" s="26">
+        <f>RSDAFC!M62*$M$35</f>
         <v>2.14779508723714E-2</v>
       </c>
-      <c r="K99" t="str">
+      <c r="K100" t="str">
         <f>RSDAFC!C62</f>
         <v>R-SW_Att_WOO_N1</v>
       </c>
     </row>
-    <row r="100" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C100" t="s">
-        <v>208</v>
-      </c>
-      <c r="D100" t="s">
-        <v>110</v>
-      </c>
-      <c r="H100" s="26">
-        <f>RSDAFC!L63*$M$34</f>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C101" t="s">
+        <v>208</v>
+      </c>
+      <c r="D101" t="s">
+        <v>110</v>
+      </c>
+      <c r="H101" s="26">
+        <f>RSDAFC!L63*$M$35</f>
         <v>2.14779508723714E-2</v>
       </c>
-      <c r="I100" s="26">
-        <f>RSDAFC!M63*$M$34</f>
+      <c r="I101" s="26">
+        <f>RSDAFC!M63*$M$35</f>
         <v>2.14779508723714E-2</v>
       </c>
-      <c r="K100" t="str">
+      <c r="K101" t="str">
         <f>RSDAFC!C63</f>
         <v>R-SW_Att_WOO_N1</v>
       </c>
     </row>
-    <row r="101" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C101" t="s">
-        <v>208</v>
-      </c>
-      <c r="D101" t="s">
-        <v>110</v>
-      </c>
-      <c r="H101" s="26">
-        <f>RSDAFC!L64*$M$34</f>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C102" t="s">
+        <v>208</v>
+      </c>
+      <c r="D102" t="s">
+        <v>110</v>
+      </c>
+      <c r="H102" s="26">
+        <f>RSDAFC!L64*$M$35</f>
         <v>1.3735723758749249E-2</v>
       </c>
-      <c r="I101" s="26">
-        <f>RSDAFC!M64*$M$34</f>
+      <c r="I102" s="26">
+        <f>RSDAFC!M64*$M$35</f>
         <v>1.3735723758749249E-2</v>
       </c>
-      <c r="K101" t="str">
+      <c r="K102" t="str">
         <f>RSDAFC!C64</f>
         <v>R-SW_Det_ELC_HPN1</v>
       </c>
     </row>
-    <row r="102" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C102" t="s">
-        <v>208</v>
-      </c>
-      <c r="D102" t="s">
-        <v>110</v>
-      </c>
-      <c r="H102" s="26">
-        <f>RSDAFC!L65*$M$34</f>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C103" t="s">
+        <v>208</v>
+      </c>
+      <c r="D103" t="s">
+        <v>110</v>
+      </c>
+      <c r="H103" s="26">
+        <f>RSDAFC!L65*$M$35</f>
         <v>1.3735723758749249E-2</v>
       </c>
-      <c r="I102" s="26">
-        <f>RSDAFC!M65*$M$34</f>
+      <c r="I103" s="26">
+        <f>RSDAFC!M65*$M$35</f>
         <v>1.3735723758749249E-2</v>
       </c>
-      <c r="K102" t="str">
+      <c r="K103" t="str">
         <f>RSDAFC!C65</f>
         <v>R-SW_Det_ELC_HPN1</v>
       </c>
     </row>
-    <row r="103" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C103" t="s">
-        <v>208</v>
-      </c>
-      <c r="D103" t="s">
-        <v>110</v>
-      </c>
-      <c r="H103" s="26">
-        <f>RSDAFC!L66*$M$34</f>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C104" t="s">
+        <v>208</v>
+      </c>
+      <c r="D104" t="s">
+        <v>110</v>
+      </c>
+      <c r="H104" s="26">
+        <f>RSDAFC!L66*$M$35</f>
         <v>1.3735723758749249E-2</v>
       </c>
-      <c r="I103" s="26">
-        <f>RSDAFC!M66*$M$34</f>
+      <c r="I104" s="26">
+        <f>RSDAFC!M66*$M$35</f>
         <v>1.3735723758749249E-2</v>
       </c>
-      <c r="K103" t="str">
+      <c r="K104" t="str">
         <f>RSDAFC!C66</f>
         <v>R-SW_Det_ELC_HPN2</v>
       </c>
     </row>
-    <row r="104" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C104" t="s">
-        <v>208</v>
-      </c>
-      <c r="D104" t="s">
-        <v>110</v>
-      </c>
-      <c r="H104" s="26">
-        <f>RSDAFC!L67*$M$34</f>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C105" t="s">
+        <v>208</v>
+      </c>
+      <c r="D105" t="s">
+        <v>110</v>
+      </c>
+      <c r="H105" s="26">
+        <f>RSDAFC!L67*$M$35</f>
         <v>1.3735723758749249E-2</v>
       </c>
-      <c r="I104" s="26">
-        <f>RSDAFC!M67*$M$34</f>
+      <c r="I105" s="26">
+        <f>RSDAFC!M67*$M$35</f>
         <v>1.3735723758749249E-2</v>
       </c>
-      <c r="K104" t="str">
+      <c r="K105" t="str">
         <f>RSDAFC!C67</f>
         <v>R-SW_Det_ELC_HPN2</v>
       </c>
     </row>
-    <row r="105" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C105" t="s">
-        <v>208</v>
-      </c>
-      <c r="D105" t="s">
-        <v>110</v>
-      </c>
-      <c r="H105" s="26">
-        <f>RSDAFC!L68*$M$34</f>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C106" t="s">
+        <v>208</v>
+      </c>
+      <c r="D106" t="s">
+        <v>110</v>
+      </c>
+      <c r="H106" s="26">
+        <f>RSDAFC!L68*$M$35</f>
         <v>1.222361012943445E-2</v>
       </c>
-      <c r="I105" s="26">
-        <f>RSDAFC!M68*$M$34</f>
+      <c r="I106" s="26">
+        <f>RSDAFC!M68*$M$35</f>
         <v>1.222361012943445E-2</v>
       </c>
-      <c r="K105" t="str">
+      <c r="K106" t="str">
         <f>RSDAFC!C68</f>
         <v>R-SW_Det_GAS_HHPN1</v>
       </c>
     </row>
-    <row r="106" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C106" t="s">
-        <v>208</v>
-      </c>
-      <c r="D106" t="s">
-        <v>110</v>
-      </c>
-      <c r="H106" s="26">
-        <f>RSDAFC!L69*$M$34</f>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C107" t="s">
+        <v>208</v>
+      </c>
+      <c r="D107" t="s">
+        <v>110</v>
+      </c>
+      <c r="H107" s="26">
+        <f>RSDAFC!L69*$M$35</f>
         <v>1.222361012943445E-2</v>
       </c>
-      <c r="I106" s="26">
-        <f>RSDAFC!M69*$M$34</f>
+      <c r="I107" s="26">
+        <f>RSDAFC!M69*$M$35</f>
         <v>1.222361012943445E-2</v>
       </c>
-      <c r="K106" t="str">
+      <c r="K107" t="str">
         <f>RSDAFC!C69</f>
         <v>R-SW_Det_GAS_HHPN1</v>
       </c>
     </row>
-    <row r="107" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C107" t="s">
-        <v>208</v>
-      </c>
-      <c r="D107" t="s">
-        <v>110</v>
-      </c>
-      <c r="H107" s="26">
-        <f>RSDAFC!L70*$M$34</f>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C108" t="s">
+        <v>208</v>
+      </c>
+      <c r="D108" t="s">
+        <v>110</v>
+      </c>
+      <c r="H108" s="26">
+        <f>RSDAFC!L70*$M$35</f>
         <v>1.222361012943445E-2</v>
       </c>
-      <c r="I107" s="26">
-        <f>RSDAFC!M70*$M$34</f>
+      <c r="I108" s="26">
+        <f>RSDAFC!M70*$M$35</f>
         <v>1.222361012943445E-2</v>
       </c>
-      <c r="K107" t="str">
+      <c r="K108" t="str">
         <f>RSDAFC!C70</f>
         <v>R-SW_Det_GAS_HPN1</v>
       </c>
     </row>
-    <row r="108" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C108" t="s">
-        <v>208</v>
-      </c>
-      <c r="D108" t="s">
-        <v>110</v>
-      </c>
-      <c r="H108" s="26">
-        <f>RSDAFC!L71*$M$34</f>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C109" t="s">
+        <v>208</v>
+      </c>
+      <c r="D109" t="s">
+        <v>110</v>
+      </c>
+      <c r="H109" s="26">
+        <f>RSDAFC!L71*$M$35</f>
         <v>1.222361012943445E-2</v>
       </c>
-      <c r="I108" s="26">
-        <f>RSDAFC!M71*$M$34</f>
+      <c r="I109" s="26">
+        <f>RSDAFC!M71*$M$35</f>
         <v>1.222361012943445E-2</v>
       </c>
-      <c r="K108" t="str">
+      <c r="K109" t="str">
         <f>RSDAFC!C71</f>
         <v>R-SW_Det_GAS_HPN1</v>
       </c>
     </row>
-    <row r="109" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C109" t="s">
-        <v>208</v>
-      </c>
-      <c r="D109" t="s">
-        <v>110</v>
-      </c>
-      <c r="H109" s="26">
-        <f>RSDAFC!L72*$M$34</f>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C110" t="s">
+        <v>208</v>
+      </c>
+      <c r="D110" t="s">
+        <v>110</v>
+      </c>
+      <c r="H110" s="26">
+        <f>RSDAFC!L72*$M$35</f>
         <v>1.222361012943445E-2</v>
       </c>
-      <c r="I109" s="26">
-        <f>RSDAFC!M72*$M$34</f>
+      <c r="I110" s="26">
+        <f>RSDAFC!M72*$M$35</f>
         <v>1.222361012943445E-2</v>
       </c>
-      <c r="K109" t="str">
+      <c r="K110" t="str">
         <f>RSDAFC!C72</f>
         <v>R-SW_Det_GAS_HPN2</v>
       </c>
     </row>
-    <row r="110" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C110" t="s">
-        <v>208</v>
-      </c>
-      <c r="D110" t="s">
-        <v>110</v>
-      </c>
-      <c r="H110" s="26">
-        <f>RSDAFC!L73*$M$34</f>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C111" t="s">
+        <v>208</v>
+      </c>
+      <c r="D111" t="s">
+        <v>110</v>
+      </c>
+      <c r="H111" s="26">
+        <f>RSDAFC!L73*$M$35</f>
         <v>1.222361012943445E-2</v>
       </c>
-      <c r="I110" s="26">
-        <f>RSDAFC!M73*$M$34</f>
+      <c r="I111" s="26">
+        <f>RSDAFC!M73*$M$35</f>
         <v>1.222361012943445E-2</v>
       </c>
-      <c r="K110" t="str">
+      <c r="K111" t="str">
         <f>RSDAFC!C73</f>
         <v>R-SW_Det_GAS_HPN2</v>
       </c>
     </row>
-    <row r="111" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C111" t="s">
-        <v>208</v>
-      </c>
-      <c r="D111" t="s">
-        <v>110</v>
-      </c>
-      <c r="H111" s="26">
-        <f>RSDAFC!L74*$M$34</f>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C112" t="s">
+        <v>208</v>
+      </c>
+      <c r="D112" t="s">
+        <v>110</v>
+      </c>
+      <c r="H112" s="26">
+        <f>RSDAFC!L74*$M$35</f>
         <v>1.222361012943445E-2</v>
       </c>
-      <c r="I111" s="26">
-        <f>RSDAFC!M74*$M$34</f>
+      <c r="I112" s="26">
+        <f>RSDAFC!M74*$M$35</f>
         <v>1.222361012943445E-2</v>
       </c>
-      <c r="K111" t="str">
+      <c r="K112" t="str">
         <f>RSDAFC!C74</f>
         <v>R-SW_Det_GAS_N1</v>
       </c>
     </row>
-    <row r="112" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C112" t="s">
-        <v>208</v>
-      </c>
-      <c r="D112" t="s">
-        <v>110</v>
-      </c>
-      <c r="H112" s="26">
-        <f>RSDAFC!L75*$M$34</f>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C113" t="s">
+        <v>208</v>
+      </c>
+      <c r="D113" t="s">
+        <v>110</v>
+      </c>
+      <c r="H113" s="26">
+        <f>RSDAFC!L75*$M$35</f>
         <v>1.222361012943445E-2</v>
       </c>
-      <c r="I112" s="26">
-        <f>RSDAFC!M75*$M$34</f>
+      <c r="I113" s="26">
+        <f>RSDAFC!M75*$M$35</f>
         <v>1.222361012943445E-2</v>
       </c>
-      <c r="K112" t="str">
+      <c r="K113" t="str">
         <f>RSDAFC!C75</f>
         <v>R-SW_Det_GAS_N1</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C113" t="s">
-        <v>208</v>
-      </c>
-      <c r="D113" t="s">
-        <v>110</v>
-      </c>
-      <c r="H113" s="26">
-        <f>RSDAFC!L76*$M$34</f>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C114" t="s">
+        <v>208</v>
+      </c>
+      <c r="D114" t="s">
+        <v>110</v>
+      </c>
+      <c r="H114" s="26">
+        <f>RSDAFC!L76*$M$35</f>
         <v>1.222361012943445E-2</v>
       </c>
-      <c r="I113" s="26">
-        <f>RSDAFC!M76*$M$34</f>
+      <c r="I114" s="26">
+        <f>RSDAFC!M76*$M$35</f>
         <v>1.222361012943445E-2</v>
       </c>
-      <c r="K113" t="str">
+      <c r="K114" t="str">
         <f>RSDAFC!C76</f>
         <v>R-SW_Det_GAS_N2</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C114" t="s">
-        <v>208</v>
-      </c>
-      <c r="D114" t="s">
-        <v>110</v>
-      </c>
-      <c r="H114" s="26">
-        <f>RSDAFC!L77*$M$34</f>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C115" t="s">
+        <v>208</v>
+      </c>
+      <c r="D115" t="s">
+        <v>110</v>
+      </c>
+      <c r="H115" s="26">
+        <f>RSDAFC!L77*$M$35</f>
         <v>1.222361012943445E-2</v>
       </c>
-      <c r="I114" s="26">
-        <f>RSDAFC!M77*$M$34</f>
+      <c r="I115" s="26">
+        <f>RSDAFC!M77*$M$35</f>
         <v>1.222361012943445E-2</v>
       </c>
-      <c r="K114" t="str">
+      <c r="K115" t="str">
         <f>RSDAFC!C77</f>
         <v>R-SW_Det_GAS_N2</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C115" t="s">
-        <v>208</v>
-      </c>
-      <c r="D115" t="s">
-        <v>110</v>
-      </c>
-      <c r="H115" s="26">
-        <f>RSDAFC!L78*$M$34</f>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C116" t="s">
+        <v>208</v>
+      </c>
+      <c r="D116" t="s">
+        <v>110</v>
+      </c>
+      <c r="H116" s="26">
+        <f>RSDAFC!L78*$M$35</f>
         <v>1.222361012943445E-2</v>
       </c>
-      <c r="I115" s="26">
-        <f>RSDAFC!M78*$M$34</f>
+      <c r="I116" s="26">
+        <f>RSDAFC!M78*$M$35</f>
         <v>1.222361012943445E-2</v>
       </c>
-      <c r="K115" t="str">
+      <c r="K116" t="str">
         <f>RSDAFC!C78</f>
         <v>R-SW_Det_GAS_N3</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C116" t="s">
-        <v>208</v>
-      </c>
-      <c r="D116" t="s">
-        <v>110</v>
-      </c>
-      <c r="H116" s="26">
-        <f>RSDAFC!L79*$M$34</f>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C117" t="s">
+        <v>208</v>
+      </c>
+      <c r="D117" t="s">
+        <v>110</v>
+      </c>
+      <c r="H117" s="26">
+        <f>RSDAFC!L79*$M$35</f>
         <v>1.222361012943445E-2</v>
       </c>
-      <c r="I116" s="26">
-        <f>RSDAFC!M79*$M$34</f>
+      <c r="I117" s="26">
+        <f>RSDAFC!M79*$M$35</f>
         <v>1.222361012943445E-2</v>
       </c>
-      <c r="K116" t="str">
+      <c r="K117" t="str">
         <f>RSDAFC!C79</f>
         <v>R-SW_Det_GAS_N3</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C117" t="s">
-        <v>208</v>
-      </c>
-      <c r="D117" t="s">
-        <v>110</v>
-      </c>
-      <c r="H117" s="26">
-        <f>RSDAFC!L80*$M$34</f>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C118" t="s">
+        <v>208</v>
+      </c>
+      <c r="D118" t="s">
+        <v>110</v>
+      </c>
+      <c r="H118" s="26">
+        <f>RSDAFC!L80*$M$35</f>
         <v>4.782102180462415E-2</v>
       </c>
-      <c r="I117" s="26">
-        <f>RSDAFC!M80*$M$34</f>
+      <c r="I118" s="26">
+        <f>RSDAFC!M80*$M$35</f>
         <v>4.782102180462415E-2</v>
       </c>
-      <c r="K117" t="str">
+      <c r="K118" t="str">
         <f>RSDAFC!C80</f>
         <v>R-SW_Det_HET_N1</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C118" t="s">
-        <v>208</v>
-      </c>
-      <c r="D118" t="s">
-        <v>110</v>
-      </c>
-      <c r="H118" s="26">
-        <f>RSDAFC!L81*$M$34</f>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C119" t="s">
+        <v>208</v>
+      </c>
+      <c r="D119" t="s">
+        <v>110</v>
+      </c>
+      <c r="H119" s="26">
+        <f>RSDAFC!L81*$M$35</f>
         <v>4.782102180462415E-2</v>
       </c>
-      <c r="I118" s="26">
-        <f>RSDAFC!M81*$M$34</f>
+      <c r="I119" s="26">
+        <f>RSDAFC!M81*$M$35</f>
         <v>4.782102180462415E-2</v>
       </c>
-      <c r="K118" t="str">
+      <c r="K119" t="str">
         <f>RSDAFC!C81</f>
         <v>R-SW_Det_HET_N1</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C119" t="s">
-        <v>208</v>
-      </c>
-      <c r="D119" t="s">
-        <v>110</v>
-      </c>
-      <c r="H119" s="26">
-        <f>RSDAFC!L82*$M$34</f>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C120" t="s">
+        <v>208</v>
+      </c>
+      <c r="D120" t="s">
+        <v>110</v>
+      </c>
+      <c r="H120" s="26">
+        <f>RSDAFC!L82*$M$35</f>
         <v>4.782102180462415E-2</v>
       </c>
-      <c r="I119" s="26">
-        <f>RSDAFC!M82*$M$34</f>
+      <c r="I120" s="26">
+        <f>RSDAFC!M82*$M$35</f>
         <v>4.782102180462415E-2</v>
       </c>
-      <c r="K119" t="str">
+      <c r="K120" t="str">
         <f>RSDAFC!C82</f>
         <v>R-SW_Det_HET_N2</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C120" t="s">
-        <v>208</v>
-      </c>
-      <c r="D120" t="s">
-        <v>110</v>
-      </c>
-      <c r="H120" s="26">
-        <f>RSDAFC!L83*$M$34</f>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C121" t="s">
+        <v>208</v>
+      </c>
+      <c r="D121" t="s">
+        <v>110</v>
+      </c>
+      <c r="H121" s="26">
+        <f>RSDAFC!L83*$M$35</f>
         <v>4.782102180462415E-2</v>
       </c>
-      <c r="I120" s="26">
-        <f>RSDAFC!M83*$M$34</f>
+      <c r="I121" s="26">
+        <f>RSDAFC!M83*$M$35</f>
         <v>4.782102180462415E-2</v>
       </c>
-      <c r="K120" t="str">
+      <c r="K121" t="str">
         <f>RSDAFC!C83</f>
         <v>R-SW_Det_HET_N2</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C121" t="s">
-        <v>208</v>
-      </c>
-      <c r="D121" t="s">
-        <v>110</v>
-      </c>
-      <c r="H121" s="26">
-        <f>RSDAFC!L84*$M$34</f>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C122" t="s">
+        <v>208</v>
+      </c>
+      <c r="D122" t="s">
+        <v>110</v>
+      </c>
+      <c r="H122" s="26">
+        <f>RSDAFC!L84*$M$35</f>
         <v>1.5039738210625601E-2</v>
       </c>
-      <c r="I121" s="26">
-        <f>RSDAFC!M84*$M$34</f>
+      <c r="I122" s="26">
+        <f>RSDAFC!M84*$M$35</f>
         <v>1.5039738210625601E-2</v>
       </c>
-      <c r="K121" t="str">
+      <c r="K122" t="str">
         <f>RSDAFC!C84</f>
         <v>R-SW_Det_KER_N1</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C122" t="s">
-        <v>208</v>
-      </c>
-      <c r="D122" t="s">
-        <v>110</v>
-      </c>
-      <c r="H122" s="26">
-        <f>RSDAFC!L85*$M$34</f>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C123" t="s">
+        <v>208</v>
+      </c>
+      <c r="D123" t="s">
+        <v>110</v>
+      </c>
+      <c r="H123" s="26">
+        <f>RSDAFC!L85*$M$35</f>
         <v>1.5039738210625601E-2</v>
       </c>
-      <c r="I122" s="26">
-        <f>RSDAFC!M85*$M$34</f>
+      <c r="I123" s="26">
+        <f>RSDAFC!M85*$M$35</f>
         <v>1.5039738210625601E-2</v>
       </c>
-      <c r="K122" t="str">
+      <c r="K123" t="str">
         <f>RSDAFC!C85</f>
         <v>R-SW_Det_KER_N1</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C123" t="s">
-        <v>208</v>
-      </c>
-      <c r="D123" t="s">
-        <v>110</v>
-      </c>
-      <c r="H123" s="26">
-        <f>RSDAFC!L86*$M$34</f>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C124" t="s">
+        <v>208</v>
+      </c>
+      <c r="D124" t="s">
+        <v>110</v>
+      </c>
+      <c r="H124" s="26">
+        <f>RSDAFC!L86*$M$35</f>
         <v>1.5039738210625601E-2</v>
       </c>
-      <c r="I123" s="26">
-        <f>RSDAFC!M86*$M$34</f>
+      <c r="I124" s="26">
+        <f>RSDAFC!M86*$M$35</f>
         <v>1.5039738210625601E-2</v>
       </c>
-      <c r="K123" t="str">
+      <c r="K124" t="str">
         <f>RSDAFC!C86</f>
         <v>R-SW_Det_KER_N2</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C124" t="s">
-        <v>208</v>
-      </c>
-      <c r="D124" t="s">
-        <v>110</v>
-      </c>
-      <c r="H124" s="26">
-        <f>RSDAFC!L87*$M$34</f>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C125" t="s">
+        <v>208</v>
+      </c>
+      <c r="D125" t="s">
+        <v>110</v>
+      </c>
+      <c r="H125" s="26">
+        <f>RSDAFC!L87*$M$35</f>
         <v>1.5039738210625601E-2</v>
       </c>
-      <c r="I124" s="26">
-        <f>RSDAFC!M87*$M$34</f>
+      <c r="I125" s="26">
+        <f>RSDAFC!M87*$M$35</f>
         <v>1.5039738210625601E-2</v>
       </c>
-      <c r="K124" t="str">
+      <c r="K125" t="str">
         <f>RSDAFC!C87</f>
         <v>R-SW_Det_KER_N2</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C125" t="s">
-        <v>208</v>
-      </c>
-      <c r="D125" t="s">
-        <v>110</v>
-      </c>
-      <c r="H125" s="26">
-        <f>RSDAFC!L88*$M$34</f>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C126" t="s">
+        <v>208</v>
+      </c>
+      <c r="D126" t="s">
+        <v>110</v>
+      </c>
+      <c r="H126" s="26">
+        <f>RSDAFC!L88*$M$35</f>
         <v>1.5039738210625601E-2</v>
       </c>
-      <c r="I125" s="26">
-        <f>RSDAFC!M88*$M$34</f>
+      <c r="I126" s="26">
+        <f>RSDAFC!M88*$M$35</f>
         <v>1.5039738210625601E-2</v>
       </c>
-      <c r="K125" t="str">
+      <c r="K126" t="str">
         <f>RSDAFC!C88</f>
         <v>R-SW_Det_KER_N3</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C126" t="s">
-        <v>208</v>
-      </c>
-      <c r="D126" t="s">
-        <v>110</v>
-      </c>
-      <c r="H126" s="26">
-        <f>RSDAFC!L89*$M$34</f>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C127" t="s">
+        <v>208</v>
+      </c>
+      <c r="D127" t="s">
+        <v>110</v>
+      </c>
+      <c r="H127" s="26">
+        <f>RSDAFC!L89*$M$35</f>
         <v>1.5039738210625601E-2</v>
       </c>
-      <c r="I126" s="26">
-        <f>RSDAFC!M89*$M$34</f>
+      <c r="I127" s="26">
+        <f>RSDAFC!M89*$M$35</f>
         <v>1.5039738210625601E-2</v>
       </c>
-      <c r="K126" t="str">
+      <c r="K127" t="str">
         <f>RSDAFC!C89</f>
         <v>R-SW_Det_KER_N3</v>
-      </c>
-    </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A127" s="39"/>
-      <c r="B127" s="39"/>
-      <c r="C127" s="39" t="s">
-        <v>208</v>
-      </c>
-      <c r="D127" s="39" t="s">
-        <v>110</v>
-      </c>
-      <c r="E127" s="39"/>
-      <c r="F127" s="39"/>
-      <c r="G127" s="39"/>
-      <c r="H127" s="40">
-        <f>H133</f>
-        <v>2.6433948538654248E-2</v>
-      </c>
-      <c r="I127" s="40">
-        <f>I133</f>
-        <v>2.6433948538654248E-2</v>
-      </c>
-      <c r="J127" s="39"/>
-      <c r="K127" s="39" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="128" spans="1:11" x14ac:dyDescent="0.25">
@@ -5636,7 +5913,7 @@
       </c>
       <c r="J128" s="39"/>
       <c r="K128" s="39" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="129" spans="1:11" x14ac:dyDescent="0.25">
@@ -5652,16 +5929,16 @@
       <c r="F129" s="39"/>
       <c r="G129" s="39"/>
       <c r="H129" s="40">
-        <f>H126</f>
-        <v>1.5039738210625601E-2</v>
+        <f>H135</f>
+        <v>2.6433948538654248E-2</v>
       </c>
       <c r="I129" s="40">
-        <f>I126</f>
-        <v>1.5039738210625601E-2</v>
+        <f>I135</f>
+        <v>2.6433948538654248E-2</v>
       </c>
       <c r="J129" s="39"/>
       <c r="K129" s="39" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="130" spans="1:11" x14ac:dyDescent="0.25">
@@ -5677,702 +5954,722 @@
       <c r="F130" s="39"/>
       <c r="G130" s="39"/>
       <c r="H130" s="40">
-        <f>H129</f>
+        <f>H127</f>
         <v>1.5039738210625601E-2</v>
       </c>
       <c r="I130" s="40">
-        <f>I129</f>
+        <f>I127</f>
         <v>1.5039738210625601E-2</v>
       </c>
       <c r="J130" s="39"/>
       <c r="K130" s="39" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A131" s="39"/>
+      <c r="B131" s="39"/>
+      <c r="C131" s="39" t="s">
+        <v>208</v>
+      </c>
+      <c r="D131" s="39" t="s">
+        <v>110</v>
+      </c>
+      <c r="E131" s="39"/>
+      <c r="F131" s="39"/>
+      <c r="G131" s="39"/>
+      <c r="H131" s="40">
+        <f>H130</f>
+        <v>1.5039738210625601E-2</v>
+      </c>
+      <c r="I131" s="40">
+        <f>I130</f>
+        <v>1.5039738210625601E-2</v>
+      </c>
+      <c r="J131" s="39"/>
+      <c r="K131" s="39" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C131" t="s">
-        <v>208</v>
-      </c>
-      <c r="D131" t="s">
-        <v>110</v>
-      </c>
-      <c r="H131" s="26">
-        <f>RSDAFC!L90*$M$34</f>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C132" t="s">
+        <v>208</v>
+      </c>
+      <c r="D132" t="s">
+        <v>110</v>
+      </c>
+      <c r="H132" s="26">
+        <f>RSDAFC!L90*$M$35</f>
         <v>2.10969847812758E-2</v>
       </c>
-      <c r="I131" s="26">
-        <f>RSDAFC!M90*$M$34</f>
+      <c r="I132" s="26">
+        <f>RSDAFC!M90*$M$35</f>
         <v>2.10969847812758E-2</v>
       </c>
-      <c r="K131" t="str">
+      <c r="K132" t="str">
         <f>RSDAFC!C90</f>
         <v>R-SW_Det_LPG_N1</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C132" t="s">
-        <v>208</v>
-      </c>
-      <c r="D132" t="s">
-        <v>110</v>
-      </c>
-      <c r="H132" s="26">
-        <f>RSDAFC!L91*$M$34</f>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C133" t="s">
+        <v>208</v>
+      </c>
+      <c r="D133" t="s">
+        <v>110</v>
+      </c>
+      <c r="H133" s="26">
+        <f>RSDAFC!L91*$M$35</f>
         <v>2.10969847812758E-2</v>
       </c>
-      <c r="I132" s="26">
-        <f>RSDAFC!M91*$M$34</f>
+      <c r="I133" s="26">
+        <f>RSDAFC!M91*$M$35</f>
         <v>2.10969847812758E-2</v>
       </c>
-      <c r="K132" t="str">
+      <c r="K133" t="str">
         <f>RSDAFC!C91</f>
         <v>R-SW_Det_LPG_N1</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C133" t="s">
-        <v>208</v>
-      </c>
-      <c r="D133" t="s">
-        <v>110</v>
-      </c>
-      <c r="H133" s="26">
-        <f>RSDAFC!L92*$M$34</f>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C134" t="s">
+        <v>208</v>
+      </c>
+      <c r="D134" t="s">
+        <v>110</v>
+      </c>
+      <c r="H134" s="26">
+        <f>RSDAFC!L92*$M$35</f>
         <v>2.6433948538654248E-2</v>
       </c>
-      <c r="I133" s="26">
-        <f>RSDAFC!M92*$M$34</f>
+      <c r="I134" s="26">
+        <f>RSDAFC!M92*$M$35</f>
         <v>2.6433948538654248E-2</v>
       </c>
-      <c r="K133" t="str">
+      <c r="K134" t="str">
         <f>RSDAFC!C92</f>
         <v>R-SW_Det_WOO_N1</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C134" t="s">
-        <v>208</v>
-      </c>
-      <c r="D134" t="s">
-        <v>110</v>
-      </c>
-      <c r="H134" s="26">
-        <f>RSDAFC!L93*$M$34</f>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C135" t="s">
+        <v>208</v>
+      </c>
+      <c r="D135" t="s">
+        <v>110</v>
+      </c>
+      <c r="H135" s="26">
+        <f>RSDAFC!L93*$M$35</f>
         <v>2.6433948538654248E-2</v>
       </c>
-      <c r="I134" s="26">
-        <f>RSDAFC!M93*$M$34</f>
+      <c r="I135" s="26">
+        <f>RSDAFC!M93*$M$35</f>
         <v>2.6433948538654248E-2</v>
       </c>
-      <c r="K134" t="str">
+      <c r="K135" t="str">
         <f>RSDAFC!C93</f>
         <v>R-SW_Det_WOO_N1</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C135" t="s">
-        <v>208</v>
-      </c>
-      <c r="D135" t="s">
-        <v>110</v>
-      </c>
-      <c r="H135" s="26">
-        <f>RSDAFA!L2*$M$34</f>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C136" t="s">
+        <v>208</v>
+      </c>
+      <c r="D136" t="s">
+        <v>110</v>
+      </c>
+      <c r="H136" s="26">
+        <f>RSDAFA!L2*$M$35</f>
         <v>9.59298200649405E-3</v>
       </c>
-      <c r="I135" s="26">
-        <f>RSDAFA!M2*$M$34</f>
+      <c r="I136" s="26">
+        <f>RSDAFA!M2*$M$35</f>
         <v>9.59298200649405E-3</v>
       </c>
-      <c r="K135" s="26" t="str">
+      <c r="K136" s="26" t="str">
         <f>RSDAFA!C2</f>
         <v>R-SH_Apt_ELC_HPN1</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C136" t="s">
-        <v>208</v>
-      </c>
-      <c r="D136" t="s">
-        <v>110</v>
-      </c>
-      <c r="H136" s="26">
-        <f>RSDAFA!L3*$M$34</f>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C137" t="s">
+        <v>208</v>
+      </c>
+      <c r="D137" t="s">
+        <v>110</v>
+      </c>
+      <c r="H137" s="26">
+        <f>RSDAFA!L3*$M$35</f>
         <v>9.59298200649405E-3</v>
       </c>
-      <c r="I136" s="26">
-        <f>RSDAFA!M3*$M$34</f>
+      <c r="I137" s="26">
+        <f>RSDAFA!M3*$M$35</f>
         <v>9.59298200649405E-3</v>
       </c>
-      <c r="K136" s="26" t="str">
+      <c r="K137" s="26" t="str">
         <f>RSDAFA!C3</f>
         <v>R-SH_Apt_ELC_HPN2</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C137" t="s">
-        <v>208</v>
-      </c>
-      <c r="D137" t="s">
-        <v>110</v>
-      </c>
-      <c r="H137" s="26">
-        <f>RSDAFA!L4*$M$34</f>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C138" t="s">
+        <v>208</v>
+      </c>
+      <c r="D138" t="s">
+        <v>110</v>
+      </c>
+      <c r="H138" s="26">
+        <f>RSDAFA!L4*$M$35</f>
         <v>9.59298200649405E-3</v>
       </c>
-      <c r="I137" s="26">
-        <f>RSDAFA!M4*$M$34</f>
+      <c r="I138" s="26">
+        <f>RSDAFA!M4*$M$35</f>
         <v>9.59298200649405E-3</v>
       </c>
-      <c r="K137" s="26" t="str">
+      <c r="K138" s="26" t="str">
         <f>RSDAFA!C4</f>
         <v>R-SH_Apt_ELC_HPN3</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C138" t="s">
-        <v>208</v>
-      </c>
-      <c r="D138" t="s">
-        <v>110</v>
-      </c>
-      <c r="H138" s="26">
-        <f>RSDAFA!L5*$M$34</f>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C139" t="s">
+        <v>208</v>
+      </c>
+      <c r="D139" t="s">
+        <v>110</v>
+      </c>
+      <c r="H139" s="26">
+        <f>RSDAFA!L5*$M$35</f>
         <v>9.59298200649405E-3</v>
       </c>
-      <c r="I138" s="26">
-        <f>RSDAFA!M5*$M$34</f>
+      <c r="I139" s="26">
+        <f>RSDAFA!M5*$M$35</f>
         <v>9.59298200649405E-3</v>
       </c>
-      <c r="K138" s="26" t="str">
+      <c r="K139" s="26" t="str">
         <f>RSDAFA!C5</f>
         <v>R-SH_Apt_ELC_N1</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C139" t="s">
-        <v>208</v>
-      </c>
-      <c r="D139" t="s">
-        <v>110</v>
-      </c>
-      <c r="H139" s="26">
-        <f>RSDAFA!L6*$M$34</f>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C140" t="s">
+        <v>208</v>
+      </c>
+      <c r="D140" t="s">
+        <v>110</v>
+      </c>
+      <c r="H140" s="26">
+        <f>RSDAFA!L6*$M$35</f>
         <v>5.9295434183648001E-3</v>
       </c>
-      <c r="I139" s="26">
-        <f>RSDAFA!M6*$M$34</f>
+      <c r="I140" s="26">
+        <f>RSDAFA!M6*$M$35</f>
         <v>5.9295434183648001E-3</v>
       </c>
-      <c r="K139" s="26" t="str">
+      <c r="K140" s="26" t="str">
         <f>RSDAFA!C6</f>
         <v>R-SH_Apt_GAS_N1</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C140" t="s">
-        <v>208</v>
-      </c>
-      <c r="D140" t="s">
-        <v>110</v>
-      </c>
-      <c r="H140" s="26">
-        <f>RSDAFA!L7*$M$34</f>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C141" t="s">
+        <v>208</v>
+      </c>
+      <c r="D141" t="s">
+        <v>110</v>
+      </c>
+      <c r="H141" s="26">
+        <f>RSDAFA!L7*$M$35</f>
         <v>1.8679913115832E-2</v>
       </c>
-      <c r="I140" s="26">
-        <f>RSDAFA!M7*$M$34</f>
+      <c r="I141" s="26">
+        <f>RSDAFA!M7*$M$35</f>
         <v>1.8679913115832E-2</v>
       </c>
-      <c r="K140" s="26" t="str">
+      <c r="K141" s="26" t="str">
         <f>RSDAFA!C7</f>
         <v>R-SH_Apt_KER_N1</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C141" t="s">
-        <v>208</v>
-      </c>
-      <c r="D141" t="s">
-        <v>110</v>
-      </c>
-      <c r="H141" s="26">
-        <f>RSDAFA!L8*$M$34</f>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C142" t="s">
+        <v>208</v>
+      </c>
+      <c r="D142" t="s">
+        <v>110</v>
+      </c>
+      <c r="H142" s="26">
+        <f>RSDAFA!L8*$M$35</f>
         <v>1.1539296595339751E-2</v>
       </c>
-      <c r="I141" s="26">
-        <f>RSDAFA!M8*$M$34</f>
+      <c r="I142" s="26">
+        <f>RSDAFA!M8*$M$35</f>
         <v>1.1539296595339751E-2</v>
       </c>
-      <c r="K141" s="26" t="str">
+      <c r="K142" s="26" t="str">
         <f>RSDAFA!C8</f>
         <v>R-SH_Apt_LPG_N1</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C142" t="s">
-        <v>208</v>
-      </c>
-      <c r="D142" t="s">
-        <v>110</v>
-      </c>
-      <c r="H142" s="26">
-        <f>RSDAFA!L9*$M$34</f>
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C143" t="s">
+        <v>208</v>
+      </c>
+      <c r="D143" t="s">
+        <v>110</v>
+      </c>
+      <c r="H143" s="26">
+        <f>RSDAFA!L9*$M$35</f>
         <v>8.8239524029044506E-3</v>
       </c>
-      <c r="I142" s="26">
-        <f>RSDAFA!M9*$M$34</f>
+      <c r="I143" s="26">
+        <f>RSDAFA!M9*$M$35</f>
         <v>8.8239524029044506E-3</v>
       </c>
-      <c r="K142" s="26" t="str">
+      <c r="K143" s="26" t="str">
         <f>RSDAFA!C9</f>
         <v>R-SH_Apt_WOO_N1</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C143" t="s">
-        <v>208</v>
-      </c>
-      <c r="D143" t="s">
-        <v>110</v>
-      </c>
-      <c r="H143" s="26">
-        <f>RSDAFA!L10*$M$34</f>
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C144" t="s">
+        <v>208</v>
+      </c>
+      <c r="D144" t="s">
+        <v>110</v>
+      </c>
+      <c r="H144" s="26">
+        <f>RSDAFA!L10*$M$35</f>
         <v>1.2326631289923951E-2</v>
       </c>
-      <c r="I143" s="26">
-        <f>RSDAFA!M10*$M$34</f>
+      <c r="I144" s="26">
+        <f>RSDAFA!M10*$M$35</f>
         <v>1.2326631289923951E-2</v>
       </c>
-      <c r="K143" s="26" t="str">
+      <c r="K144" s="26" t="str">
         <f>RSDAFA!C10</f>
         <v>R-SH_Att_ELC_HPN1</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C144" t="s">
-        <v>208</v>
-      </c>
-      <c r="D144" t="s">
-        <v>110</v>
-      </c>
-      <c r="H144" s="26">
-        <f>RSDAFA!L11*$M$34</f>
+    <row r="145" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C145" t="s">
+        <v>208</v>
+      </c>
+      <c r="D145" t="s">
+        <v>110</v>
+      </c>
+      <c r="H145" s="26">
+        <f>RSDAFA!L11*$M$35</f>
         <v>1.2326631289923951E-2</v>
       </c>
-      <c r="I144" s="26">
-        <f>RSDAFA!M11*$M$34</f>
+      <c r="I145" s="26">
+        <f>RSDAFA!M11*$M$35</f>
         <v>1.2326631289923951E-2</v>
       </c>
-      <c r="K144" s="26" t="str">
+      <c r="K145" s="26" t="str">
         <f>RSDAFA!C11</f>
         <v>R-SH_Att_ELC_HPN2</v>
       </c>
     </row>
-    <row r="145" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C145" t="s">
-        <v>208</v>
-      </c>
-      <c r="D145" t="s">
-        <v>110</v>
-      </c>
-      <c r="H145" s="26">
-        <f>RSDAFA!L12*$M$34</f>
+    <row r="146" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C146" t="s">
+        <v>208</v>
+      </c>
+      <c r="D146" t="s">
+        <v>110</v>
+      </c>
+      <c r="H146" s="26">
+        <f>RSDAFA!L12*$M$35</f>
         <v>1.2326631289923951E-2</v>
       </c>
-      <c r="I145" s="26">
-        <f>RSDAFA!M12*$M$34</f>
+      <c r="I146" s="26">
+        <f>RSDAFA!M12*$M$35</f>
         <v>1.2326631289923951E-2</v>
       </c>
-      <c r="K145" s="26" t="str">
+      <c r="K146" s="26" t="str">
         <f>RSDAFA!C12</f>
         <v>R-SH_Att_ELC_HPN3</v>
       </c>
     </row>
-    <row r="146" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C146" t="s">
-        <v>208</v>
-      </c>
-      <c r="D146" t="s">
-        <v>110</v>
-      </c>
-      <c r="H146" s="26">
-        <f>RSDAFA!L13*$M$34</f>
+    <row r="147" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C147" t="s">
+        <v>208</v>
+      </c>
+      <c r="D147" t="s">
+        <v>110</v>
+      </c>
+      <c r="H147" s="26">
+        <f>RSDAFA!L13*$M$35</f>
         <v>1.2326631289923951E-2</v>
       </c>
-      <c r="I146" s="26">
-        <f>RSDAFA!M13*$M$34</f>
+      <c r="I147" s="26">
+        <f>RSDAFA!M13*$M$35</f>
         <v>1.2326631289923951E-2</v>
       </c>
-      <c r="K146" s="26" t="str">
+      <c r="K147" s="26" t="str">
         <f>RSDAFA!C13</f>
         <v>R-SH_Att_ELC_N1</v>
       </c>
     </row>
-    <row r="147" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C147" t="s">
-        <v>208</v>
-      </c>
-      <c r="D147" t="s">
-        <v>110</v>
-      </c>
-      <c r="H147" s="26">
-        <f>RSDAFA!L14*$M$34</f>
+    <row r="148" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C148" t="s">
+        <v>208</v>
+      </c>
+      <c r="D148" t="s">
+        <v>110</v>
+      </c>
+      <c r="H148" s="26">
+        <f>RSDAFA!L14*$M$35</f>
         <v>1.10479456620104E-2</v>
       </c>
-      <c r="I147" s="26">
-        <f>RSDAFA!M14*$M$34</f>
+      <c r="I148" s="26">
+        <f>RSDAFA!M14*$M$35</f>
         <v>1.10479456620104E-2</v>
       </c>
-      <c r="K147" s="26" t="str">
+      <c r="K148" s="26" t="str">
         <f>RSDAFA!C14</f>
         <v>R-SH_Att_GAS_N1</v>
       </c>
     </row>
-    <row r="148" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C148" t="s">
-        <v>208</v>
-      </c>
-      <c r="D148" t="s">
-        <v>110</v>
-      </c>
-      <c r="H148" s="26">
-        <f>RSDAFA!L15*$M$34</f>
+    <row r="149" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C149" t="s">
+        <v>208</v>
+      </c>
+      <c r="D149" t="s">
+        <v>110</v>
+      </c>
+      <c r="H149" s="26">
+        <f>RSDAFA!L15*$M$35</f>
         <v>1.418438071184145E-2</v>
       </c>
-      <c r="I148" s="26">
-        <f>RSDAFA!M15*$M$34</f>
+      <c r="I149" s="26">
+        <f>RSDAFA!M15*$M$35</f>
         <v>1.418438071184145E-2</v>
       </c>
-      <c r="K148" s="26" t="str">
+      <c r="K149" s="26" t="str">
         <f>RSDAFA!C15</f>
         <v>R-SH_Att_KER_N1</v>
       </c>
     </row>
-    <row r="149" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C149" t="s">
-        <v>208</v>
-      </c>
-      <c r="D149" t="s">
-        <v>110</v>
-      </c>
-      <c r="H149" s="26">
-        <f>RSDAFA!L16*$M$34</f>
+    <row r="150" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C150" t="s">
+        <v>208</v>
+      </c>
+      <c r="D150" t="s">
+        <v>110</v>
+      </c>
+      <c r="H150" s="26">
+        <f>RSDAFA!L16*$M$35</f>
         <v>1.5468436444358601E-2</v>
       </c>
-      <c r="I149" s="26">
-        <f>RSDAFA!M16*$M$34</f>
+      <c r="I150" s="26">
+        <f>RSDAFA!M16*$M$35</f>
         <v>1.5468436444358601E-2</v>
       </c>
-      <c r="K149" s="26" t="str">
+      <c r="K150" s="26" t="str">
         <f>RSDAFA!C16</f>
         <v>R-SH_Att_LPG_N1</v>
       </c>
     </row>
-    <row r="150" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C150" t="s">
-        <v>208</v>
-      </c>
-      <c r="D150" t="s">
-        <v>110</v>
-      </c>
-      <c r="H150" s="26">
-        <f>RSDAFA!L17*$M$34</f>
+    <row r="151" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C151" t="s">
+        <v>208</v>
+      </c>
+      <c r="D151" t="s">
+        <v>110</v>
+      </c>
+      <c r="H151" s="26">
+        <f>RSDAFA!L17*$M$35</f>
         <v>3.7533433216504153E-2</v>
       </c>
-      <c r="I150" s="26">
-        <f>RSDAFA!M17*$M$34</f>
+      <c r="I151" s="26">
+        <f>RSDAFA!M17*$M$35</f>
         <v>3.7533433216504153E-2</v>
       </c>
-      <c r="K150" s="26" t="str">
+      <c r="K151" s="26" t="str">
         <f>RSDAFA!C17</f>
         <v>R-SH_Att_WOO_N1</v>
       </c>
     </row>
-    <row r="151" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C151" t="s">
-        <v>208</v>
-      </c>
-      <c r="D151" t="s">
-        <v>110</v>
-      </c>
-      <c r="H151" s="26">
-        <f>RSDAFA!L18*$M$34</f>
+    <row r="152" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C152" t="s">
+        <v>208</v>
+      </c>
+      <c r="D152" t="s">
+        <v>110</v>
+      </c>
+      <c r="H152" s="26">
+        <f>RSDAFA!L18*$M$35</f>
         <v>2.08072041359634E-2</v>
       </c>
-      <c r="I151" s="26">
-        <f>RSDAFA!M18*$M$34</f>
+      <c r="I152" s="26">
+        <f>RSDAFA!M18*$M$35</f>
         <v>2.08072041359634E-2</v>
       </c>
-      <c r="K151" s="26" t="str">
+      <c r="K152" s="26" t="str">
         <f>RSDAFA!C18</f>
         <v>R-SH_Det_ELC_HPN1</v>
       </c>
     </row>
-    <row r="152" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C152" t="s">
-        <v>208</v>
-      </c>
-      <c r="D152" t="s">
-        <v>110</v>
-      </c>
-      <c r="H152" s="26">
-        <f>RSDAFA!L19*$M$34</f>
+    <row r="153" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C153" t="s">
+        <v>208</v>
+      </c>
+      <c r="D153" t="s">
+        <v>110</v>
+      </c>
+      <c r="H153" s="26">
+        <f>RSDAFA!L19*$M$35</f>
         <v>2.08072041359634E-2</v>
       </c>
-      <c r="I152" s="26">
-        <f>RSDAFA!M19*$M$34</f>
+      <c r="I153" s="26">
+        <f>RSDAFA!M19*$M$35</f>
         <v>2.08072041359634E-2</v>
       </c>
-      <c r="K152" s="26" t="str">
+      <c r="K153" s="26" t="str">
         <f>RSDAFA!C19</f>
         <v>R-SH_Det_ELC_HPN2</v>
       </c>
     </row>
-    <row r="153" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C153" t="s">
-        <v>208</v>
-      </c>
-      <c r="D153" t="s">
-        <v>110</v>
-      </c>
-      <c r="H153" s="26">
-        <f>RSDAFA!L20*$M$34</f>
+    <row r="154" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C154" t="s">
+        <v>208</v>
+      </c>
+      <c r="D154" t="s">
+        <v>110</v>
+      </c>
+      <c r="H154" s="26">
+        <f>RSDAFA!L20*$M$35</f>
         <v>2.08072041359634E-2</v>
       </c>
-      <c r="I153" s="26">
-        <f>RSDAFA!M20*$M$34</f>
+      <c r="I154" s="26">
+        <f>RSDAFA!M20*$M$35</f>
         <v>2.08072041359634E-2</v>
       </c>
-      <c r="K153" s="26" t="str">
+      <c r="K154" s="26" t="str">
         <f>RSDAFA!C20</f>
         <v>R-SH_Det_ELC_HPN3</v>
       </c>
     </row>
-    <row r="154" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C154" t="s">
-        <v>208</v>
-      </c>
-      <c r="D154" t="s">
-        <v>110</v>
-      </c>
-      <c r="H154" s="26">
-        <f>RSDAFA!L21*$M$34</f>
+    <row r="155" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C155" t="s">
+        <v>208</v>
+      </c>
+      <c r="D155" t="s">
+        <v>110</v>
+      </c>
+      <c r="H155" s="26">
+        <f>RSDAFA!L21*$M$35</f>
         <v>2.08072041359634E-2</v>
       </c>
-      <c r="I154" s="26">
-        <f>RSDAFA!M21*$M$34</f>
+      <c r="I155" s="26">
+        <f>RSDAFA!M21*$M$35</f>
         <v>2.08072041359634E-2</v>
       </c>
-      <c r="K154" s="26" t="str">
+      <c r="K155" s="26" t="str">
         <f>RSDAFA!C21</f>
         <v>R-SH_Det_ELC_N1</v>
       </c>
     </row>
-    <row r="155" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C155" t="s">
-        <v>208</v>
-      </c>
-      <c r="D155" t="s">
-        <v>110</v>
-      </c>
-      <c r="H155" s="26">
-        <f>RSDAFA!L22*$M$34</f>
+    <row r="156" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C156" t="s">
+        <v>208</v>
+      </c>
+      <c r="D156" t="s">
+        <v>110</v>
+      </c>
+      <c r="H156" s="26">
+        <f>RSDAFA!L22*$M$35</f>
         <v>1.852031558004625E-2</v>
       </c>
-      <c r="I155" s="26">
-        <f>RSDAFA!M22*$M$34</f>
+      <c r="I156" s="26">
+        <f>RSDAFA!M22*$M$35</f>
         <v>1.852031558004625E-2</v>
       </c>
-      <c r="K155" s="26" t="str">
+      <c r="K156" s="26" t="str">
         <f>RSDAFA!C22</f>
         <v>R-SH_Det_GAS_N1</v>
       </c>
     </row>
-    <row r="156" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C156" t="s">
-        <v>208</v>
-      </c>
-      <c r="D156" t="s">
-        <v>110</v>
-      </c>
-      <c r="H156" s="26">
-        <f>RSDAFA!L23*$M$34</f>
+    <row r="157" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C157" t="s">
+        <v>208</v>
+      </c>
+      <c r="D157" t="s">
+        <v>110</v>
+      </c>
+      <c r="H157" s="26">
+        <f>RSDAFA!L23*$M$35</f>
         <v>2.3310863988210799E-2</v>
       </c>
-      <c r="I156" s="26">
-        <f>RSDAFA!M23*$M$34</f>
+      <c r="I157" s="26">
+        <f>RSDAFA!M23*$M$35</f>
         <v>2.3310863988210799E-2</v>
       </c>
-      <c r="K156" s="26" t="str">
+      <c r="K157" s="26" t="str">
         <f>RSDAFA!C23</f>
         <v>R-SH_Det_KER_N1</v>
       </c>
     </row>
-    <row r="157" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C157" t="s">
-        <v>208</v>
-      </c>
-      <c r="D157" t="s">
-        <v>110</v>
-      </c>
-      <c r="H157" s="26">
-        <f>RSDAFA!L24*$M$34</f>
+    <row r="158" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C158" t="s">
+        <v>208</v>
+      </c>
+      <c r="D158" t="s">
+        <v>110</v>
+      </c>
+      <c r="H158" s="26">
+        <f>RSDAFA!L24*$M$35</f>
         <v>3.3516837935026751E-2</v>
       </c>
-      <c r="I157" s="26">
-        <f>RSDAFA!M24*$M$34</f>
+      <c r="I158" s="26">
+        <f>RSDAFA!M24*$M$35</f>
         <v>3.3516837935026751E-2</v>
       </c>
-      <c r="K157" s="26" t="str">
+      <c r="K158" s="26" t="str">
         <f>RSDAFA!C24</f>
         <v>R-SH_Det_LPG_N1</v>
       </c>
     </row>
-    <row r="158" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C158" t="s">
-        <v>208</v>
-      </c>
-      <c r="D158" t="s">
-        <v>110</v>
-      </c>
-      <c r="H158" s="26">
-        <f>RSDAFA!L25*$M$34</f>
+    <row r="159" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C159" t="s">
+        <v>208</v>
+      </c>
+      <c r="D159" t="s">
+        <v>110</v>
+      </c>
+      <c r="H159" s="26">
+        <f>RSDAFA!L25*$M$35</f>
         <v>4.5576915292050248E-2</v>
       </c>
-      <c r="I158" s="26">
-        <f>RSDAFA!M25*$M$34</f>
+      <c r="I159" s="26">
+        <f>RSDAFA!M25*$M$35</f>
         <v>4.5576915292050248E-2</v>
       </c>
-      <c r="K158" s="26" t="str">
+      <c r="K159" s="26" t="str">
         <f>RSDAFA!C25</f>
         <v>R-SH_Det_WOO_N1</v>
       </c>
     </row>
-    <row r="159" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C159" t="s">
-        <v>208</v>
-      </c>
-      <c r="D159" t="s">
-        <v>110</v>
-      </c>
-      <c r="H159" s="26">
-        <f>RSDAFA!L26*$M$34</f>
+    <row r="160" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C160" t="s">
+        <v>208</v>
+      </c>
+      <c r="D160" t="s">
+        <v>110</v>
+      </c>
+      <c r="H160" s="26">
+        <f>RSDAFA!L26*$M$35</f>
         <v>1.1367849827582301E-2</v>
       </c>
-      <c r="I159" s="26">
-        <f>RSDAFA!M26*$M$34</f>
+      <c r="I160" s="26">
+        <f>RSDAFA!M26*$M$35</f>
         <v>1.1367849827582301E-2</v>
       </c>
-      <c r="K159" s="26" t="str">
+      <c r="K160" s="26" t="str">
         <f>RSDAFA!C26</f>
         <v>R-WH_Apt_ELC_N1</v>
       </c>
     </row>
-    <row r="160" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C160" t="s">
-        <v>208</v>
-      </c>
-      <c r="D160" t="s">
-        <v>110</v>
-      </c>
-      <c r="H160" s="26">
-        <f>RSDAFA!L27*$M$34</f>
+    <row r="161" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C161" t="s">
+        <v>208</v>
+      </c>
+      <c r="D161" t="s">
+        <v>110</v>
+      </c>
+      <c r="H161" s="26">
+        <f>RSDAFA!L27*$M$35</f>
         <v>4.3149364997261599E-3</v>
       </c>
-      <c r="I160" s="26">
-        <f>RSDAFA!M27*$M$34</f>
+      <c r="I161" s="26">
+        <f>RSDAFA!M27*$M$35</f>
         <v>4.3149364997261599E-3</v>
       </c>
-      <c r="K160" s="26" t="str">
+      <c r="K161" s="26" t="str">
         <f>RSDAFA!C27</f>
         <v>R-WH_Apt_SOL_N1</v>
       </c>
     </row>
-    <row r="161" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C161" t="s">
-        <v>208</v>
-      </c>
-      <c r="D161" t="s">
-        <v>110</v>
-      </c>
-      <c r="H161" s="26">
-        <f>RSDAFA!L28*$M$34</f>
+    <row r="162" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C162" t="s">
+        <v>208</v>
+      </c>
+      <c r="D162" t="s">
+        <v>110</v>
+      </c>
+      <c r="H162" s="26">
+        <f>RSDAFA!L28*$M$35</f>
         <v>6.4637842351524498E-3</v>
       </c>
-      <c r="I161" s="26">
-        <f>RSDAFA!M28*$M$34</f>
+      <c r="I162" s="26">
+        <f>RSDAFA!M28*$M$35</f>
         <v>6.4637842351524498E-3</v>
       </c>
-      <c r="K161" s="26" t="str">
+      <c r="K162" s="26" t="str">
         <f>RSDAFA!C28</f>
         <v>R-WH_Att_ELC_N1</v>
       </c>
     </row>
-    <row r="162" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C162" t="s">
-        <v>208</v>
-      </c>
-      <c r="D162" t="s">
-        <v>110</v>
-      </c>
-      <c r="H162" s="26">
-        <f>RSDAFA!L29*$M$34</f>
+    <row r="163" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C163" t="s">
+        <v>208</v>
+      </c>
+      <c r="D163" t="s">
+        <v>110</v>
+      </c>
+      <c r="H163" s="26">
+        <f>RSDAFA!L29*$M$35</f>
         <v>1.72048031425758E-2</v>
       </c>
-      <c r="I162" s="26">
-        <f>RSDAFA!M29*$M$34</f>
+      <c r="I163" s="26">
+        <f>RSDAFA!M29*$M$35</f>
         <v>1.72048031425758E-2</v>
       </c>
-      <c r="K162" s="26" t="str">
+      <c r="K163" s="26" t="str">
         <f>RSDAFA!C29</f>
         <v>R-WH_Att_SOL_N1</v>
       </c>
     </row>
-    <row r="163" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C163" t="s">
-        <v>208</v>
-      </c>
-      <c r="D163" t="s">
-        <v>110</v>
-      </c>
-      <c r="H163" s="26">
-        <f>RSDAFA!L30*$M$34</f>
+    <row r="164" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C164" t="s">
+        <v>208</v>
+      </c>
+      <c r="D164" t="s">
+        <v>110</v>
+      </c>
+      <c r="H164" s="26">
+        <f>RSDAFA!L30*$M$35</f>
         <v>6.6642433815351501E-3</v>
       </c>
-      <c r="I163" s="26">
-        <f>RSDAFA!M30*$M$34</f>
+      <c r="I164" s="26">
+        <f>RSDAFA!M30*$M$35</f>
         <v>6.6642433815351501E-3</v>
       </c>
-      <c r="K163" s="26" t="str">
+      <c r="K164" s="26" t="str">
         <f>RSDAFA!C30</f>
         <v>R-WH_Det_ELC_N1</v>
       </c>
     </row>
-    <row r="164" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C164" t="s">
-        <v>208</v>
-      </c>
-      <c r="D164" t="s">
-        <v>110</v>
-      </c>
-      <c r="H164" s="26">
-        <f>RSDAFA!L31*$M$34</f>
+    <row r="165" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C165" t="s">
+        <v>208</v>
+      </c>
+      <c r="D165" t="s">
+        <v>110</v>
+      </c>
+      <c r="H165" s="26">
+        <f>RSDAFA!L31*$M$35</f>
         <v>5.6525755788417502E-2</v>
       </c>
-      <c r="I164" s="26">
-        <f>RSDAFA!M31*$M$34</f>
+      <c r="I165" s="26">
+        <f>RSDAFA!M31*$M$35</f>
         <v>5.6525755788417502E-2</v>
       </c>
-      <c r="K164" s="26" t="str">
+      <c r="K165" s="26" t="str">
         <f>RSDAFA!C31</f>
         <v>R-WH_Det_SOL_N1</v>
       </c>
-    </row>
-    <row r="165" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="H165" s="26"/>
-      <c r="I165" s="26"/>
-      <c r="K165" s="26"/>
     </row>
     <row r="166" spans="3:11" x14ac:dyDescent="0.25">
       <c r="H166" s="26"/>
@@ -6458,6 +6755,11 @@
       <c r="H182" s="26"/>
       <c r="I182" s="26"/>
       <c r="K182" s="26"/>
+    </row>
+    <row r="183" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H183" s="26"/>
+      <c r="I183" s="26"/>
+      <c r="K183" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -6469,7 +6771,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB6377ED-B160-4F16-923E-B56DAAEBF3A1}">
   <dimension ref="B3:I9"/>
   <sheetViews>
@@ -6597,7 +6899,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2A6683C-C57D-4A33-B9D9-D05BA0CBEA1C}">
   <dimension ref="A1:M93"/>
   <sheetViews>
@@ -10431,7 +10733,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D772440E-5AFD-47E0-A6C0-EF255248451F}">
   <dimension ref="A1:M31"/>
   <sheetViews>

</xml_diff>

<commit_message>
Reduce AFA of new PC by 5*
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_Temporary_Fixes.xlsx
+++ b/SuppXLS/Scen_B_Temporary_Fixes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HannahD\Documents\GitHub\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FEF21E0-C74D-4E7E-89B4-409302323446}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05464919-69B6-4589-B434-8CC3AF30EF45}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4575" yWindow="16050" windowWidth="19650" windowHeight="11070" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="15" r:id="rId1"/>
@@ -19,9 +19,10 @@
     <sheet name="SUP_biogas" sheetId="1" r:id="rId4"/>
     <sheet name="SRV" sheetId="26" r:id="rId5"/>
     <sheet name="RSD" sheetId="22" r:id="rId6"/>
-    <sheet name="DataFill" sheetId="23" r:id="rId7"/>
-    <sheet name="RSDAFC" sheetId="25" r:id="rId8"/>
-    <sheet name="RSDAFA" sheetId="24" r:id="rId9"/>
+    <sheet name="TRA" sheetId="27" r:id="rId7"/>
+    <sheet name="DataFill" sheetId="23" r:id="rId8"/>
+    <sheet name="RSDAFC" sheetId="25" r:id="rId9"/>
+    <sheet name="RSDAFA" sheetId="24" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="__123Graph_AEUMILKPN" hidden="1">#REF!</definedName>
@@ -114,6 +115,29 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Gary Goldstein</author>
+  </authors>
+  <commentList>
+    <comment ref="I3" authorId="0" shapeId="0" xr:uid="{A471135C-592B-4866-91BC-4736F16982C7}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Define the qualifiers based upon technology set + topology + name + descriptions, according to both include and exclude specifications.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
 <metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
@@ -137,7 +161,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1807" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1820" uniqueCount="250">
   <si>
     <t>UC_N</t>
   </si>
@@ -898,6 +922,15 @@
   </si>
   <si>
     <t>FT-RSDPEA</t>
+  </si>
+  <si>
+    <t>AFA</t>
+  </si>
+  <si>
+    <t>*0.95</t>
+  </si>
+  <si>
+    <t>T-CAR*1</t>
   </si>
 </sst>
 </file>
@@ -2521,6 +2554,1296 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D772440E-5AFD-47E0-A6C0-EF255248451F}">
+  <dimension ref="A1:M31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I1" t="s">
+        <v>121</v>
+      </c>
+      <c r="J1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K1" t="s">
+        <v>123</v>
+      </c>
+      <c r="L1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F2" t="s">
+        <v>126</v>
+      </c>
+      <c r="G2">
+        <v>2018</v>
+      </c>
+      <c r="H2" t="s">
+        <v>126</v>
+      </c>
+      <c r="I2" t="s">
+        <v>126</v>
+      </c>
+      <c r="J2" t="s">
+        <v>126</v>
+      </c>
+      <c r="K2" t="s">
+        <v>126</v>
+      </c>
+      <c r="L2">
+        <v>1.91859640129881E-2</v>
+      </c>
+      <c r="M2">
+        <v>1.91859640129881E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F3" t="s">
+        <v>126</v>
+      </c>
+      <c r="G3">
+        <v>2018</v>
+      </c>
+      <c r="H3" t="s">
+        <v>126</v>
+      </c>
+      <c r="I3" t="s">
+        <v>126</v>
+      </c>
+      <c r="J3" t="s">
+        <v>126</v>
+      </c>
+      <c r="K3" t="s">
+        <v>126</v>
+      </c>
+      <c r="L3">
+        <v>1.91859640129881E-2</v>
+      </c>
+      <c r="M3">
+        <v>1.91859640129881E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D4" t="s">
+        <v>126</v>
+      </c>
+      <c r="E4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F4" t="s">
+        <v>126</v>
+      </c>
+      <c r="G4">
+        <v>2018</v>
+      </c>
+      <c r="H4" t="s">
+        <v>126</v>
+      </c>
+      <c r="I4" t="s">
+        <v>126</v>
+      </c>
+      <c r="J4" t="s">
+        <v>126</v>
+      </c>
+      <c r="K4" t="s">
+        <v>126</v>
+      </c>
+      <c r="L4">
+        <v>1.91859640129881E-2</v>
+      </c>
+      <c r="M4">
+        <v>1.91859640129881E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C5" t="s">
+        <v>129</v>
+      </c>
+      <c r="D5" t="s">
+        <v>126</v>
+      </c>
+      <c r="E5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F5" t="s">
+        <v>126</v>
+      </c>
+      <c r="G5">
+        <v>2018</v>
+      </c>
+      <c r="H5" t="s">
+        <v>126</v>
+      </c>
+      <c r="I5" t="s">
+        <v>126</v>
+      </c>
+      <c r="J5" t="s">
+        <v>126</v>
+      </c>
+      <c r="K5" t="s">
+        <v>126</v>
+      </c>
+      <c r="L5">
+        <v>1.91859640129881E-2</v>
+      </c>
+      <c r="M5">
+        <v>1.91859640129881E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B6" t="s">
+        <v>110</v>
+      </c>
+      <c r="C6" t="s">
+        <v>130</v>
+      </c>
+      <c r="D6" t="s">
+        <v>126</v>
+      </c>
+      <c r="E6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F6" t="s">
+        <v>126</v>
+      </c>
+      <c r="G6">
+        <v>2018</v>
+      </c>
+      <c r="H6" t="s">
+        <v>126</v>
+      </c>
+      <c r="I6" t="s">
+        <v>126</v>
+      </c>
+      <c r="J6" t="s">
+        <v>126</v>
+      </c>
+      <c r="K6" t="s">
+        <v>126</v>
+      </c>
+      <c r="L6">
+        <v>1.18590868367296E-2</v>
+      </c>
+      <c r="M6">
+        <v>1.18590868367296E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>124</v>
+      </c>
+      <c r="B7" t="s">
+        <v>110</v>
+      </c>
+      <c r="C7" t="s">
+        <v>131</v>
+      </c>
+      <c r="D7" t="s">
+        <v>126</v>
+      </c>
+      <c r="E7" t="s">
+        <v>83</v>
+      </c>
+      <c r="F7" t="s">
+        <v>126</v>
+      </c>
+      <c r="G7">
+        <v>2018</v>
+      </c>
+      <c r="H7" t="s">
+        <v>126</v>
+      </c>
+      <c r="I7" t="s">
+        <v>126</v>
+      </c>
+      <c r="J7" t="s">
+        <v>126</v>
+      </c>
+      <c r="K7" t="s">
+        <v>126</v>
+      </c>
+      <c r="L7">
+        <v>3.7359826231663999E-2</v>
+      </c>
+      <c r="M7">
+        <v>3.7359826231663999E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B8" t="s">
+        <v>110</v>
+      </c>
+      <c r="C8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D8" t="s">
+        <v>126</v>
+      </c>
+      <c r="E8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F8" t="s">
+        <v>126</v>
+      </c>
+      <c r="G8">
+        <v>2018</v>
+      </c>
+      <c r="H8" t="s">
+        <v>126</v>
+      </c>
+      <c r="I8" t="s">
+        <v>126</v>
+      </c>
+      <c r="J8" t="s">
+        <v>126</v>
+      </c>
+      <c r="K8" t="s">
+        <v>126</v>
+      </c>
+      <c r="L8">
+        <v>2.3078593190679501E-2</v>
+      </c>
+      <c r="M8">
+        <v>2.3078593190679501E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>124</v>
+      </c>
+      <c r="B9" t="s">
+        <v>110</v>
+      </c>
+      <c r="C9" t="s">
+        <v>133</v>
+      </c>
+      <c r="D9" t="s">
+        <v>126</v>
+      </c>
+      <c r="E9" t="s">
+        <v>83</v>
+      </c>
+      <c r="F9" t="s">
+        <v>126</v>
+      </c>
+      <c r="G9">
+        <v>2018</v>
+      </c>
+      <c r="H9" t="s">
+        <v>126</v>
+      </c>
+      <c r="I9" t="s">
+        <v>126</v>
+      </c>
+      <c r="J9" t="s">
+        <v>126</v>
+      </c>
+      <c r="K9" t="s">
+        <v>126</v>
+      </c>
+      <c r="L9">
+        <v>1.7647904805808901E-2</v>
+      </c>
+      <c r="M9">
+        <v>1.7647904805808901E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>124</v>
+      </c>
+      <c r="B10" t="s">
+        <v>110</v>
+      </c>
+      <c r="C10" t="s">
+        <v>134</v>
+      </c>
+      <c r="D10" t="s">
+        <v>126</v>
+      </c>
+      <c r="E10" t="s">
+        <v>83</v>
+      </c>
+      <c r="F10" t="s">
+        <v>126</v>
+      </c>
+      <c r="G10">
+        <v>2018</v>
+      </c>
+      <c r="H10" t="s">
+        <v>126</v>
+      </c>
+      <c r="I10" t="s">
+        <v>126</v>
+      </c>
+      <c r="J10" t="s">
+        <v>126</v>
+      </c>
+      <c r="K10" t="s">
+        <v>126</v>
+      </c>
+      <c r="L10">
+        <v>2.4653262579847901E-2</v>
+      </c>
+      <c r="M10">
+        <v>2.4653262579847901E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C11" t="s">
+        <v>135</v>
+      </c>
+      <c r="D11" t="s">
+        <v>126</v>
+      </c>
+      <c r="E11" t="s">
+        <v>83</v>
+      </c>
+      <c r="F11" t="s">
+        <v>126</v>
+      </c>
+      <c r="G11">
+        <v>2018</v>
+      </c>
+      <c r="H11" t="s">
+        <v>126</v>
+      </c>
+      <c r="I11" t="s">
+        <v>126</v>
+      </c>
+      <c r="J11" t="s">
+        <v>126</v>
+      </c>
+      <c r="K11" t="s">
+        <v>126</v>
+      </c>
+      <c r="L11">
+        <v>2.4653262579847901E-2</v>
+      </c>
+      <c r="M11">
+        <v>2.4653262579847901E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>124</v>
+      </c>
+      <c r="B12" t="s">
+        <v>110</v>
+      </c>
+      <c r="C12" t="s">
+        <v>136</v>
+      </c>
+      <c r="D12" t="s">
+        <v>126</v>
+      </c>
+      <c r="E12" t="s">
+        <v>83</v>
+      </c>
+      <c r="F12" t="s">
+        <v>126</v>
+      </c>
+      <c r="G12">
+        <v>2018</v>
+      </c>
+      <c r="H12" t="s">
+        <v>126</v>
+      </c>
+      <c r="I12" t="s">
+        <v>126</v>
+      </c>
+      <c r="J12" t="s">
+        <v>126</v>
+      </c>
+      <c r="K12" t="s">
+        <v>126</v>
+      </c>
+      <c r="L12">
+        <v>2.4653262579847901E-2</v>
+      </c>
+      <c r="M12">
+        <v>2.4653262579847901E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B13" t="s">
+        <v>110</v>
+      </c>
+      <c r="C13" t="s">
+        <v>137</v>
+      </c>
+      <c r="D13" t="s">
+        <v>126</v>
+      </c>
+      <c r="E13" t="s">
+        <v>83</v>
+      </c>
+      <c r="F13" t="s">
+        <v>126</v>
+      </c>
+      <c r="G13">
+        <v>2018</v>
+      </c>
+      <c r="H13" t="s">
+        <v>126</v>
+      </c>
+      <c r="I13" t="s">
+        <v>126</v>
+      </c>
+      <c r="J13" t="s">
+        <v>126</v>
+      </c>
+      <c r="K13" t="s">
+        <v>126</v>
+      </c>
+      <c r="L13">
+        <v>2.4653262579847901E-2</v>
+      </c>
+      <c r="M13">
+        <v>2.4653262579847901E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>124</v>
+      </c>
+      <c r="B14" t="s">
+        <v>110</v>
+      </c>
+      <c r="C14" t="s">
+        <v>138</v>
+      </c>
+      <c r="D14" t="s">
+        <v>126</v>
+      </c>
+      <c r="E14" t="s">
+        <v>83</v>
+      </c>
+      <c r="F14" t="s">
+        <v>126</v>
+      </c>
+      <c r="G14">
+        <v>2018</v>
+      </c>
+      <c r="H14" t="s">
+        <v>126</v>
+      </c>
+      <c r="I14" t="s">
+        <v>126</v>
+      </c>
+      <c r="J14" t="s">
+        <v>126</v>
+      </c>
+      <c r="K14" t="s">
+        <v>126</v>
+      </c>
+      <c r="L14">
+        <v>2.2095891324020799E-2</v>
+      </c>
+      <c r="M14">
+        <v>2.2095891324020799E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>124</v>
+      </c>
+      <c r="B15" t="s">
+        <v>110</v>
+      </c>
+      <c r="C15" t="s">
+        <v>139</v>
+      </c>
+      <c r="D15" t="s">
+        <v>126</v>
+      </c>
+      <c r="E15" t="s">
+        <v>83</v>
+      </c>
+      <c r="F15" t="s">
+        <v>126</v>
+      </c>
+      <c r="G15">
+        <v>2018</v>
+      </c>
+      <c r="H15" t="s">
+        <v>126</v>
+      </c>
+      <c r="I15" t="s">
+        <v>126</v>
+      </c>
+      <c r="J15" t="s">
+        <v>126</v>
+      </c>
+      <c r="K15" t="s">
+        <v>126</v>
+      </c>
+      <c r="L15">
+        <v>2.8368761423682901E-2</v>
+      </c>
+      <c r="M15">
+        <v>2.8368761423682901E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>124</v>
+      </c>
+      <c r="B16" t="s">
+        <v>110</v>
+      </c>
+      <c r="C16" t="s">
+        <v>140</v>
+      </c>
+      <c r="D16" t="s">
+        <v>126</v>
+      </c>
+      <c r="E16" t="s">
+        <v>83</v>
+      </c>
+      <c r="F16" t="s">
+        <v>126</v>
+      </c>
+      <c r="G16">
+        <v>2018</v>
+      </c>
+      <c r="H16" t="s">
+        <v>126</v>
+      </c>
+      <c r="I16" t="s">
+        <v>126</v>
+      </c>
+      <c r="J16" t="s">
+        <v>126</v>
+      </c>
+      <c r="K16" t="s">
+        <v>126</v>
+      </c>
+      <c r="L16">
+        <v>3.0936872888717201E-2</v>
+      </c>
+      <c r="M16">
+        <v>3.0936872888717201E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>124</v>
+      </c>
+      <c r="B17" t="s">
+        <v>110</v>
+      </c>
+      <c r="C17" t="s">
+        <v>141</v>
+      </c>
+      <c r="D17" t="s">
+        <v>126</v>
+      </c>
+      <c r="E17" t="s">
+        <v>83</v>
+      </c>
+      <c r="F17" t="s">
+        <v>126</v>
+      </c>
+      <c r="G17">
+        <v>2018</v>
+      </c>
+      <c r="H17" t="s">
+        <v>126</v>
+      </c>
+      <c r="I17" t="s">
+        <v>126</v>
+      </c>
+      <c r="J17" t="s">
+        <v>126</v>
+      </c>
+      <c r="K17" t="s">
+        <v>126</v>
+      </c>
+      <c r="L17">
+        <v>7.5066866433008306E-2</v>
+      </c>
+      <c r="M17">
+        <v>7.5066866433008306E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>124</v>
+      </c>
+      <c r="B18" t="s">
+        <v>110</v>
+      </c>
+      <c r="C18" t="s">
+        <v>142</v>
+      </c>
+      <c r="D18" t="s">
+        <v>126</v>
+      </c>
+      <c r="E18" t="s">
+        <v>83</v>
+      </c>
+      <c r="F18" t="s">
+        <v>126</v>
+      </c>
+      <c r="G18">
+        <v>2018</v>
+      </c>
+      <c r="H18" t="s">
+        <v>126</v>
+      </c>
+      <c r="I18" t="s">
+        <v>126</v>
+      </c>
+      <c r="J18" t="s">
+        <v>126</v>
+      </c>
+      <c r="K18" t="s">
+        <v>126</v>
+      </c>
+      <c r="L18">
+        <v>4.1614408271926799E-2</v>
+      </c>
+      <c r="M18">
+        <v>4.1614408271926799E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>124</v>
+      </c>
+      <c r="B19" t="s">
+        <v>110</v>
+      </c>
+      <c r="C19" t="s">
+        <v>143</v>
+      </c>
+      <c r="D19" t="s">
+        <v>126</v>
+      </c>
+      <c r="E19" t="s">
+        <v>83</v>
+      </c>
+      <c r="F19" t="s">
+        <v>126</v>
+      </c>
+      <c r="G19">
+        <v>2018</v>
+      </c>
+      <c r="H19" t="s">
+        <v>126</v>
+      </c>
+      <c r="I19" t="s">
+        <v>126</v>
+      </c>
+      <c r="J19" t="s">
+        <v>126</v>
+      </c>
+      <c r="K19" t="s">
+        <v>126</v>
+      </c>
+      <c r="L19">
+        <v>4.1614408271926799E-2</v>
+      </c>
+      <c r="M19">
+        <v>4.1614408271926799E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>124</v>
+      </c>
+      <c r="B20" t="s">
+        <v>110</v>
+      </c>
+      <c r="C20" t="s">
+        <v>144</v>
+      </c>
+      <c r="D20" t="s">
+        <v>126</v>
+      </c>
+      <c r="E20" t="s">
+        <v>83</v>
+      </c>
+      <c r="F20" t="s">
+        <v>126</v>
+      </c>
+      <c r="G20">
+        <v>2018</v>
+      </c>
+      <c r="H20" t="s">
+        <v>126</v>
+      </c>
+      <c r="I20" t="s">
+        <v>126</v>
+      </c>
+      <c r="J20" t="s">
+        <v>126</v>
+      </c>
+      <c r="K20" t="s">
+        <v>126</v>
+      </c>
+      <c r="L20">
+        <v>4.1614408271926799E-2</v>
+      </c>
+      <c r="M20">
+        <v>4.1614408271926799E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>124</v>
+      </c>
+      <c r="B21" t="s">
+        <v>110</v>
+      </c>
+      <c r="C21" t="s">
+        <v>145</v>
+      </c>
+      <c r="D21" t="s">
+        <v>126</v>
+      </c>
+      <c r="E21" t="s">
+        <v>83</v>
+      </c>
+      <c r="F21" t="s">
+        <v>126</v>
+      </c>
+      <c r="G21">
+        <v>2018</v>
+      </c>
+      <c r="H21" t="s">
+        <v>126</v>
+      </c>
+      <c r="I21" t="s">
+        <v>126</v>
+      </c>
+      <c r="J21" t="s">
+        <v>126</v>
+      </c>
+      <c r="K21" t="s">
+        <v>126</v>
+      </c>
+      <c r="L21">
+        <v>4.1614408271926799E-2</v>
+      </c>
+      <c r="M21">
+        <v>4.1614408271926799E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>124</v>
+      </c>
+      <c r="B22" t="s">
+        <v>110</v>
+      </c>
+      <c r="C22" t="s">
+        <v>146</v>
+      </c>
+      <c r="D22" t="s">
+        <v>126</v>
+      </c>
+      <c r="E22" t="s">
+        <v>83</v>
+      </c>
+      <c r="F22" t="s">
+        <v>126</v>
+      </c>
+      <c r="G22">
+        <v>2018</v>
+      </c>
+      <c r="H22" t="s">
+        <v>126</v>
+      </c>
+      <c r="I22" t="s">
+        <v>126</v>
+      </c>
+      <c r="J22" t="s">
+        <v>126</v>
+      </c>
+      <c r="K22" t="s">
+        <v>126</v>
+      </c>
+      <c r="L22">
+        <v>3.7040631160092499E-2</v>
+      </c>
+      <c r="M22">
+        <v>3.7040631160092499E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>124</v>
+      </c>
+      <c r="B23" t="s">
+        <v>110</v>
+      </c>
+      <c r="C23" t="s">
+        <v>147</v>
+      </c>
+      <c r="D23" t="s">
+        <v>126</v>
+      </c>
+      <c r="E23" t="s">
+        <v>83</v>
+      </c>
+      <c r="F23" t="s">
+        <v>126</v>
+      </c>
+      <c r="G23">
+        <v>2018</v>
+      </c>
+      <c r="H23" t="s">
+        <v>126</v>
+      </c>
+      <c r="I23" t="s">
+        <v>126</v>
+      </c>
+      <c r="J23" t="s">
+        <v>126</v>
+      </c>
+      <c r="K23" t="s">
+        <v>126</v>
+      </c>
+      <c r="L23">
+        <v>4.6621727976421598E-2</v>
+      </c>
+      <c r="M23">
+        <v>4.6621727976421598E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>124</v>
+      </c>
+      <c r="B24" t="s">
+        <v>110</v>
+      </c>
+      <c r="C24" t="s">
+        <v>148</v>
+      </c>
+      <c r="D24" t="s">
+        <v>126</v>
+      </c>
+      <c r="E24" t="s">
+        <v>83</v>
+      </c>
+      <c r="F24" t="s">
+        <v>126</v>
+      </c>
+      <c r="G24">
+        <v>2018</v>
+      </c>
+      <c r="H24" t="s">
+        <v>126</v>
+      </c>
+      <c r="I24" t="s">
+        <v>126</v>
+      </c>
+      <c r="J24" t="s">
+        <v>126</v>
+      </c>
+      <c r="K24" t="s">
+        <v>126</v>
+      </c>
+      <c r="L24">
+        <v>6.7033675870053502E-2</v>
+      </c>
+      <c r="M24">
+        <v>6.7033675870053502E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>124</v>
+      </c>
+      <c r="B25" t="s">
+        <v>110</v>
+      </c>
+      <c r="C25" t="s">
+        <v>149</v>
+      </c>
+      <c r="D25" t="s">
+        <v>126</v>
+      </c>
+      <c r="E25" t="s">
+        <v>83</v>
+      </c>
+      <c r="F25" t="s">
+        <v>126</v>
+      </c>
+      <c r="G25">
+        <v>2018</v>
+      </c>
+      <c r="H25" t="s">
+        <v>126</v>
+      </c>
+      <c r="I25" t="s">
+        <v>126</v>
+      </c>
+      <c r="J25" t="s">
+        <v>126</v>
+      </c>
+      <c r="K25" t="s">
+        <v>126</v>
+      </c>
+      <c r="L25">
+        <v>9.1153830584100495E-2</v>
+      </c>
+      <c r="M25">
+        <v>9.1153830584100495E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>124</v>
+      </c>
+      <c r="B26" t="s">
+        <v>110</v>
+      </c>
+      <c r="C26" t="s">
+        <v>150</v>
+      </c>
+      <c r="D26" t="s">
+        <v>126</v>
+      </c>
+      <c r="E26" t="s">
+        <v>83</v>
+      </c>
+      <c r="F26" t="s">
+        <v>126</v>
+      </c>
+      <c r="G26">
+        <v>2018</v>
+      </c>
+      <c r="H26" t="s">
+        <v>126</v>
+      </c>
+      <c r="I26" t="s">
+        <v>126</v>
+      </c>
+      <c r="J26" t="s">
+        <v>126</v>
+      </c>
+      <c r="K26" t="s">
+        <v>126</v>
+      </c>
+      <c r="L26">
+        <v>2.2735699655164601E-2</v>
+      </c>
+      <c r="M26">
+        <v>2.2735699655164601E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>124</v>
+      </c>
+      <c r="B27" t="s">
+        <v>110</v>
+      </c>
+      <c r="C27" t="s">
+        <v>151</v>
+      </c>
+      <c r="D27" t="s">
+        <v>126</v>
+      </c>
+      <c r="E27" t="s">
+        <v>83</v>
+      </c>
+      <c r="F27" t="s">
+        <v>126</v>
+      </c>
+      <c r="G27">
+        <v>2018</v>
+      </c>
+      <c r="H27" t="s">
+        <v>126</v>
+      </c>
+      <c r="I27" t="s">
+        <v>126</v>
+      </c>
+      <c r="J27" t="s">
+        <v>126</v>
+      </c>
+      <c r="K27" t="s">
+        <v>126</v>
+      </c>
+      <c r="L27">
+        <v>8.6298729994523198E-3</v>
+      </c>
+      <c r="M27">
+        <v>8.6298729994523198E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>124</v>
+      </c>
+      <c r="B28" t="s">
+        <v>110</v>
+      </c>
+      <c r="C28" t="s">
+        <v>152</v>
+      </c>
+      <c r="D28" t="s">
+        <v>126</v>
+      </c>
+      <c r="E28" t="s">
+        <v>83</v>
+      </c>
+      <c r="F28" t="s">
+        <v>126</v>
+      </c>
+      <c r="G28">
+        <v>2018</v>
+      </c>
+      <c r="H28" t="s">
+        <v>126</v>
+      </c>
+      <c r="I28" t="s">
+        <v>126</v>
+      </c>
+      <c r="J28" t="s">
+        <v>126</v>
+      </c>
+      <c r="K28" t="s">
+        <v>126</v>
+      </c>
+      <c r="L28">
+        <v>1.29275684703049E-2</v>
+      </c>
+      <c r="M28">
+        <v>1.29275684703049E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>124</v>
+      </c>
+      <c r="B29" t="s">
+        <v>110</v>
+      </c>
+      <c r="C29" t="s">
+        <v>153</v>
+      </c>
+      <c r="D29" t="s">
+        <v>126</v>
+      </c>
+      <c r="E29" t="s">
+        <v>83</v>
+      </c>
+      <c r="F29" t="s">
+        <v>126</v>
+      </c>
+      <c r="G29">
+        <v>2018</v>
+      </c>
+      <c r="H29" t="s">
+        <v>126</v>
+      </c>
+      <c r="I29" t="s">
+        <v>126</v>
+      </c>
+      <c r="J29" t="s">
+        <v>126</v>
+      </c>
+      <c r="K29" t="s">
+        <v>126</v>
+      </c>
+      <c r="L29">
+        <v>3.4409606285151599E-2</v>
+      </c>
+      <c r="M29">
+        <v>3.4409606285151599E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>124</v>
+      </c>
+      <c r="B30" t="s">
+        <v>110</v>
+      </c>
+      <c r="C30" t="s">
+        <v>154</v>
+      </c>
+      <c r="D30" t="s">
+        <v>126</v>
+      </c>
+      <c r="E30" t="s">
+        <v>83</v>
+      </c>
+      <c r="F30" t="s">
+        <v>126</v>
+      </c>
+      <c r="G30">
+        <v>2018</v>
+      </c>
+      <c r="H30" t="s">
+        <v>126</v>
+      </c>
+      <c r="I30" t="s">
+        <v>126</v>
+      </c>
+      <c r="J30" t="s">
+        <v>126</v>
+      </c>
+      <c r="K30" t="s">
+        <v>126</v>
+      </c>
+      <c r="L30">
+        <v>1.33284867630703E-2</v>
+      </c>
+      <c r="M30">
+        <v>1.33284867630703E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>124</v>
+      </c>
+      <c r="B31" t="s">
+        <v>110</v>
+      </c>
+      <c r="C31" t="s">
+        <v>155</v>
+      </c>
+      <c r="D31" t="s">
+        <v>126</v>
+      </c>
+      <c r="E31" t="s">
+        <v>83</v>
+      </c>
+      <c r="F31" t="s">
+        <v>126</v>
+      </c>
+      <c r="G31">
+        <v>2018</v>
+      </c>
+      <c r="H31" t="s">
+        <v>126</v>
+      </c>
+      <c r="I31" t="s">
+        <v>126</v>
+      </c>
+      <c r="J31" t="s">
+        <v>126</v>
+      </c>
+      <c r="K31" t="s">
+        <v>126</v>
+      </c>
+      <c r="L31">
+        <v>0.113051511576835</v>
+      </c>
+      <c r="M31">
+        <v>0.113051511576835</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE79BAD-EA44-47F0-A194-320DE6C9FB50}">
   <dimension ref="B2:M15"/>
@@ -3375,8 +4698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{209CF89D-3AC9-4E2E-BCF6-79A710F8BD8A}">
   <dimension ref="A1:S183"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L44" sqref="L44"/>
+    <sheetView topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23:K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6772,6 +8095,82 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8FB1178-AF9A-473D-9FB3-41C2F896D89C}">
+  <dimension ref="B3:K5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="8"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+    </row>
+    <row r="4" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="11" t="str">
+        <f>IF(Regions!C$3&lt;&gt;"",Regions!C$3,"*")</f>
+        <v>IE</v>
+      </c>
+      <c r="I4" s="11" t="str">
+        <f>IF(Regions!D$3&lt;&gt;"",Regions!D$3,"*")</f>
+        <v>National</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>247</v>
+      </c>
+      <c r="H5" t="s">
+        <v>248</v>
+      </c>
+      <c r="I5" t="s">
+        <v>248</v>
+      </c>
+      <c r="K5" t="s">
+        <v>249</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB6377ED-B160-4F16-923E-B56DAAEBF3A1}">
   <dimension ref="B3:I9"/>
   <sheetViews>
@@ -6899,7 +8298,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2A6683C-C57D-4A33-B9D9-D05BA0CBEA1C}">
   <dimension ref="A1:M93"/>
   <sheetViews>
@@ -10731,1294 +12130,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D772440E-5AFD-47E0-A6C0-EF255248451F}">
-  <dimension ref="A1:M31"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D1" t="s">
-        <v>116</v>
-      </c>
-      <c r="E1" t="s">
-        <v>117</v>
-      </c>
-      <c r="F1" t="s">
-        <v>118</v>
-      </c>
-      <c r="G1" t="s">
-        <v>119</v>
-      </c>
-      <c r="H1" t="s">
-        <v>120</v>
-      </c>
-      <c r="I1" t="s">
-        <v>121</v>
-      </c>
-      <c r="J1" t="s">
-        <v>122</v>
-      </c>
-      <c r="K1" t="s">
-        <v>123</v>
-      </c>
-      <c r="L1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E2" t="s">
-        <v>83</v>
-      </c>
-      <c r="F2" t="s">
-        <v>126</v>
-      </c>
-      <c r="G2">
-        <v>2018</v>
-      </c>
-      <c r="H2" t="s">
-        <v>126</v>
-      </c>
-      <c r="I2" t="s">
-        <v>126</v>
-      </c>
-      <c r="J2" t="s">
-        <v>126</v>
-      </c>
-      <c r="K2" t="s">
-        <v>126</v>
-      </c>
-      <c r="L2">
-        <v>1.91859640129881E-2</v>
-      </c>
-      <c r="M2">
-        <v>1.91859640129881E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>124</v>
-      </c>
-      <c r="B3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C3" t="s">
-        <v>127</v>
-      </c>
-      <c r="D3" t="s">
-        <v>126</v>
-      </c>
-      <c r="E3" t="s">
-        <v>83</v>
-      </c>
-      <c r="F3" t="s">
-        <v>126</v>
-      </c>
-      <c r="G3">
-        <v>2018</v>
-      </c>
-      <c r="H3" t="s">
-        <v>126</v>
-      </c>
-      <c r="I3" t="s">
-        <v>126</v>
-      </c>
-      <c r="J3" t="s">
-        <v>126</v>
-      </c>
-      <c r="K3" t="s">
-        <v>126</v>
-      </c>
-      <c r="L3">
-        <v>1.91859640129881E-2</v>
-      </c>
-      <c r="M3">
-        <v>1.91859640129881E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>124</v>
-      </c>
-      <c r="B4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C4" t="s">
-        <v>128</v>
-      </c>
-      <c r="D4" t="s">
-        <v>126</v>
-      </c>
-      <c r="E4" t="s">
-        <v>83</v>
-      </c>
-      <c r="F4" t="s">
-        <v>126</v>
-      </c>
-      <c r="G4">
-        <v>2018</v>
-      </c>
-      <c r="H4" t="s">
-        <v>126</v>
-      </c>
-      <c r="I4" t="s">
-        <v>126</v>
-      </c>
-      <c r="J4" t="s">
-        <v>126</v>
-      </c>
-      <c r="K4" t="s">
-        <v>126</v>
-      </c>
-      <c r="L4">
-        <v>1.91859640129881E-2</v>
-      </c>
-      <c r="M4">
-        <v>1.91859640129881E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>124</v>
-      </c>
-      <c r="B5" t="s">
-        <v>110</v>
-      </c>
-      <c r="C5" t="s">
-        <v>129</v>
-      </c>
-      <c r="D5" t="s">
-        <v>126</v>
-      </c>
-      <c r="E5" t="s">
-        <v>83</v>
-      </c>
-      <c r="F5" t="s">
-        <v>126</v>
-      </c>
-      <c r="G5">
-        <v>2018</v>
-      </c>
-      <c r="H5" t="s">
-        <v>126</v>
-      </c>
-      <c r="I5" t="s">
-        <v>126</v>
-      </c>
-      <c r="J5" t="s">
-        <v>126</v>
-      </c>
-      <c r="K5" t="s">
-        <v>126</v>
-      </c>
-      <c r="L5">
-        <v>1.91859640129881E-2</v>
-      </c>
-      <c r="M5">
-        <v>1.91859640129881E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>124</v>
-      </c>
-      <c r="B6" t="s">
-        <v>110</v>
-      </c>
-      <c r="C6" t="s">
-        <v>130</v>
-      </c>
-      <c r="D6" t="s">
-        <v>126</v>
-      </c>
-      <c r="E6" t="s">
-        <v>83</v>
-      </c>
-      <c r="F6" t="s">
-        <v>126</v>
-      </c>
-      <c r="G6">
-        <v>2018</v>
-      </c>
-      <c r="H6" t="s">
-        <v>126</v>
-      </c>
-      <c r="I6" t="s">
-        <v>126</v>
-      </c>
-      <c r="J6" t="s">
-        <v>126</v>
-      </c>
-      <c r="K6" t="s">
-        <v>126</v>
-      </c>
-      <c r="L6">
-        <v>1.18590868367296E-2</v>
-      </c>
-      <c r="M6">
-        <v>1.18590868367296E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>124</v>
-      </c>
-      <c r="B7" t="s">
-        <v>110</v>
-      </c>
-      <c r="C7" t="s">
-        <v>131</v>
-      </c>
-      <c r="D7" t="s">
-        <v>126</v>
-      </c>
-      <c r="E7" t="s">
-        <v>83</v>
-      </c>
-      <c r="F7" t="s">
-        <v>126</v>
-      </c>
-      <c r="G7">
-        <v>2018</v>
-      </c>
-      <c r="H7" t="s">
-        <v>126</v>
-      </c>
-      <c r="I7" t="s">
-        <v>126</v>
-      </c>
-      <c r="J7" t="s">
-        <v>126</v>
-      </c>
-      <c r="K7" t="s">
-        <v>126</v>
-      </c>
-      <c r="L7">
-        <v>3.7359826231663999E-2</v>
-      </c>
-      <c r="M7">
-        <v>3.7359826231663999E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>124</v>
-      </c>
-      <c r="B8" t="s">
-        <v>110</v>
-      </c>
-      <c r="C8" t="s">
-        <v>132</v>
-      </c>
-      <c r="D8" t="s">
-        <v>126</v>
-      </c>
-      <c r="E8" t="s">
-        <v>83</v>
-      </c>
-      <c r="F8" t="s">
-        <v>126</v>
-      </c>
-      <c r="G8">
-        <v>2018</v>
-      </c>
-      <c r="H8" t="s">
-        <v>126</v>
-      </c>
-      <c r="I8" t="s">
-        <v>126</v>
-      </c>
-      <c r="J8" t="s">
-        <v>126</v>
-      </c>
-      <c r="K8" t="s">
-        <v>126</v>
-      </c>
-      <c r="L8">
-        <v>2.3078593190679501E-2</v>
-      </c>
-      <c r="M8">
-        <v>2.3078593190679501E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>124</v>
-      </c>
-      <c r="B9" t="s">
-        <v>110</v>
-      </c>
-      <c r="C9" t="s">
-        <v>133</v>
-      </c>
-      <c r="D9" t="s">
-        <v>126</v>
-      </c>
-      <c r="E9" t="s">
-        <v>83</v>
-      </c>
-      <c r="F9" t="s">
-        <v>126</v>
-      </c>
-      <c r="G9">
-        <v>2018</v>
-      </c>
-      <c r="H9" t="s">
-        <v>126</v>
-      </c>
-      <c r="I9" t="s">
-        <v>126</v>
-      </c>
-      <c r="J9" t="s">
-        <v>126</v>
-      </c>
-      <c r="K9" t="s">
-        <v>126</v>
-      </c>
-      <c r="L9">
-        <v>1.7647904805808901E-2</v>
-      </c>
-      <c r="M9">
-        <v>1.7647904805808901E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>124</v>
-      </c>
-      <c r="B10" t="s">
-        <v>110</v>
-      </c>
-      <c r="C10" t="s">
-        <v>134</v>
-      </c>
-      <c r="D10" t="s">
-        <v>126</v>
-      </c>
-      <c r="E10" t="s">
-        <v>83</v>
-      </c>
-      <c r="F10" t="s">
-        <v>126</v>
-      </c>
-      <c r="G10">
-        <v>2018</v>
-      </c>
-      <c r="H10" t="s">
-        <v>126</v>
-      </c>
-      <c r="I10" t="s">
-        <v>126</v>
-      </c>
-      <c r="J10" t="s">
-        <v>126</v>
-      </c>
-      <c r="K10" t="s">
-        <v>126</v>
-      </c>
-      <c r="L10">
-        <v>2.4653262579847901E-2</v>
-      </c>
-      <c r="M10">
-        <v>2.4653262579847901E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>124</v>
-      </c>
-      <c r="B11" t="s">
-        <v>110</v>
-      </c>
-      <c r="C11" t="s">
-        <v>135</v>
-      </c>
-      <c r="D11" t="s">
-        <v>126</v>
-      </c>
-      <c r="E11" t="s">
-        <v>83</v>
-      </c>
-      <c r="F11" t="s">
-        <v>126</v>
-      </c>
-      <c r="G11">
-        <v>2018</v>
-      </c>
-      <c r="H11" t="s">
-        <v>126</v>
-      </c>
-      <c r="I11" t="s">
-        <v>126</v>
-      </c>
-      <c r="J11" t="s">
-        <v>126</v>
-      </c>
-      <c r="K11" t="s">
-        <v>126</v>
-      </c>
-      <c r="L11">
-        <v>2.4653262579847901E-2</v>
-      </c>
-      <c r="M11">
-        <v>2.4653262579847901E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>124</v>
-      </c>
-      <c r="B12" t="s">
-        <v>110</v>
-      </c>
-      <c r="C12" t="s">
-        <v>136</v>
-      </c>
-      <c r="D12" t="s">
-        <v>126</v>
-      </c>
-      <c r="E12" t="s">
-        <v>83</v>
-      </c>
-      <c r="F12" t="s">
-        <v>126</v>
-      </c>
-      <c r="G12">
-        <v>2018</v>
-      </c>
-      <c r="H12" t="s">
-        <v>126</v>
-      </c>
-      <c r="I12" t="s">
-        <v>126</v>
-      </c>
-      <c r="J12" t="s">
-        <v>126</v>
-      </c>
-      <c r="K12" t="s">
-        <v>126</v>
-      </c>
-      <c r="L12">
-        <v>2.4653262579847901E-2</v>
-      </c>
-      <c r="M12">
-        <v>2.4653262579847901E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>124</v>
-      </c>
-      <c r="B13" t="s">
-        <v>110</v>
-      </c>
-      <c r="C13" t="s">
-        <v>137</v>
-      </c>
-      <c r="D13" t="s">
-        <v>126</v>
-      </c>
-      <c r="E13" t="s">
-        <v>83</v>
-      </c>
-      <c r="F13" t="s">
-        <v>126</v>
-      </c>
-      <c r="G13">
-        <v>2018</v>
-      </c>
-      <c r="H13" t="s">
-        <v>126</v>
-      </c>
-      <c r="I13" t="s">
-        <v>126</v>
-      </c>
-      <c r="J13" t="s">
-        <v>126</v>
-      </c>
-      <c r="K13" t="s">
-        <v>126</v>
-      </c>
-      <c r="L13">
-        <v>2.4653262579847901E-2</v>
-      </c>
-      <c r="M13">
-        <v>2.4653262579847901E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>124</v>
-      </c>
-      <c r="B14" t="s">
-        <v>110</v>
-      </c>
-      <c r="C14" t="s">
-        <v>138</v>
-      </c>
-      <c r="D14" t="s">
-        <v>126</v>
-      </c>
-      <c r="E14" t="s">
-        <v>83</v>
-      </c>
-      <c r="F14" t="s">
-        <v>126</v>
-      </c>
-      <c r="G14">
-        <v>2018</v>
-      </c>
-      <c r="H14" t="s">
-        <v>126</v>
-      </c>
-      <c r="I14" t="s">
-        <v>126</v>
-      </c>
-      <c r="J14" t="s">
-        <v>126</v>
-      </c>
-      <c r="K14" t="s">
-        <v>126</v>
-      </c>
-      <c r="L14">
-        <v>2.2095891324020799E-2</v>
-      </c>
-      <c r="M14">
-        <v>2.2095891324020799E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>124</v>
-      </c>
-      <c r="B15" t="s">
-        <v>110</v>
-      </c>
-      <c r="C15" t="s">
-        <v>139</v>
-      </c>
-      <c r="D15" t="s">
-        <v>126</v>
-      </c>
-      <c r="E15" t="s">
-        <v>83</v>
-      </c>
-      <c r="F15" t="s">
-        <v>126</v>
-      </c>
-      <c r="G15">
-        <v>2018</v>
-      </c>
-      <c r="H15" t="s">
-        <v>126</v>
-      </c>
-      <c r="I15" t="s">
-        <v>126</v>
-      </c>
-      <c r="J15" t="s">
-        <v>126</v>
-      </c>
-      <c r="K15" t="s">
-        <v>126</v>
-      </c>
-      <c r="L15">
-        <v>2.8368761423682901E-2</v>
-      </c>
-      <c r="M15">
-        <v>2.8368761423682901E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>124</v>
-      </c>
-      <c r="B16" t="s">
-        <v>110</v>
-      </c>
-      <c r="C16" t="s">
-        <v>140</v>
-      </c>
-      <c r="D16" t="s">
-        <v>126</v>
-      </c>
-      <c r="E16" t="s">
-        <v>83</v>
-      </c>
-      <c r="F16" t="s">
-        <v>126</v>
-      </c>
-      <c r="G16">
-        <v>2018</v>
-      </c>
-      <c r="H16" t="s">
-        <v>126</v>
-      </c>
-      <c r="I16" t="s">
-        <v>126</v>
-      </c>
-      <c r="J16" t="s">
-        <v>126</v>
-      </c>
-      <c r="K16" t="s">
-        <v>126</v>
-      </c>
-      <c r="L16">
-        <v>3.0936872888717201E-2</v>
-      </c>
-      <c r="M16">
-        <v>3.0936872888717201E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>124</v>
-      </c>
-      <c r="B17" t="s">
-        <v>110</v>
-      </c>
-      <c r="C17" t="s">
-        <v>141</v>
-      </c>
-      <c r="D17" t="s">
-        <v>126</v>
-      </c>
-      <c r="E17" t="s">
-        <v>83</v>
-      </c>
-      <c r="F17" t="s">
-        <v>126</v>
-      </c>
-      <c r="G17">
-        <v>2018</v>
-      </c>
-      <c r="H17" t="s">
-        <v>126</v>
-      </c>
-      <c r="I17" t="s">
-        <v>126</v>
-      </c>
-      <c r="J17" t="s">
-        <v>126</v>
-      </c>
-      <c r="K17" t="s">
-        <v>126</v>
-      </c>
-      <c r="L17">
-        <v>7.5066866433008306E-2</v>
-      </c>
-      <c r="M17">
-        <v>7.5066866433008306E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>124</v>
-      </c>
-      <c r="B18" t="s">
-        <v>110</v>
-      </c>
-      <c r="C18" t="s">
-        <v>142</v>
-      </c>
-      <c r="D18" t="s">
-        <v>126</v>
-      </c>
-      <c r="E18" t="s">
-        <v>83</v>
-      </c>
-      <c r="F18" t="s">
-        <v>126</v>
-      </c>
-      <c r="G18">
-        <v>2018</v>
-      </c>
-      <c r="H18" t="s">
-        <v>126</v>
-      </c>
-      <c r="I18" t="s">
-        <v>126</v>
-      </c>
-      <c r="J18" t="s">
-        <v>126</v>
-      </c>
-      <c r="K18" t="s">
-        <v>126</v>
-      </c>
-      <c r="L18">
-        <v>4.1614408271926799E-2</v>
-      </c>
-      <c r="M18">
-        <v>4.1614408271926799E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>124</v>
-      </c>
-      <c r="B19" t="s">
-        <v>110</v>
-      </c>
-      <c r="C19" t="s">
-        <v>143</v>
-      </c>
-      <c r="D19" t="s">
-        <v>126</v>
-      </c>
-      <c r="E19" t="s">
-        <v>83</v>
-      </c>
-      <c r="F19" t="s">
-        <v>126</v>
-      </c>
-      <c r="G19">
-        <v>2018</v>
-      </c>
-      <c r="H19" t="s">
-        <v>126</v>
-      </c>
-      <c r="I19" t="s">
-        <v>126</v>
-      </c>
-      <c r="J19" t="s">
-        <v>126</v>
-      </c>
-      <c r="K19" t="s">
-        <v>126</v>
-      </c>
-      <c r="L19">
-        <v>4.1614408271926799E-2</v>
-      </c>
-      <c r="M19">
-        <v>4.1614408271926799E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>124</v>
-      </c>
-      <c r="B20" t="s">
-        <v>110</v>
-      </c>
-      <c r="C20" t="s">
-        <v>144</v>
-      </c>
-      <c r="D20" t="s">
-        <v>126</v>
-      </c>
-      <c r="E20" t="s">
-        <v>83</v>
-      </c>
-      <c r="F20" t="s">
-        <v>126</v>
-      </c>
-      <c r="G20">
-        <v>2018</v>
-      </c>
-      <c r="H20" t="s">
-        <v>126</v>
-      </c>
-      <c r="I20" t="s">
-        <v>126</v>
-      </c>
-      <c r="J20" t="s">
-        <v>126</v>
-      </c>
-      <c r="K20" t="s">
-        <v>126</v>
-      </c>
-      <c r="L20">
-        <v>4.1614408271926799E-2</v>
-      </c>
-      <c r="M20">
-        <v>4.1614408271926799E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>124</v>
-      </c>
-      <c r="B21" t="s">
-        <v>110</v>
-      </c>
-      <c r="C21" t="s">
-        <v>145</v>
-      </c>
-      <c r="D21" t="s">
-        <v>126</v>
-      </c>
-      <c r="E21" t="s">
-        <v>83</v>
-      </c>
-      <c r="F21" t="s">
-        <v>126</v>
-      </c>
-      <c r="G21">
-        <v>2018</v>
-      </c>
-      <c r="H21" t="s">
-        <v>126</v>
-      </c>
-      <c r="I21" t="s">
-        <v>126</v>
-      </c>
-      <c r="J21" t="s">
-        <v>126</v>
-      </c>
-      <c r="K21" t="s">
-        <v>126</v>
-      </c>
-      <c r="L21">
-        <v>4.1614408271926799E-2</v>
-      </c>
-      <c r="M21">
-        <v>4.1614408271926799E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>124</v>
-      </c>
-      <c r="B22" t="s">
-        <v>110</v>
-      </c>
-      <c r="C22" t="s">
-        <v>146</v>
-      </c>
-      <c r="D22" t="s">
-        <v>126</v>
-      </c>
-      <c r="E22" t="s">
-        <v>83</v>
-      </c>
-      <c r="F22" t="s">
-        <v>126</v>
-      </c>
-      <c r="G22">
-        <v>2018</v>
-      </c>
-      <c r="H22" t="s">
-        <v>126</v>
-      </c>
-      <c r="I22" t="s">
-        <v>126</v>
-      </c>
-      <c r="J22" t="s">
-        <v>126</v>
-      </c>
-      <c r="K22" t="s">
-        <v>126</v>
-      </c>
-      <c r="L22">
-        <v>3.7040631160092499E-2</v>
-      </c>
-      <c r="M22">
-        <v>3.7040631160092499E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>124</v>
-      </c>
-      <c r="B23" t="s">
-        <v>110</v>
-      </c>
-      <c r="C23" t="s">
-        <v>147</v>
-      </c>
-      <c r="D23" t="s">
-        <v>126</v>
-      </c>
-      <c r="E23" t="s">
-        <v>83</v>
-      </c>
-      <c r="F23" t="s">
-        <v>126</v>
-      </c>
-      <c r="G23">
-        <v>2018</v>
-      </c>
-      <c r="H23" t="s">
-        <v>126</v>
-      </c>
-      <c r="I23" t="s">
-        <v>126</v>
-      </c>
-      <c r="J23" t="s">
-        <v>126</v>
-      </c>
-      <c r="K23" t="s">
-        <v>126</v>
-      </c>
-      <c r="L23">
-        <v>4.6621727976421598E-2</v>
-      </c>
-      <c r="M23">
-        <v>4.6621727976421598E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>124</v>
-      </c>
-      <c r="B24" t="s">
-        <v>110</v>
-      </c>
-      <c r="C24" t="s">
-        <v>148</v>
-      </c>
-      <c r="D24" t="s">
-        <v>126</v>
-      </c>
-      <c r="E24" t="s">
-        <v>83</v>
-      </c>
-      <c r="F24" t="s">
-        <v>126</v>
-      </c>
-      <c r="G24">
-        <v>2018</v>
-      </c>
-      <c r="H24" t="s">
-        <v>126</v>
-      </c>
-      <c r="I24" t="s">
-        <v>126</v>
-      </c>
-      <c r="J24" t="s">
-        <v>126</v>
-      </c>
-      <c r="K24" t="s">
-        <v>126</v>
-      </c>
-      <c r="L24">
-        <v>6.7033675870053502E-2</v>
-      </c>
-      <c r="M24">
-        <v>6.7033675870053502E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>124</v>
-      </c>
-      <c r="B25" t="s">
-        <v>110</v>
-      </c>
-      <c r="C25" t="s">
-        <v>149</v>
-      </c>
-      <c r="D25" t="s">
-        <v>126</v>
-      </c>
-      <c r="E25" t="s">
-        <v>83</v>
-      </c>
-      <c r="F25" t="s">
-        <v>126</v>
-      </c>
-      <c r="G25">
-        <v>2018</v>
-      </c>
-      <c r="H25" t="s">
-        <v>126</v>
-      </c>
-      <c r="I25" t="s">
-        <v>126</v>
-      </c>
-      <c r="J25" t="s">
-        <v>126</v>
-      </c>
-      <c r="K25" t="s">
-        <v>126</v>
-      </c>
-      <c r="L25">
-        <v>9.1153830584100495E-2</v>
-      </c>
-      <c r="M25">
-        <v>9.1153830584100495E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>124</v>
-      </c>
-      <c r="B26" t="s">
-        <v>110</v>
-      </c>
-      <c r="C26" t="s">
-        <v>150</v>
-      </c>
-      <c r="D26" t="s">
-        <v>126</v>
-      </c>
-      <c r="E26" t="s">
-        <v>83</v>
-      </c>
-      <c r="F26" t="s">
-        <v>126</v>
-      </c>
-      <c r="G26">
-        <v>2018</v>
-      </c>
-      <c r="H26" t="s">
-        <v>126</v>
-      </c>
-      <c r="I26" t="s">
-        <v>126</v>
-      </c>
-      <c r="J26" t="s">
-        <v>126</v>
-      </c>
-      <c r="K26" t="s">
-        <v>126</v>
-      </c>
-      <c r="L26">
-        <v>2.2735699655164601E-2</v>
-      </c>
-      <c r="M26">
-        <v>2.2735699655164601E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>124</v>
-      </c>
-      <c r="B27" t="s">
-        <v>110</v>
-      </c>
-      <c r="C27" t="s">
-        <v>151</v>
-      </c>
-      <c r="D27" t="s">
-        <v>126</v>
-      </c>
-      <c r="E27" t="s">
-        <v>83</v>
-      </c>
-      <c r="F27" t="s">
-        <v>126</v>
-      </c>
-      <c r="G27">
-        <v>2018</v>
-      </c>
-      <c r="H27" t="s">
-        <v>126</v>
-      </c>
-      <c r="I27" t="s">
-        <v>126</v>
-      </c>
-      <c r="J27" t="s">
-        <v>126</v>
-      </c>
-      <c r="K27" t="s">
-        <v>126</v>
-      </c>
-      <c r="L27">
-        <v>8.6298729994523198E-3</v>
-      </c>
-      <c r="M27">
-        <v>8.6298729994523198E-3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>124</v>
-      </c>
-      <c r="B28" t="s">
-        <v>110</v>
-      </c>
-      <c r="C28" t="s">
-        <v>152</v>
-      </c>
-      <c r="D28" t="s">
-        <v>126</v>
-      </c>
-      <c r="E28" t="s">
-        <v>83</v>
-      </c>
-      <c r="F28" t="s">
-        <v>126</v>
-      </c>
-      <c r="G28">
-        <v>2018</v>
-      </c>
-      <c r="H28" t="s">
-        <v>126</v>
-      </c>
-      <c r="I28" t="s">
-        <v>126</v>
-      </c>
-      <c r="J28" t="s">
-        <v>126</v>
-      </c>
-      <c r="K28" t="s">
-        <v>126</v>
-      </c>
-      <c r="L28">
-        <v>1.29275684703049E-2</v>
-      </c>
-      <c r="M28">
-        <v>1.29275684703049E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>124</v>
-      </c>
-      <c r="B29" t="s">
-        <v>110</v>
-      </c>
-      <c r="C29" t="s">
-        <v>153</v>
-      </c>
-      <c r="D29" t="s">
-        <v>126</v>
-      </c>
-      <c r="E29" t="s">
-        <v>83</v>
-      </c>
-      <c r="F29" t="s">
-        <v>126</v>
-      </c>
-      <c r="G29">
-        <v>2018</v>
-      </c>
-      <c r="H29" t="s">
-        <v>126</v>
-      </c>
-      <c r="I29" t="s">
-        <v>126</v>
-      </c>
-      <c r="J29" t="s">
-        <v>126</v>
-      </c>
-      <c r="K29" t="s">
-        <v>126</v>
-      </c>
-      <c r="L29">
-        <v>3.4409606285151599E-2</v>
-      </c>
-      <c r="M29">
-        <v>3.4409606285151599E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>124</v>
-      </c>
-      <c r="B30" t="s">
-        <v>110</v>
-      </c>
-      <c r="C30" t="s">
-        <v>154</v>
-      </c>
-      <c r="D30" t="s">
-        <v>126</v>
-      </c>
-      <c r="E30" t="s">
-        <v>83</v>
-      </c>
-      <c r="F30" t="s">
-        <v>126</v>
-      </c>
-      <c r="G30">
-        <v>2018</v>
-      </c>
-      <c r="H30" t="s">
-        <v>126</v>
-      </c>
-      <c r="I30" t="s">
-        <v>126</v>
-      </c>
-      <c r="J30" t="s">
-        <v>126</v>
-      </c>
-      <c r="K30" t="s">
-        <v>126</v>
-      </c>
-      <c r="L30">
-        <v>1.33284867630703E-2</v>
-      </c>
-      <c r="M30">
-        <v>1.33284867630703E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>124</v>
-      </c>
-      <c r="B31" t="s">
-        <v>110</v>
-      </c>
-      <c r="C31" t="s">
-        <v>155</v>
-      </c>
-      <c r="D31" t="s">
-        <v>126</v>
-      </c>
-      <c r="E31" t="s">
-        <v>83</v>
-      </c>
-      <c r="F31" t="s">
-        <v>126</v>
-      </c>
-      <c r="G31">
-        <v>2018</v>
-      </c>
-      <c r="H31" t="s">
-        <v>126</v>
-      </c>
-      <c r="I31" t="s">
-        <v>126</v>
-      </c>
-      <c r="J31" t="s">
-        <v>126</v>
-      </c>
-      <c r="K31" t="s">
-        <v>126</v>
-      </c>
-      <c r="L31">
-        <v>0.113051511576835</v>
-      </c>
-      <c r="M31">
-        <v>0.113051511576835</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
PWR: limit consumption of gas, coal and peat
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_Temporary_Fixes.xlsx
+++ b/SuppXLS/Scen_B_Temporary_Fixes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HannahD\Documents\GitHub\Irish-TIMES-model\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05464919-69B6-4589-B434-8CC3AF30EF45}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{294EB6CC-2331-40B5-9023-859C7A104EFD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4575" yWindow="16050" windowWidth="19650" windowHeight="11070" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="15" r:id="rId1"/>
@@ -161,7 +161,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1820" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1838" uniqueCount="253">
   <si>
     <t>UC_N</t>
   </si>
@@ -931,6 +931,15 @@
   </si>
   <si>
     <t>T-CAR*1</t>
+  </si>
+  <si>
+    <t>FT-PWRCOA</t>
+  </si>
+  <si>
+    <t>FT-PWRGAS</t>
+  </si>
+  <si>
+    <t>FT-PWRPEA</t>
   </si>
 </sst>
 </file>
@@ -3846,16 +3855,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE79BAD-EA44-47F0-A194-320DE6C9FB50}">
-  <dimension ref="B2:M15"/>
+  <dimension ref="B2:M25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
@@ -3994,54 +4004,166 @@
         <v>91</v>
       </c>
     </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" t="s">
+        <v>229</v>
+      </c>
+      <c r="E12">
+        <v>2018</v>
+      </c>
+      <c r="F12">
+        <v>20.6</v>
+      </c>
+      <c r="G12">
+        <f>F12</f>
+        <v>20.6</v>
+      </c>
+      <c r="I12" t="s">
+        <v>250</v>
+      </c>
+    </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B13" s="7" t="s">
+      <c r="C13" t="s">
+        <v>83</v>
+      </c>
+      <c r="D13" t="s">
+        <v>229</v>
+      </c>
+      <c r="E13">
+        <v>2018</v>
+      </c>
+      <c r="F13">
+        <v>22.7</v>
+      </c>
+      <c r="G13">
+        <f>F13</f>
+        <v>22.7</v>
+      </c>
+      <c r="I13" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14" t="s">
+        <v>229</v>
+      </c>
+      <c r="E14">
+        <v>2018</v>
+      </c>
+      <c r="F14">
+        <v>105</v>
+      </c>
+      <c r="G14">
+        <f>F14</f>
+        <v>105</v>
+      </c>
+      <c r="I14" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16" t="s">
+        <v>229</v>
+      </c>
+      <c r="E16">
+        <v>2020</v>
+      </c>
+      <c r="F16">
+        <v>20.5</v>
+      </c>
+      <c r="G16">
+        <f>F16</f>
+        <v>20.5</v>
+      </c>
+      <c r="I16" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>83</v>
+      </c>
+      <c r="D17" t="s">
+        <v>229</v>
+      </c>
+      <c r="E17">
+        <v>2020</v>
+      </c>
+      <c r="I17" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" t="s">
+        <v>229</v>
+      </c>
+      <c r="E18">
+        <v>2020</v>
+      </c>
+      <c r="I18" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B23" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="10" t="s">
+    <row r="24" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C24" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D24" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E24" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F14" s="11" t="str">
+      <c r="F24" s="11" t="str">
         <f>IF(Regions!C$3&lt;&gt;"",Regions!C$3,"*")</f>
         <v>IE</v>
       </c>
-      <c r="G14" s="11" t="str">
+      <c r="G24" s="11" t="str">
         <f>IF(Regions!D$3&lt;&gt;"",Regions!D$3,"*")</f>
         <v>National</v>
       </c>
-      <c r="H14" s="12" t="s">
+      <c r="H24" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I14" s="12" t="s">
+      <c r="I24" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="J14" s="12" t="s">
+      <c r="J24" s="12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="D15" t="s">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
         <v>79</v>
       </c>
-      <c r="F15">
+      <c r="F25">
         <v>2035</v>
       </c>
-      <c r="G15">
-        <f>F15</f>
+      <c r="G25">
+        <f>F25</f>
         <v>2035</v>
       </c>
-      <c r="I15" t="s">
+      <c r="I25" t="s">
         <v>236</v>
       </c>
     </row>
@@ -8098,7 +8220,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8FB1178-AF9A-473D-9FB3-41C2F896D89C}">
   <dimension ref="B3:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
PWR: set a limit on gas consumption in 2020
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_Temporary_Fixes.xlsx
+++ b/SuppXLS/Scen_B_Temporary_Fixes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{294EB6CC-2331-40B5-9023-859C7A104EFD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B108BD9-9888-4C8F-8F3C-A3B090EED405}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -161,7 +161,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1838" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1832" uniqueCount="253">
   <si>
     <t>UC_N</t>
   </si>
@@ -3855,10 +3855,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE79BAD-EA44-47F0-A194-320DE6C9FB50}">
-  <dimension ref="B2:M25"/>
+  <dimension ref="B2:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3949,7 +3949,7 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <f>F8</f>
+        <f t="shared" ref="G8:G15" si="0">F8</f>
         <v>0</v>
       </c>
       <c r="H8" t="s">
@@ -3967,7 +3967,7 @@
         <v>5</v>
       </c>
       <c r="G9">
-        <f>F9</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="H9" t="s">
@@ -3982,7 +3982,7 @@
         <v>2030</v>
       </c>
       <c r="G10">
-        <f>F10</f>
+        <f t="shared" si="0"/>
         <v>2030</v>
       </c>
       <c r="I10" t="s">
@@ -3997,7 +3997,7 @@
         <v>5</v>
       </c>
       <c r="G11">
-        <f>F11</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="I11" t="s">
@@ -4018,7 +4018,7 @@
         <v>20.6</v>
       </c>
       <c r="G12">
-        <f>F12</f>
+        <f t="shared" si="0"/>
         <v>20.6</v>
       </c>
       <c r="I12" t="s">
@@ -4039,7 +4039,7 @@
         <v>22.7</v>
       </c>
       <c r="G13">
-        <f>F13</f>
+        <f t="shared" si="0"/>
         <v>22.7</v>
       </c>
       <c r="I13" t="s">
@@ -4060,110 +4060,82 @@
         <v>105</v>
       </c>
       <c r="G14">
-        <f>F14</f>
+        <f t="shared" si="0"/>
         <v>105</v>
       </c>
       <c r="I14" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
-        <v>83</v>
-      </c>
-      <c r="D16" t="s">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>83</v>
+      </c>
+      <c r="D15" t="s">
         <v>229</v>
       </c>
-      <c r="E16">
+      <c r="E15">
         <v>2020</v>
       </c>
-      <c r="F16">
-        <v>20.5</v>
-      </c>
-      <c r="G16">
-        <f>F16</f>
-        <v>20.5</v>
-      </c>
-      <c r="I16" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
-        <v>83</v>
-      </c>
-      <c r="D17" t="s">
-        <v>229</v>
-      </c>
-      <c r="E17">
-        <v>2020</v>
-      </c>
-      <c r="I17" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
-        <v>83</v>
-      </c>
-      <c r="D18" t="s">
-        <v>229</v>
-      </c>
-      <c r="E18">
-        <v>2020</v>
-      </c>
-      <c r="I18" t="s">
+      <c r="F15">
+        <v>108</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>108</v>
+      </c>
+      <c r="I15" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B23" s="7" t="s">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="10" t="s">
+    <row r="21" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C21" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="D21" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="E21" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F24" s="11" t="str">
+      <c r="F21" s="11" t="str">
         <f>IF(Regions!C$3&lt;&gt;"",Regions!C$3,"*")</f>
         <v>IE</v>
       </c>
-      <c r="G24" s="11" t="str">
+      <c r="G21" s="11" t="str">
         <f>IF(Regions!D$3&lt;&gt;"",Regions!D$3,"*")</f>
         <v>National</v>
       </c>
-      <c r="H24" s="12" t="s">
+      <c r="H21" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I24" s="12" t="s">
+      <c r="I21" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="J24" s="12" t="s">
+      <c r="J21" s="12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D25" t="s">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
         <v>79</v>
       </c>
-      <c r="F25">
+      <c r="F22">
         <v>2035</v>
       </c>
-      <c r="G25">
-        <f>F25</f>
+      <c r="G22">
+        <f>F22</f>
         <v>2035</v>
       </c>
-      <c r="I25" t="s">
+      <c r="I22" t="s">
         <v>236</v>
       </c>
     </row>

</xml_diff>

<commit_message>
PWR: increase PV potential in 2030 to ca. 3 GW
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_Temporary_Fixes.xlsx
+++ b/SuppXLS/Scen_B_Temporary_Fixes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B108BD9-9888-4C8F-8F3C-A3B090EED405}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4124E791-F4A8-43E4-B0DF-C7EAB753B312}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -161,7 +161,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1832" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1859" uniqueCount="259">
   <si>
     <t>UC_N</t>
   </si>
@@ -941,6 +941,25 @@
   <si>
     <t>FT-PWRPEA</t>
   </si>
+  <si>
+    <t>UC_FLO</t>
+  </si>
+  <si>
+    <t>UC_RHSRTS~0</t>
+  </si>
+  <si>
+    <t>ELC_SOLCAP</t>
+  </si>
+  <si>
+    <t>P-RNW-SOL*</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>ELCC</t>
+  </si>
+  <si>
+    <t>Solar PV potenatial</t>
+  </si>
 </sst>
 </file>
 
@@ -949,7 +968,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1028,6 +1047,14 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1312,7 +1339,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1388,6 +1415,15 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1806,7 +1842,7 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.140625" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" customWidth="1"/>
@@ -1838,7 +1874,7 @@
     <col min="30" max="30" width="6.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30">
       <c r="C3" s="13" t="str" cm="1">
         <f t="array" ref="C3">IF(LEFT(INDEX(C5:C7,$A$4),1)&lt;&gt;"*",INDEX(C5:C7,$A$4),"")</f>
         <v>IE</v>
@@ -1952,12 +1988,12 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30">
       <c r="A4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -2072,7 +2108,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -2189,7 +2225,7 @@
         <v>*IE-MN</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -2306,7 +2342,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="10" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" ht="15.75" thickBot="1">
       <c r="A10" s="15" t="s">
         <v>24</v>
       </c>
@@ -2314,7 +2350,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30">
       <c r="A11" s="16" t="s">
         <v>26</v>
       </c>
@@ -2322,7 +2358,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30">
       <c r="A12" s="17" t="s">
         <v>28</v>
       </c>
@@ -2330,7 +2366,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30">
       <c r="A13" s="17" t="s">
         <v>30</v>
       </c>
@@ -2338,7 +2374,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30">
       <c r="A14" s="17" t="s">
         <v>32</v>
       </c>
@@ -2346,7 +2382,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30">
       <c r="A15" s="17" t="s">
         <v>34</v>
       </c>
@@ -2354,7 +2390,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30">
       <c r="A16" s="17" t="s">
         <v>36</v>
       </c>
@@ -2362,7 +2398,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17" s="17" t="s">
         <v>38</v>
       </c>
@@ -2370,7 +2406,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18" s="17" t="s">
         <v>40</v>
       </c>
@@ -2378,7 +2414,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2">
       <c r="A19" s="17" t="s">
         <v>42</v>
       </c>
@@ -2386,7 +2422,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2">
       <c r="A20" s="17" t="s">
         <v>44</v>
       </c>
@@ -2394,7 +2430,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2">
       <c r="A21" s="17" t="s">
         <v>46</v>
       </c>
@@ -2402,7 +2438,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2">
       <c r="A22" s="17" t="s">
         <v>48</v>
       </c>
@@ -2410,7 +2446,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2">
       <c r="A23" s="17" t="s">
         <v>50</v>
       </c>
@@ -2418,7 +2454,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2">
       <c r="A24" s="17" t="s">
         <v>52</v>
       </c>
@@ -2426,7 +2462,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2">
       <c r="A25" s="17" t="s">
         <v>54</v>
       </c>
@@ -2434,7 +2470,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2">
       <c r="A26" s="17" t="s">
         <v>56</v>
       </c>
@@ -2442,7 +2478,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2">
       <c r="A27" s="17" t="s">
         <v>58</v>
       </c>
@@ -2450,7 +2486,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2">
       <c r="A28" s="17" t="s">
         <v>60</v>
       </c>
@@ -2458,7 +2494,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2">
       <c r="A29" s="17" t="s">
         <v>62</v>
       </c>
@@ -2466,7 +2502,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2">
       <c r="A30" s="17" t="s">
         <v>64</v>
       </c>
@@ -2474,7 +2510,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2">
       <c r="A31" s="17" t="s">
         <v>66</v>
       </c>
@@ -2482,7 +2518,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2">
       <c r="A32" s="17" t="s">
         <v>68</v>
       </c>
@@ -2490,7 +2526,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2">
       <c r="A33" s="17" t="s">
         <v>70</v>
       </c>
@@ -2498,7 +2534,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2">
       <c r="A34" s="17" t="s">
         <v>72</v>
       </c>
@@ -2506,7 +2542,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2">
       <c r="A35" s="17" t="s">
         <v>74</v>
       </c>
@@ -2514,7 +2550,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2">
       <c r="A36" s="17" t="s">
         <v>76</v>
       </c>
@@ -2522,7 +2558,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2">
       <c r="A37" s="18" t="s">
         <v>78</v>
       </c>
@@ -2571,13 +2607,13 @@
       <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>113</v>
       </c>
@@ -2618,7 +2654,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>124</v>
       </c>
@@ -2659,7 +2695,7 @@
         <v>1.91859640129881E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>124</v>
       </c>
@@ -2700,7 +2736,7 @@
         <v>1.91859640129881E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>124</v>
       </c>
@@ -2741,7 +2777,7 @@
         <v>1.91859640129881E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
         <v>124</v>
       </c>
@@ -2782,7 +2818,7 @@
         <v>1.91859640129881E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13">
       <c r="A6" t="s">
         <v>124</v>
       </c>
@@ -2823,7 +2859,7 @@
         <v>1.18590868367296E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13">
       <c r="A7" t="s">
         <v>124</v>
       </c>
@@ -2864,7 +2900,7 @@
         <v>3.7359826231663999E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13">
       <c r="A8" t="s">
         <v>124</v>
       </c>
@@ -2905,7 +2941,7 @@
         <v>2.3078593190679501E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13">
       <c r="A9" t="s">
         <v>124</v>
       </c>
@@ -2946,7 +2982,7 @@
         <v>1.7647904805808901E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13">
       <c r="A10" t="s">
         <v>124</v>
       </c>
@@ -2987,7 +3023,7 @@
         <v>2.4653262579847901E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13">
       <c r="A11" t="s">
         <v>124</v>
       </c>
@@ -3028,7 +3064,7 @@
         <v>2.4653262579847901E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13">
       <c r="A12" t="s">
         <v>124</v>
       </c>
@@ -3069,7 +3105,7 @@
         <v>2.4653262579847901E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13">
       <c r="A13" t="s">
         <v>124</v>
       </c>
@@ -3110,7 +3146,7 @@
         <v>2.4653262579847901E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13">
       <c r="A14" t="s">
         <v>124</v>
       </c>
@@ -3151,7 +3187,7 @@
         <v>2.2095891324020799E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13">
       <c r="A15" t="s">
         <v>124</v>
       </c>
@@ -3192,7 +3228,7 @@
         <v>2.8368761423682901E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13">
       <c r="A16" t="s">
         <v>124</v>
       </c>
@@ -3233,7 +3269,7 @@
         <v>3.0936872888717201E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13">
       <c r="A17" t="s">
         <v>124</v>
       </c>
@@ -3274,7 +3310,7 @@
         <v>7.5066866433008306E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13">
       <c r="A18" t="s">
         <v>124</v>
       </c>
@@ -3315,7 +3351,7 @@
         <v>4.1614408271926799E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13">
       <c r="A19" t="s">
         <v>124</v>
       </c>
@@ -3356,7 +3392,7 @@
         <v>4.1614408271926799E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13">
       <c r="A20" t="s">
         <v>124</v>
       </c>
@@ -3397,7 +3433,7 @@
         <v>4.1614408271926799E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13">
       <c r="A21" t="s">
         <v>124</v>
       </c>
@@ -3438,7 +3474,7 @@
         <v>4.1614408271926799E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13">
       <c r="A22" t="s">
         <v>124</v>
       </c>
@@ -3479,7 +3515,7 @@
         <v>3.7040631160092499E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13">
       <c r="A23" t="s">
         <v>124</v>
       </c>
@@ -3520,7 +3556,7 @@
         <v>4.6621727976421598E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13">
       <c r="A24" t="s">
         <v>124</v>
       </c>
@@ -3561,7 +3597,7 @@
         <v>6.7033675870053502E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13">
       <c r="A25" t="s">
         <v>124</v>
       </c>
@@ -3602,7 +3638,7 @@
         <v>9.1153830584100495E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13">
       <c r="A26" t="s">
         <v>124</v>
       </c>
@@ -3643,7 +3679,7 @@
         <v>2.2735699655164601E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13">
       <c r="A27" t="s">
         <v>124</v>
       </c>
@@ -3684,7 +3720,7 @@
         <v>8.6298729994523198E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13">
       <c r="A28" t="s">
         <v>124</v>
       </c>
@@ -3725,7 +3761,7 @@
         <v>1.29275684703049E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13">
       <c r="A29" t="s">
         <v>124</v>
       </c>
@@ -3766,7 +3802,7 @@
         <v>3.4409606285151599E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13">
       <c r="A30" t="s">
         <v>124</v>
       </c>
@@ -3807,7 +3843,7 @@
         <v>1.33284867630703E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13">
       <c r="A31" t="s">
         <v>124</v>
       </c>
@@ -3855,25 +3891,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE79BAD-EA44-47F0-A194-320DE6C9FB50}">
-  <dimension ref="B2:M22"/>
+  <dimension ref="B2:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:13">
       <c r="B2" s="7" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:13" ht="15.75" thickBot="1">
       <c r="B3" s="10" t="s">
         <v>12</v>
       </c>
@@ -3901,13 +3937,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:13">
       <c r="B6" s="7" t="s">
         <v>88</v>
       </c>
       <c r="M6" s="9"/>
     </row>
-    <row r="7" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:13" ht="15.75" thickBot="1">
       <c r="B7" s="10" t="s">
         <v>12</v>
       </c>
@@ -3938,7 +3974,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:13">
       <c r="D8" t="s">
         <v>90</v>
       </c>
@@ -3956,7 +3992,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:13">
       <c r="D9" t="s">
         <v>90</v>
       </c>
@@ -3974,7 +4010,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:13">
       <c r="D10" t="s">
         <v>79</v>
       </c>
@@ -3989,7 +4025,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:13">
       <c r="D11" t="s">
         <v>92</v>
       </c>
@@ -4004,7 +4040,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:13">
       <c r="C12" t="s">
         <v>83</v>
       </c>
@@ -4025,7 +4061,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:13">
       <c r="C13" t="s">
         <v>83</v>
       </c>
@@ -4046,7 +4082,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:13">
       <c r="C14" t="s">
         <v>83</v>
       </c>
@@ -4067,7 +4103,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:13">
       <c r="C15" t="s">
         <v>83</v>
       </c>
@@ -4088,12 +4124,12 @@
         <v>251</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:15">
       <c r="B20" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:15" ht="15.75" thickBot="1">
       <c r="B21" s="10" t="s">
         <v>12</v>
       </c>
@@ -4124,7 +4160,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:15">
       <c r="D22" t="s">
         <v>79</v>
       </c>
@@ -4138,6 +4174,138 @@
       <c r="I22" t="s">
         <v>236</v>
       </c>
+    </row>
+    <row r="26" spans="2:15">
+      <c r="B26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="2:15">
+      <c r="C27" s="44" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,"~UC_Sets: R_E:",_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,"")))</f>
+        <v>~UC_Sets: R_E: IE,National</v>
+      </c>
+    </row>
+    <row r="28" spans="2:15">
+      <c r="C28" s="44" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="2:15">
+      <c r="K29" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="2:15">
+      <c r="C30" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="D30" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="F30" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="G30" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="H30" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="I30" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="J30" s="47" t="s">
+        <v>2</v>
+      </c>
+      <c r="K30" s="47" t="s">
+        <v>9</v>
+      </c>
+      <c r="L30" s="48" t="s">
+        <v>253</v>
+      </c>
+      <c r="M30" s="48" t="s">
+        <v>17</v>
+      </c>
+      <c r="N30" s="48" t="s">
+        <v>254</v>
+      </c>
+      <c r="O30" s="49" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="2:15">
+      <c r="C31" t="s">
+        <v>255</v>
+      </c>
+      <c r="E31" s="50" t="s">
+        <v>256</v>
+      </c>
+      <c r="H31" t="s">
+        <v>257</v>
+      </c>
+      <c r="J31">
+        <v>2020</v>
+      </c>
+      <c r="K31" t="s">
+        <v>83</v>
+      </c>
+      <c r="L31">
+        <v>1</v>
+      </c>
+      <c r="M31">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="N31">
+        <v>15</v>
+      </c>
+      <c r="O31" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="32" spans="2:15">
+      <c r="E32" s="50" t="s">
+        <v>256</v>
+      </c>
+      <c r="H32" t="s">
+        <v>257</v>
+      </c>
+      <c r="J32">
+        <v>2030</v>
+      </c>
+      <c r="K32" t="s">
+        <v>83</v>
+      </c>
+      <c r="L32">
+        <v>1</v>
+      </c>
+      <c r="M32">
+        <v>9.4499999999999993</v>
+      </c>
+    </row>
+    <row r="33" spans="5:14">
+      <c r="E33" s="50" t="s">
+        <v>256</v>
+      </c>
+      <c r="H33" t="s">
+        <v>257</v>
+      </c>
+      <c r="J33">
+        <v>2050</v>
+      </c>
+      <c r="K33" t="s">
+        <v>83</v>
+      </c>
+      <c r="L33">
+        <v>1</v>
+      </c>
+      <c r="M33">
+        <v>11.03</v>
+      </c>
+      <c r="N33" s="48"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4152,7 +4320,7 @@
       <selection activeCell="B11" sqref="B11:I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
@@ -4164,7 +4332,7 @@
     <col min="10" max="10" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12">
       <c r="B3" s="7" t="s">
         <v>88</v>
       </c>
@@ -4172,7 +4340,7 @@
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
     </row>
-    <row r="4" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:12" ht="15.75" thickBot="1">
       <c r="B4" s="10" t="s">
         <v>12</v>
       </c>
@@ -4206,7 +4374,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12">
       <c r="C5" t="s">
         <v>83</v>
       </c>
@@ -4230,7 +4398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12">
       <c r="C6" t="str">
         <f>C5</f>
         <v>UP</v>
@@ -4254,14 +4422,14 @@
         <v>IMPBIO*1G*2,IMPBIO*1G*3,IMPBIO*1G*4</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12">
       <c r="B11" s="7" t="s">
         <v>88</v>
       </c>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
     </row>
-    <row r="12" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:12" ht="15.75" thickBot="1">
       <c r="B12" s="10" t="s">
         <v>12</v>
       </c>
@@ -4289,7 +4457,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12">
       <c r="C13" t="s">
         <v>83</v>
       </c>
@@ -4313,7 +4481,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12">
       <c r="C14" t="str">
         <f>C13</f>
         <v>UP</v>
@@ -4340,7 +4508,7 @@
         <v>*GRID*</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:12">
       <c r="C15" t="s">
         <v>83</v>
       </c>
@@ -4361,7 +4529,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12">
       <c r="C16" t="str">
         <f>C15</f>
         <v>UP</v>
@@ -4398,35 +4566,35 @@
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15">
       <c r="B2" s="1" t="str">
         <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3:D3)</f>
         <v>~UC_Sets: R_E: IE,National</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15">
       <c r="B3" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15">
       <c r="J4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15">
       <c r="B5" s="4" t="s">
         <v>0</v>
       </c>
@@ -4464,7 +4632,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15">
       <c r="B6" t="s">
         <v>85</v>
       </c>
@@ -4487,7 +4655,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15">
       <c r="I7">
         <v>0</v>
       </c>
@@ -4495,12 +4663,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15">
       <c r="B13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15">
       <c r="C14" s="7" t="s">
         <v>15</v>
       </c>
@@ -4508,7 +4676,7 @@
       <c r="K14" s="9"/>
       <c r="L14" s="9"/>
     </row>
-    <row r="15" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" ht="15.75" thickBot="1">
       <c r="C15" s="10" t="s">
         <v>12</v>
       </c>
@@ -4542,7 +4710,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15">
       <c r="E16" t="s">
         <v>79</v>
       </c>
@@ -4574,20 +4742,20 @@
       <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9">
       <c r="B3" s="7" t="s">
         <v>88</v>
       </c>
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
     </row>
-    <row r="4" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:9" ht="15.75" thickBot="1">
       <c r="B4" s="10" t="s">
         <v>12</v>
       </c>
@@ -4615,7 +4783,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9">
       <c r="C5" t="s">
         <v>83</v>
       </c>
@@ -4636,7 +4804,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9">
       <c r="C6" t="s">
         <v>83</v>
       </c>
@@ -4657,7 +4825,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9">
       <c r="C7" t="s">
         <v>83</v>
       </c>
@@ -4678,7 +4846,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9">
       <c r="C8" t="s">
         <v>83</v>
       </c>
@@ -4699,7 +4867,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9">
       <c r="C9" t="s">
         <v>83</v>
       </c>
@@ -4720,7 +4888,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9">
       <c r="C10" t="s">
         <v>83</v>
       </c>
@@ -4741,7 +4909,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9">
       <c r="C11" t="s">
         <v>83</v>
       </c>
@@ -4762,7 +4930,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9">
       <c r="C12" t="s">
         <v>83</v>
       </c>
@@ -4796,7 +4964,7 @@
       <selection activeCell="B23" sqref="B23:K24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="27.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
@@ -4809,28 +4977,28 @@
     <col min="14" max="14" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="B2" s="1" t="str">
         <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3:D3)</f>
         <v>~UC_Sets: R_E: IE,National</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="B3" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="I4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="B5" s="4" t="s">
         <v>0</v>
       </c>
@@ -4865,7 +5033,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12">
       <c r="B6" t="s">
         <v>98</v>
       </c>
@@ -4891,7 +5059,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12">
       <c r="D7" s="36" t="s">
         <v>217</v>
       </c>
@@ -4908,7 +5076,7 @@
       <c r="K7" s="36"/>
       <c r="L7" s="36"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12">
       <c r="D8" s="36" t="s">
         <v>220</v>
       </c>
@@ -4927,7 +5095,7 @@
       <c r="K8" s="36"/>
       <c r="L8" s="36"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12">
       <c r="D9" s="37"/>
       <c r="E9" s="37"/>
       <c r="F9" s="37"/>
@@ -4944,7 +5112,7 @@
       </c>
       <c r="L9" s="37"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12">
       <c r="B10" t="s">
         <v>97</v>
       </c>
@@ -4970,7 +5138,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12">
       <c r="D11" s="36" t="s">
         <v>218</v>
       </c>
@@ -4987,7 +5155,7 @@
       <c r="K11" s="36"/>
       <c r="L11" s="36"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12">
       <c r="D12" s="36" t="s">
         <v>220</v>
       </c>
@@ -5006,7 +5174,7 @@
       <c r="K12" s="36"/>
       <c r="L12" s="36"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12">
       <c r="D13" s="37"/>
       <c r="E13" s="37"/>
       <c r="F13" s="37"/>
@@ -5021,7 +5189,7 @@
       </c>
       <c r="L13" s="37"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12">
       <c r="B14" t="s">
         <v>96</v>
       </c>
@@ -5047,7 +5215,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12">
       <c r="D15" s="36" t="s">
         <v>219</v>
       </c>
@@ -5064,7 +5232,7 @@
       <c r="K15" s="36"/>
       <c r="L15" s="36"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12">
       <c r="D16" s="36" t="s">
         <v>220</v>
       </c>
@@ -5083,7 +5251,7 @@
       <c r="K16" s="36"/>
       <c r="L16" s="36"/>
     </row>
-    <row r="17" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:19" ht="15.75" thickBot="1">
       <c r="D17" s="37"/>
       <c r="E17" s="37"/>
       <c r="F17" s="37"/>
@@ -5100,7 +5268,7 @@
       </c>
       <c r="L17" s="37"/>
     </row>
-    <row r="18" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:19" ht="15.75" thickBot="1">
       <c r="N18" s="41">
         <v>2018</v>
       </c>
@@ -5112,7 +5280,7 @@
       <c r="R18" s="42"/>
       <c r="S18" s="43"/>
     </row>
-    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:19">
       <c r="N19" s="29" t="s">
         <v>211</v>
       </c>
@@ -5132,7 +5300,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="20" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:19">
       <c r="L20" t="s">
         <v>214</v>
       </c>
@@ -5158,7 +5326,7 @@
         <v>42368.736851186717</v>
       </c>
     </row>
-    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:19">
       <c r="L21" t="s">
         <v>215</v>
       </c>
@@ -5184,7 +5352,7 @@
         <v>49085.372703580208</v>
       </c>
     </row>
-    <row r="22" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:19" ht="15.75" thickBot="1">
       <c r="L22" t="s">
         <v>216</v>
       </c>
@@ -5210,7 +5378,7 @@
         <v>80871.401315733063</v>
       </c>
     </row>
-    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:19">
       <c r="B23" s="7" t="s">
         <v>88</v>
       </c>
@@ -5218,7 +5386,7 @@
       <c r="J23" s="9"/>
       <c r="K23" s="9"/>
     </row>
-    <row r="24" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:19" ht="15.75" thickBot="1">
       <c r="B24" s="10" t="s">
         <v>12</v>
       </c>
@@ -5252,7 +5420,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:19">
       <c r="C25" t="s">
         <v>83</v>
       </c>
@@ -5275,7 +5443,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="26" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:19">
       <c r="C26" t="s">
         <v>83</v>
       </c>
@@ -5295,7 +5463,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="27" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:19">
       <c r="C27" t="s">
         <v>83</v>
       </c>
@@ -5315,7 +5483,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="28" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:19">
       <c r="C28" t="s">
         <v>83</v>
       </c>
@@ -5335,7 +5503,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="29" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:19">
       <c r="C29" t="s">
         <v>83</v>
       </c>
@@ -5355,7 +5523,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="30" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:19">
       <c r="C30" t="s">
         <v>83</v>
       </c>
@@ -5375,15 +5543,15 @@
         <v>246</v>
       </c>
     </row>
-    <row r="31" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:19">
       <c r="H31" s="26"/>
       <c r="I31" s="26"/>
     </row>
-    <row r="32" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:19">
       <c r="H32" s="26"/>
       <c r="I32" s="26"/>
     </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:13">
       <c r="B33" s="7" t="s">
         <v>88</v>
       </c>
@@ -5391,7 +5559,7 @@
       <c r="J33" s="9"/>
       <c r="K33" s="9"/>
     </row>
-    <row r="34" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:13" ht="15.75" thickBot="1">
       <c r="B34" s="10" t="s">
         <v>12</v>
       </c>
@@ -5425,7 +5593,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:13">
       <c r="C35" t="s">
         <v>208</v>
       </c>
@@ -5448,7 +5616,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:13">
       <c r="C36" t="s">
         <v>208</v>
       </c>
@@ -5468,7 +5636,7 @@
         <v>R-HC_Apt_ELC_HPN1</v>
       </c>
     </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:13">
       <c r="C37" t="s">
         <v>208</v>
       </c>
@@ -5488,7 +5656,7 @@
         <v>R-HC_Apt_ELC_HPN1</v>
       </c>
     </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:13">
       <c r="C38" t="s">
         <v>208</v>
       </c>
@@ -5508,7 +5676,7 @@
         <v>R-HC_Apt_ELC_HPN2</v>
       </c>
     </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:13">
       <c r="C39" t="s">
         <v>208</v>
       </c>
@@ -5528,7 +5696,7 @@
         <v>R-HC_Apt_ELC_HPN2</v>
       </c>
     </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:13">
       <c r="C40" t="s">
         <v>208</v>
       </c>
@@ -5548,7 +5716,7 @@
         <v>R-HC_Att_ELC_HPN1</v>
       </c>
     </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:13">
       <c r="C41" t="s">
         <v>208</v>
       </c>
@@ -5568,7 +5736,7 @@
         <v>R-HC_Att_ELC_HPN1</v>
       </c>
     </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:13">
       <c r="C42" t="s">
         <v>208</v>
       </c>
@@ -5588,7 +5756,7 @@
         <v>R-HC_Att_ELC_HPN2</v>
       </c>
     </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:13">
       <c r="C43" t="s">
         <v>208</v>
       </c>
@@ -5608,7 +5776,7 @@
         <v>R-HC_Att_ELC_HPN2</v>
       </c>
     </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:13">
       <c r="C44" t="s">
         <v>208</v>
       </c>
@@ -5628,7 +5796,7 @@
         <v>R-HC_Det_ELC_HPN1</v>
       </c>
     </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:13">
       <c r="C45" t="s">
         <v>208</v>
       </c>
@@ -5648,7 +5816,7 @@
         <v>R-HC_Det_ELC_HPN1</v>
       </c>
     </row>
-    <row r="46" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:13">
       <c r="C46" t="s">
         <v>208</v>
       </c>
@@ -5668,7 +5836,7 @@
         <v>R-HC_Det_ELC_HPN2</v>
       </c>
     </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:13">
       <c r="C47" t="s">
         <v>208</v>
       </c>
@@ -5688,7 +5856,7 @@
         <v>R-HC_Det_ELC_HPN2</v>
       </c>
     </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:13">
       <c r="C48" t="s">
         <v>208</v>
       </c>
@@ -5708,7 +5876,7 @@
         <v>R-SW_Apt_ELC_HPN1</v>
       </c>
     </row>
-    <row r="49" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:11">
       <c r="C49" t="s">
         <v>208</v>
       </c>
@@ -5728,7 +5896,7 @@
         <v>R-SW_Apt_ELC_HPN1</v>
       </c>
     </row>
-    <row r="50" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:11">
       <c r="C50" t="s">
         <v>208</v>
       </c>
@@ -5748,7 +5916,7 @@
         <v>R-SW_Apt_GAS_HHPN1</v>
       </c>
     </row>
-    <row r="51" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:11">
       <c r="C51" t="s">
         <v>208</v>
       </c>
@@ -5768,7 +5936,7 @@
         <v>R-SW_Apt_GAS_HHPN1</v>
       </c>
     </row>
-    <row r="52" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:11">
       <c r="C52" t="s">
         <v>208</v>
       </c>
@@ -5788,7 +5956,7 @@
         <v>R-SW_Apt_GAS_HPN1</v>
       </c>
     </row>
-    <row r="53" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:11">
       <c r="C53" t="s">
         <v>208</v>
       </c>
@@ -5808,7 +5976,7 @@
         <v>R-SW_Apt_GAS_HPN1</v>
       </c>
     </row>
-    <row r="54" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:11">
       <c r="C54" t="s">
         <v>208</v>
       </c>
@@ -5828,7 +5996,7 @@
         <v>R-SW_Apt_GAS_HPN2</v>
       </c>
     </row>
-    <row r="55" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:11">
       <c r="C55" t="s">
         <v>208</v>
       </c>
@@ -5848,7 +6016,7 @@
         <v>R-SW_Apt_GAS_HPN2</v>
       </c>
     </row>
-    <row r="56" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:11">
       <c r="C56" t="s">
         <v>208</v>
       </c>
@@ -5868,7 +6036,7 @@
         <v>R-SW_Apt_GAS_N1</v>
       </c>
     </row>
-    <row r="57" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:11">
       <c r="C57" t="s">
         <v>208</v>
       </c>
@@ -5888,7 +6056,7 @@
         <v>R-SW_Apt_GAS_N1</v>
       </c>
     </row>
-    <row r="58" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:11">
       <c r="C58" t="s">
         <v>208</v>
       </c>
@@ -5908,7 +6076,7 @@
         <v>R-SW_Apt_HET_N1</v>
       </c>
     </row>
-    <row r="59" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:11">
       <c r="C59" t="s">
         <v>208</v>
       </c>
@@ -5928,7 +6096,7 @@
         <v>R-SW_Apt_HET_N1</v>
       </c>
     </row>
-    <row r="60" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:11">
       <c r="C60" t="s">
         <v>208</v>
       </c>
@@ -5948,7 +6116,7 @@
         <v>R-SW_Apt_HET_N2</v>
       </c>
     </row>
-    <row r="61" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:11">
       <c r="C61" t="s">
         <v>208</v>
       </c>
@@ -5968,7 +6136,7 @@
         <v>R-SW_Apt_HET_N2</v>
       </c>
     </row>
-    <row r="62" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:11">
       <c r="C62" t="s">
         <v>208</v>
       </c>
@@ -5988,7 +6156,7 @@
         <v>R-SW_Apt_KER_N1</v>
       </c>
     </row>
-    <row r="63" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:11">
       <c r="C63" t="s">
         <v>208</v>
       </c>
@@ -6008,7 +6176,7 @@
         <v>R-SW_Apt_KER_N1</v>
       </c>
     </row>
-    <row r="64" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:11">
       <c r="C64" t="s">
         <v>208</v>
       </c>
@@ -6028,7 +6196,7 @@
         <v>R-SW_Apt_LPG_N1</v>
       </c>
     </row>
-    <row r="65" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:11">
       <c r="C65" t="s">
         <v>208</v>
       </c>
@@ -6048,7 +6216,7 @@
         <v>R-SW_Apt_LPG_N1</v>
       </c>
     </row>
-    <row r="66" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:11">
       <c r="C66" t="s">
         <v>208</v>
       </c>
@@ -6068,7 +6236,7 @@
         <v>R-SW_Apt_WOO_N1</v>
       </c>
     </row>
-    <row r="67" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:11">
       <c r="C67" t="s">
         <v>208</v>
       </c>
@@ -6088,7 +6256,7 @@
         <v>R-SW_Apt_WOO_N1</v>
       </c>
     </row>
-    <row r="68" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:11">
       <c r="C68" t="s">
         <v>208</v>
       </c>
@@ -6108,7 +6276,7 @@
         <v>R-SW_Att_ELC_HPN1</v>
       </c>
     </row>
-    <row r="69" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:11">
       <c r="C69" t="s">
         <v>208</v>
       </c>
@@ -6128,7 +6296,7 @@
         <v>R-SW_Att_ELC_HPN1</v>
       </c>
     </row>
-    <row r="70" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:11">
       <c r="C70" t="s">
         <v>208</v>
       </c>
@@ -6148,7 +6316,7 @@
         <v>R-SW_Att_ELC_HPN2</v>
       </c>
     </row>
-    <row r="71" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:11">
       <c r="C71" t="s">
         <v>208</v>
       </c>
@@ -6168,7 +6336,7 @@
         <v>R-SW_Att_ELC_HPN2</v>
       </c>
     </row>
-    <row r="72" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:11">
       <c r="C72" t="s">
         <v>208</v>
       </c>
@@ -6188,7 +6356,7 @@
         <v>R-SW_Att_GAS_HHPN1</v>
       </c>
     </row>
-    <row r="73" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:11">
       <c r="C73" t="s">
         <v>208</v>
       </c>
@@ -6208,7 +6376,7 @@
         <v>R-SW_Att_GAS_HHPN1</v>
       </c>
     </row>
-    <row r="74" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:11">
       <c r="C74" t="s">
         <v>208</v>
       </c>
@@ -6228,7 +6396,7 @@
         <v>R-SW_Att_GAS_HPN1</v>
       </c>
     </row>
-    <row r="75" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:11">
       <c r="C75" t="s">
         <v>208</v>
       </c>
@@ -6248,7 +6416,7 @@
         <v>R-SW_Att_GAS_HPN1</v>
       </c>
     </row>
-    <row r="76" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:11">
       <c r="C76" t="s">
         <v>208</v>
       </c>
@@ -6268,7 +6436,7 @@
         <v>R-SW_Att_GAS_HPN2</v>
       </c>
     </row>
-    <row r="77" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:11">
       <c r="C77" t="s">
         <v>208</v>
       </c>
@@ -6288,7 +6456,7 @@
         <v>R-SW_Att_GAS_HPN2</v>
       </c>
     </row>
-    <row r="78" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:11">
       <c r="C78" t="s">
         <v>208</v>
       </c>
@@ -6308,7 +6476,7 @@
         <v>R-SW_Att_GAS_N1</v>
       </c>
     </row>
-    <row r="79" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:11">
       <c r="C79" t="s">
         <v>208</v>
       </c>
@@ -6328,7 +6496,7 @@
         <v>R-SW_Att_GAS_N1</v>
       </c>
     </row>
-    <row r="80" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:11">
       <c r="C80" t="s">
         <v>208</v>
       </c>
@@ -6348,7 +6516,7 @@
         <v>R-SW_Att_GAS_N2</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11">
       <c r="C81" t="s">
         <v>208</v>
       </c>
@@ -6368,7 +6536,7 @@
         <v>R-SW_Att_GAS_N2</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11">
       <c r="C82" t="s">
         <v>208</v>
       </c>
@@ -6388,7 +6556,7 @@
         <v>R-SW_Att_GAS_N3</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11">
       <c r="C83" t="s">
         <v>208</v>
       </c>
@@ -6408,7 +6576,7 @@
         <v>R-SW_Att_GAS_N3</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11">
       <c r="C84" t="s">
         <v>208</v>
       </c>
@@ -6428,7 +6596,7 @@
         <v>R-SW_Att_HET_N1</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11">
       <c r="C85" t="s">
         <v>208</v>
       </c>
@@ -6448,7 +6616,7 @@
         <v>R-SW_Att_HET_N1</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11">
       <c r="C86" t="s">
         <v>208</v>
       </c>
@@ -6468,7 +6636,7 @@
         <v>R-SW_Att_HET_N2</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11">
       <c r="C87" t="s">
         <v>208</v>
       </c>
@@ -6488,7 +6656,7 @@
         <v>R-SW_Att_HET_N2</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11">
       <c r="C88" t="s">
         <v>208</v>
       </c>
@@ -6508,7 +6676,7 @@
         <v>R-SW_Att_KER_N1</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11">
       <c r="C89" t="s">
         <v>208</v>
       </c>
@@ -6528,7 +6696,7 @@
         <v>R-SW_Att_KER_N1</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11">
       <c r="C90" t="s">
         <v>208</v>
       </c>
@@ -6548,7 +6716,7 @@
         <v>R-SW_Att_KER_N2</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11">
       <c r="C91" t="s">
         <v>208</v>
       </c>
@@ -6568,7 +6736,7 @@
         <v>R-SW_Att_KER_N2</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11">
       <c r="C92" t="s">
         <v>208</v>
       </c>
@@ -6588,7 +6756,7 @@
         <v>R-SW_Att_KER_N3</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11">
       <c r="C93" t="s">
         <v>208</v>
       </c>
@@ -6608,7 +6776,7 @@
         <v>R-SW_Att_KER_N3</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11">
       <c r="A94" s="39"/>
       <c r="B94" s="39"/>
       <c r="C94" s="39" t="s">
@@ -6633,7 +6801,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11">
       <c r="A95" s="39"/>
       <c r="B95" s="39"/>
       <c r="C95" s="39" t="s">
@@ -6658,7 +6826,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11">
       <c r="A96" s="39"/>
       <c r="B96" s="39"/>
       <c r="C96" s="39" t="s">
@@ -6683,7 +6851,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11">
       <c r="A97" s="39"/>
       <c r="B97" s="39"/>
       <c r="C97" s="39" t="s">
@@ -6708,7 +6876,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11">
       <c r="C98" t="s">
         <v>208</v>
       </c>
@@ -6728,7 +6896,7 @@
         <v>R-SW_Att_LPG_N1</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11">
       <c r="C99" t="s">
         <v>208</v>
       </c>
@@ -6748,7 +6916,7 @@
         <v>R-SW_Att_LPG_N1</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11">
       <c r="C100" t="s">
         <v>208</v>
       </c>
@@ -6768,7 +6936,7 @@
         <v>R-SW_Att_WOO_N1</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11">
       <c r="C101" t="s">
         <v>208</v>
       </c>
@@ -6788,7 +6956,7 @@
         <v>R-SW_Att_WOO_N1</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11">
       <c r="C102" t="s">
         <v>208</v>
       </c>
@@ -6808,7 +6976,7 @@
         <v>R-SW_Det_ELC_HPN1</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11">
       <c r="C103" t="s">
         <v>208</v>
       </c>
@@ -6828,7 +6996,7 @@
         <v>R-SW_Det_ELC_HPN1</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11">
       <c r="C104" t="s">
         <v>208</v>
       </c>
@@ -6848,7 +7016,7 @@
         <v>R-SW_Det_ELC_HPN2</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11">
       <c r="C105" t="s">
         <v>208</v>
       </c>
@@ -6868,7 +7036,7 @@
         <v>R-SW_Det_ELC_HPN2</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11">
       <c r="C106" t="s">
         <v>208</v>
       </c>
@@ -6888,7 +7056,7 @@
         <v>R-SW_Det_GAS_HHPN1</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11">
       <c r="C107" t="s">
         <v>208</v>
       </c>
@@ -6908,7 +7076,7 @@
         <v>R-SW_Det_GAS_HHPN1</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11">
       <c r="C108" t="s">
         <v>208</v>
       </c>
@@ -6928,7 +7096,7 @@
         <v>R-SW_Det_GAS_HPN1</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11">
       <c r="C109" t="s">
         <v>208</v>
       </c>
@@ -6948,7 +7116,7 @@
         <v>R-SW_Det_GAS_HPN1</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11">
       <c r="C110" t="s">
         <v>208</v>
       </c>
@@ -6968,7 +7136,7 @@
         <v>R-SW_Det_GAS_HPN2</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11">
       <c r="C111" t="s">
         <v>208</v>
       </c>
@@ -6988,7 +7156,7 @@
         <v>R-SW_Det_GAS_HPN2</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11">
       <c r="C112" t="s">
         <v>208</v>
       </c>
@@ -7008,7 +7176,7 @@
         <v>R-SW_Det_GAS_N1</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11">
       <c r="C113" t="s">
         <v>208</v>
       </c>
@@ -7028,7 +7196,7 @@
         <v>R-SW_Det_GAS_N1</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11">
       <c r="C114" t="s">
         <v>208</v>
       </c>
@@ -7048,7 +7216,7 @@
         <v>R-SW_Det_GAS_N2</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11">
       <c r="C115" t="s">
         <v>208</v>
       </c>
@@ -7068,7 +7236,7 @@
         <v>R-SW_Det_GAS_N2</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11">
       <c r="C116" t="s">
         <v>208</v>
       </c>
@@ -7088,7 +7256,7 @@
         <v>R-SW_Det_GAS_N3</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11">
       <c r="C117" t="s">
         <v>208</v>
       </c>
@@ -7108,7 +7276,7 @@
         <v>R-SW_Det_GAS_N3</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11">
       <c r="C118" t="s">
         <v>208</v>
       </c>
@@ -7128,7 +7296,7 @@
         <v>R-SW_Det_HET_N1</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11">
       <c r="C119" t="s">
         <v>208</v>
       </c>
@@ -7148,7 +7316,7 @@
         <v>R-SW_Det_HET_N1</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11">
       <c r="C120" t="s">
         <v>208</v>
       </c>
@@ -7168,7 +7336,7 @@
         <v>R-SW_Det_HET_N2</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11">
       <c r="C121" t="s">
         <v>208</v>
       </c>
@@ -7188,7 +7356,7 @@
         <v>R-SW_Det_HET_N2</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11">
       <c r="C122" t="s">
         <v>208</v>
       </c>
@@ -7208,7 +7376,7 @@
         <v>R-SW_Det_KER_N1</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11">
       <c r="C123" t="s">
         <v>208</v>
       </c>
@@ -7228,7 +7396,7 @@
         <v>R-SW_Det_KER_N1</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11">
       <c r="C124" t="s">
         <v>208</v>
       </c>
@@ -7248,7 +7416,7 @@
         <v>R-SW_Det_KER_N2</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11">
       <c r="C125" t="s">
         <v>208</v>
       </c>
@@ -7268,7 +7436,7 @@
         <v>R-SW_Det_KER_N2</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11">
       <c r="C126" t="s">
         <v>208</v>
       </c>
@@ -7288,7 +7456,7 @@
         <v>R-SW_Det_KER_N3</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11">
       <c r="C127" t="s">
         <v>208</v>
       </c>
@@ -7308,7 +7476,7 @@
         <v>R-SW_Det_KER_N3</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11">
       <c r="A128" s="39"/>
       <c r="B128" s="39"/>
       <c r="C128" s="39" t="s">
@@ -7333,7 +7501,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11">
       <c r="A129" s="39"/>
       <c r="B129" s="39"/>
       <c r="C129" s="39" t="s">
@@ -7358,7 +7526,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11">
       <c r="A130" s="39"/>
       <c r="B130" s="39"/>
       <c r="C130" s="39" t="s">
@@ -7383,7 +7551,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11">
       <c r="A131" s="39"/>
       <c r="B131" s="39"/>
       <c r="C131" s="39" t="s">
@@ -7408,7 +7576,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:11">
       <c r="C132" t="s">
         <v>208</v>
       </c>
@@ -7428,7 +7596,7 @@
         <v>R-SW_Det_LPG_N1</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:11">
       <c r="C133" t="s">
         <v>208</v>
       </c>
@@ -7448,7 +7616,7 @@
         <v>R-SW_Det_LPG_N1</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:11">
       <c r="C134" t="s">
         <v>208</v>
       </c>
@@ -7468,7 +7636,7 @@
         <v>R-SW_Det_WOO_N1</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:11">
       <c r="C135" t="s">
         <v>208</v>
       </c>
@@ -7488,7 +7656,7 @@
         <v>R-SW_Det_WOO_N1</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:11">
       <c r="C136" t="s">
         <v>208</v>
       </c>
@@ -7508,7 +7676,7 @@
         <v>R-SH_Apt_ELC_HPN1</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:11">
       <c r="C137" t="s">
         <v>208</v>
       </c>
@@ -7528,7 +7696,7 @@
         <v>R-SH_Apt_ELC_HPN2</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:11">
       <c r="C138" t="s">
         <v>208</v>
       </c>
@@ -7548,7 +7716,7 @@
         <v>R-SH_Apt_ELC_HPN3</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:11">
       <c r="C139" t="s">
         <v>208</v>
       </c>
@@ -7568,7 +7736,7 @@
         <v>R-SH_Apt_ELC_N1</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:11">
       <c r="C140" t="s">
         <v>208</v>
       </c>
@@ -7588,7 +7756,7 @@
         <v>R-SH_Apt_GAS_N1</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:11">
       <c r="C141" t="s">
         <v>208</v>
       </c>
@@ -7608,7 +7776,7 @@
         <v>R-SH_Apt_KER_N1</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:11">
       <c r="C142" t="s">
         <v>208</v>
       </c>
@@ -7628,7 +7796,7 @@
         <v>R-SH_Apt_LPG_N1</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:11">
       <c r="C143" t="s">
         <v>208</v>
       </c>
@@ -7648,7 +7816,7 @@
         <v>R-SH_Apt_WOO_N1</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:11">
       <c r="C144" t="s">
         <v>208</v>
       </c>
@@ -7668,7 +7836,7 @@
         <v>R-SH_Att_ELC_HPN1</v>
       </c>
     </row>
-    <row r="145" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="145" spans="3:11">
       <c r="C145" t="s">
         <v>208</v>
       </c>
@@ -7688,7 +7856,7 @@
         <v>R-SH_Att_ELC_HPN2</v>
       </c>
     </row>
-    <row r="146" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="146" spans="3:11">
       <c r="C146" t="s">
         <v>208</v>
       </c>
@@ -7708,7 +7876,7 @@
         <v>R-SH_Att_ELC_HPN3</v>
       </c>
     </row>
-    <row r="147" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="147" spans="3:11">
       <c r="C147" t="s">
         <v>208</v>
       </c>
@@ -7728,7 +7896,7 @@
         <v>R-SH_Att_ELC_N1</v>
       </c>
     </row>
-    <row r="148" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="148" spans="3:11">
       <c r="C148" t="s">
         <v>208</v>
       </c>
@@ -7748,7 +7916,7 @@
         <v>R-SH_Att_GAS_N1</v>
       </c>
     </row>
-    <row r="149" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="149" spans="3:11">
       <c r="C149" t="s">
         <v>208</v>
       </c>
@@ -7768,7 +7936,7 @@
         <v>R-SH_Att_KER_N1</v>
       </c>
     </row>
-    <row r="150" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="150" spans="3:11">
       <c r="C150" t="s">
         <v>208</v>
       </c>
@@ -7788,7 +7956,7 @@
         <v>R-SH_Att_LPG_N1</v>
       </c>
     </row>
-    <row r="151" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="151" spans="3:11">
       <c r="C151" t="s">
         <v>208</v>
       </c>
@@ -7808,7 +7976,7 @@
         <v>R-SH_Att_WOO_N1</v>
       </c>
     </row>
-    <row r="152" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="152" spans="3:11">
       <c r="C152" t="s">
         <v>208</v>
       </c>
@@ -7828,7 +7996,7 @@
         <v>R-SH_Det_ELC_HPN1</v>
       </c>
     </row>
-    <row r="153" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="153" spans="3:11">
       <c r="C153" t="s">
         <v>208</v>
       </c>
@@ -7848,7 +8016,7 @@
         <v>R-SH_Det_ELC_HPN2</v>
       </c>
     </row>
-    <row r="154" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="154" spans="3:11">
       <c r="C154" t="s">
         <v>208</v>
       </c>
@@ -7868,7 +8036,7 @@
         <v>R-SH_Det_ELC_HPN3</v>
       </c>
     </row>
-    <row r="155" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="155" spans="3:11">
       <c r="C155" t="s">
         <v>208</v>
       </c>
@@ -7888,7 +8056,7 @@
         <v>R-SH_Det_ELC_N1</v>
       </c>
     </row>
-    <row r="156" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="156" spans="3:11">
       <c r="C156" t="s">
         <v>208</v>
       </c>
@@ -7908,7 +8076,7 @@
         <v>R-SH_Det_GAS_N1</v>
       </c>
     </row>
-    <row r="157" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="157" spans="3:11">
       <c r="C157" t="s">
         <v>208</v>
       </c>
@@ -7928,7 +8096,7 @@
         <v>R-SH_Det_KER_N1</v>
       </c>
     </row>
-    <row r="158" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="158" spans="3:11">
       <c r="C158" t="s">
         <v>208</v>
       </c>
@@ -7948,7 +8116,7 @@
         <v>R-SH_Det_LPG_N1</v>
       </c>
     </row>
-    <row r="159" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="159" spans="3:11">
       <c r="C159" t="s">
         <v>208</v>
       </c>
@@ -7968,7 +8136,7 @@
         <v>R-SH_Det_WOO_N1</v>
       </c>
     </row>
-    <row r="160" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="160" spans="3:11">
       <c r="C160" t="s">
         <v>208</v>
       </c>
@@ -7988,7 +8156,7 @@
         <v>R-WH_Apt_ELC_N1</v>
       </c>
     </row>
-    <row r="161" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="161" spans="3:11">
       <c r="C161" t="s">
         <v>208</v>
       </c>
@@ -8008,7 +8176,7 @@
         <v>R-WH_Apt_SOL_N1</v>
       </c>
     </row>
-    <row r="162" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="162" spans="3:11">
       <c r="C162" t="s">
         <v>208</v>
       </c>
@@ -8028,7 +8196,7 @@
         <v>R-WH_Att_ELC_N1</v>
       </c>
     </row>
-    <row r="163" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="163" spans="3:11">
       <c r="C163" t="s">
         <v>208</v>
       </c>
@@ -8048,7 +8216,7 @@
         <v>R-WH_Att_SOL_N1</v>
       </c>
     </row>
-    <row r="164" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="164" spans="3:11">
       <c r="C164" t="s">
         <v>208</v>
       </c>
@@ -8068,7 +8236,7 @@
         <v>R-WH_Det_ELC_N1</v>
       </c>
     </row>
-    <row r="165" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="165" spans="3:11">
       <c r="C165" t="s">
         <v>208</v>
       </c>
@@ -8088,92 +8256,92 @@
         <v>R-WH_Det_SOL_N1</v>
       </c>
     </row>
-    <row r="166" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="166" spans="3:11">
       <c r="H166" s="26"/>
       <c r="I166" s="26"/>
       <c r="K166" s="26"/>
     </row>
-    <row r="167" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="167" spans="3:11">
       <c r="H167" s="26"/>
       <c r="I167" s="26"/>
       <c r="K167" s="26"/>
     </row>
-    <row r="168" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="168" spans="3:11">
       <c r="H168" s="26"/>
       <c r="I168" s="26"/>
       <c r="K168" s="26"/>
     </row>
-    <row r="169" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="169" spans="3:11">
       <c r="H169" s="26"/>
       <c r="I169" s="26"/>
       <c r="K169" s="26"/>
     </row>
-    <row r="170" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="170" spans="3:11">
       <c r="H170" s="26"/>
       <c r="I170" s="26"/>
       <c r="K170" s="26"/>
     </row>
-    <row r="171" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="171" spans="3:11">
       <c r="H171" s="26"/>
       <c r="I171" s="26"/>
       <c r="K171" s="26"/>
     </row>
-    <row r="172" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="172" spans="3:11">
       <c r="H172" s="26"/>
       <c r="I172" s="26"/>
       <c r="K172" s="26"/>
     </row>
-    <row r="173" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="173" spans="3:11">
       <c r="H173" s="26"/>
       <c r="I173" s="26"/>
       <c r="K173" s="26"/>
     </row>
-    <row r="174" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="174" spans="3:11">
       <c r="H174" s="26"/>
       <c r="I174" s="26"/>
       <c r="K174" s="26"/>
     </row>
-    <row r="175" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="175" spans="3:11">
       <c r="H175" s="26"/>
       <c r="I175" s="26"/>
       <c r="K175" s="26"/>
     </row>
-    <row r="176" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="176" spans="3:11">
       <c r="H176" s="26"/>
       <c r="I176" s="26"/>
       <c r="K176" s="26"/>
     </row>
-    <row r="177" spans="8:11" x14ac:dyDescent="0.25">
+    <row r="177" spans="8:11">
       <c r="H177" s="26"/>
       <c r="I177" s="26"/>
       <c r="K177" s="26"/>
     </row>
-    <row r="178" spans="8:11" x14ac:dyDescent="0.25">
+    <row r="178" spans="8:11">
       <c r="H178" s="26"/>
       <c r="I178" s="26"/>
       <c r="K178" s="26"/>
     </row>
-    <row r="179" spans="8:11" x14ac:dyDescent="0.25">
+    <row r="179" spans="8:11">
       <c r="H179" s="26"/>
       <c r="I179" s="26"/>
       <c r="K179" s="26"/>
     </row>
-    <row r="180" spans="8:11" x14ac:dyDescent="0.25">
+    <row r="180" spans="8:11">
       <c r="H180" s="26"/>
       <c r="I180" s="26"/>
       <c r="K180" s="26"/>
     </row>
-    <row r="181" spans="8:11" x14ac:dyDescent="0.25">
+    <row r="181" spans="8:11">
       <c r="H181" s="26"/>
       <c r="I181" s="26"/>
       <c r="K181" s="26"/>
     </row>
-    <row r="182" spans="8:11" x14ac:dyDescent="0.25">
+    <row r="182" spans="8:11">
       <c r="H182" s="26"/>
       <c r="I182" s="26"/>
       <c r="K182" s="26"/>
     </row>
-    <row r="183" spans="8:11" x14ac:dyDescent="0.25">
+    <row r="183" spans="8:11">
       <c r="H183" s="26"/>
       <c r="I183" s="26"/>
       <c r="K183" s="26"/>
@@ -8196,13 +8364,13 @@
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="13.5703125" customWidth="1"/>
     <col min="6" max="6" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11">
       <c r="B3" s="7" t="s">
         <v>15</v>
       </c>
@@ -8210,7 +8378,7 @@
       <c r="J3" s="9"/>
       <c r="K3" s="9"/>
     </row>
-    <row r="4" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:11" ht="15.75" thickBot="1">
       <c r="B4" s="10" t="s">
         <v>12</v>
       </c>
@@ -8244,7 +8412,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11">
       <c r="D5" t="s">
         <v>247</v>
       </c>
@@ -8272,7 +8440,7 @@
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
@@ -8281,7 +8449,7 @@
     <col min="8" max="9" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9">
       <c r="B3" s="22" t="s">
         <v>209</v>
       </c>
@@ -8291,7 +8459,7 @@
       <c r="F3" s="20"/>
       <c r="G3" s="20"/>
     </row>
-    <row r="4" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:9" ht="15.75" thickBot="1">
       <c r="B4" s="23" t="s">
         <v>106</v>
       </c>
@@ -8314,7 +8482,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9">
       <c r="B5" s="21"/>
       <c r="C5" s="21"/>
       <c r="D5" s="21" t="s">
@@ -8331,7 +8499,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9">
       <c r="B7" s="22" t="s">
         <v>210</v>
       </c>
@@ -8341,7 +8509,7 @@
       <c r="F7" s="20"/>
       <c r="G7" s="20"/>
     </row>
-    <row r="8" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:9" ht="15.75" thickBot="1">
       <c r="B8" s="23" t="s">
         <v>106</v>
       </c>
@@ -8367,7 +8535,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9">
       <c r="B9" s="21"/>
       <c r="C9" s="21"/>
       <c r="D9" s="21" t="s">
@@ -8400,7 +8568,7 @@
       <selection activeCell="A28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
@@ -8408,7 +8576,7 @@
     <col min="8" max="8" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>113</v>
       </c>
@@ -8449,7 +8617,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>124</v>
       </c>
@@ -8490,7 +8658,7 @@
         <v>2.4813655183930802E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>124</v>
       </c>
@@ -8531,7 +8699,7 @@
         <v>2.4813655183930802E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>124</v>
       </c>
@@ -8572,7 +8740,7 @@
         <v>2.4813655183930802E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
         <v>124</v>
       </c>
@@ -8613,7 +8781,7 @@
         <v>2.4813655183930802E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13">
       <c r="A6" t="s">
         <v>124</v>
       </c>
@@ -8654,7 +8822,7 @@
         <v>1.73685782056223E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13">
       <c r="A7" t="s">
         <v>124</v>
       </c>
@@ -8695,7 +8863,7 @@
         <v>1.73685782056223E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13">
       <c r="A8" t="s">
         <v>124</v>
       </c>
@@ -8736,7 +8904,7 @@
         <v>1.73685782056223E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13">
       <c r="A9" t="s">
         <v>124</v>
       </c>
@@ -8777,7 +8945,7 @@
         <v>1.73685782056223E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13">
       <c r="A10" t="s">
         <v>124</v>
       </c>
@@ -8818,7 +8986,7 @@
         <v>3.17870115673878E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13">
       <c r="A11" t="s">
         <v>124</v>
       </c>
@@ -8859,7 +9027,7 @@
         <v>3.17870115673878E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13">
       <c r="A12" t="s">
         <v>124</v>
       </c>
@@ -8900,7 +9068,7 @@
         <v>3.17870115673878E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13">
       <c r="A13" t="s">
         <v>124</v>
       </c>
@@ -8941,7 +9109,7 @@
         <v>3.17870115673878E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13">
       <c r="A14" t="s">
         <v>124</v>
       </c>
@@ -8982,7 +9150,7 @@
         <v>2.0960831834076401E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13">
       <c r="A15" t="s">
         <v>124</v>
       </c>
@@ -9023,7 +9191,7 @@
         <v>2.0960831834076401E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13">
       <c r="A16" t="s">
         <v>124</v>
       </c>
@@ -9064,7 +9232,7 @@
         <v>9.4795012067416702E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13">
       <c r="A17" t="s">
         <v>124</v>
       </c>
@@ -9105,7 +9273,7 @@
         <v>9.4795012067416702E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13">
       <c r="A18" t="s">
         <v>124</v>
       </c>
@@ -9146,7 +9314,7 @@
         <v>9.4795012067416702E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13">
       <c r="A19" t="s">
         <v>124</v>
       </c>
@@ -9187,7 +9355,7 @@
         <v>9.4795012067416702E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13">
       <c r="A20" t="s">
         <v>124</v>
       </c>
@@ -9228,7 +9396,7 @@
         <v>9.4795012067416702E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13">
       <c r="A21" t="s">
         <v>124</v>
       </c>
@@ -9269,7 +9437,7 @@
         <v>9.4795012067416702E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13">
       <c r="A22" t="s">
         <v>124</v>
       </c>
@@ -9310,7 +9478,7 @@
         <v>9.4795012067416702E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13">
       <c r="A23" t="s">
         <v>124</v>
       </c>
@@ -9351,7 +9519,7 @@
         <v>9.4795012067416702E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13">
       <c r="A24" t="s">
         <v>124</v>
       </c>
@@ -9392,7 +9560,7 @@
         <v>7.0869783672800502E-4</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13">
       <c r="A25" t="s">
         <v>124</v>
       </c>
@@ -9433,7 +9601,7 @@
         <v>7.0869783672800502E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13">
       <c r="A26" t="s">
         <v>124</v>
       </c>
@@ -9474,7 +9642,7 @@
         <v>7.0869783672800502E-4</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13">
       <c r="A27" t="s">
         <v>124</v>
       </c>
@@ -9515,7 +9683,7 @@
         <v>7.0869783672800502E-4</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13">
       <c r="A28" t="s">
         <v>124</v>
       </c>
@@ -9556,7 +9724,7 @@
         <v>2.39860043810185E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13">
       <c r="A29" t="s">
         <v>124</v>
       </c>
@@ -9597,7 +9765,7 @@
         <v>2.39860043810185E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13">
       <c r="A30" t="s">
         <v>124</v>
       </c>
@@ -9638,7 +9806,7 @@
         <v>1.78079112619931E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13">
       <c r="A31" t="s">
         <v>124</v>
       </c>
@@ -9679,7 +9847,7 @@
         <v>1.78079112619931E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13">
       <c r="A32" t="s">
         <v>124</v>
       </c>
@@ -9720,7 +9888,7 @@
         <v>1.37038901278922E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13">
       <c r="A33" t="s">
         <v>124</v>
       </c>
@@ -9761,7 +9929,7 @@
         <v>1.37038901278922E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13">
       <c r="A34" t="s">
         <v>124</v>
       </c>
@@ -9802,7 +9970,7 @@
         <v>1.87904155250764E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13">
       <c r="A35" t="s">
         <v>124</v>
       </c>
@@ -9843,7 +10011,7 @@
         <v>1.87904155250764E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13">
       <c r="A36" t="s">
         <v>124</v>
       </c>
@@ -9884,7 +10052,7 @@
         <v>1.87904155250764E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13">
       <c r="A37" t="s">
         <v>124</v>
       </c>
@@ -9925,7 +10093,7 @@
         <v>1.87904155250764E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13">
       <c r="A38" t="s">
         <v>124</v>
       </c>
@@ -9966,7 +10134,7 @@
         <v>1.5651300362142601E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13">
       <c r="A39" t="s">
         <v>124</v>
       </c>
@@ -10007,7 +10175,7 @@
         <v>1.5651300362142601E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13">
       <c r="A40" t="s">
         <v>124</v>
       </c>
@@ -10048,7 +10216,7 @@
         <v>1.5651300362142601E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13">
       <c r="A41" t="s">
         <v>124</v>
       </c>
@@ -10089,7 +10257,7 @@
         <v>1.5651300362142601E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13">
       <c r="A42" t="s">
         <v>124</v>
       </c>
@@ -10130,7 +10298,7 @@
         <v>1.5651300362142601E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13">
       <c r="A43" t="s">
         <v>124</v>
       </c>
@@ -10171,7 +10339,7 @@
         <v>1.5651300362142601E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13">
       <c r="A44" t="s">
         <v>124</v>
       </c>
@@ -10212,7 +10380,7 @@
         <v>1.5651300362142601E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13">
       <c r="A45" t="s">
         <v>124</v>
       </c>
@@ -10253,7 +10421,7 @@
         <v>1.5651300362142601E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13">
       <c r="A46" t="s">
         <v>124</v>
       </c>
@@ -10294,7 +10462,7 @@
         <v>1.5651300362142601E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13">
       <c r="A47" t="s">
         <v>124</v>
       </c>
@@ -10335,7 +10503,7 @@
         <v>1.5651300362142601E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13">
       <c r="A48" t="s">
         <v>124</v>
       </c>
@@ -10376,7 +10544,7 @@
         <v>1.5651300362142601E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13">
       <c r="A49" t="s">
         <v>124</v>
       </c>
@@ -10417,7 +10585,7 @@
         <v>1.5651300362142601E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13">
       <c r="A50" t="s">
         <v>124</v>
       </c>
@@ -10458,7 +10626,7 @@
         <v>7.5978921044014096E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13">
       <c r="A51" t="s">
         <v>124</v>
       </c>
@@ -10499,7 +10667,7 @@
         <v>7.5978921044014096E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13">
       <c r="A52" t="s">
         <v>124</v>
       </c>
@@ -10540,7 +10708,7 @@
         <v>7.5978921044014096E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13">
       <c r="A53" t="s">
         <v>124</v>
       </c>
@@ -10581,7 +10749,7 @@
         <v>7.5978921044014096E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13">
       <c r="A54" t="s">
         <v>124</v>
       </c>
@@ -10622,7 +10790,7 @@
         <v>1.9679944818874001E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13">
       <c r="A55" t="s">
         <v>124</v>
       </c>
@@ -10663,7 +10831,7 @@
         <v>1.9679944818874001E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13">
       <c r="A56" t="s">
         <v>124</v>
       </c>
@@ -10704,7 +10872,7 @@
         <v>1.9679944818874001E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13">
       <c r="A57" t="s">
         <v>124</v>
       </c>
@@ -10745,7 +10913,7 @@
         <v>1.9679944818874001E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13">
       <c r="A58" t="s">
         <v>124</v>
       </c>
@@ -10786,7 +10954,7 @@
         <v>1.9679944818874001E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13">
       <c r="A59" t="s">
         <v>124</v>
       </c>
@@ -10827,7 +10995,7 @@
         <v>1.9679944818874001E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13">
       <c r="A60" t="s">
         <v>124</v>
       </c>
@@ -10868,7 +11036,7 @@
         <v>2.3397171732945601E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13">
       <c r="A61" t="s">
         <v>124</v>
       </c>
@@ -10909,7 +11077,7 @@
         <v>2.3397171732945601E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13">
       <c r="A62" t="s">
         <v>124</v>
       </c>
@@ -10950,7 +11118,7 @@
         <v>4.29559017447428E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13">
       <c r="A63" t="s">
         <v>124</v>
       </c>
@@ -10991,7 +11159,7 @@
         <v>4.29559017447428E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13">
       <c r="A64" t="s">
         <v>124</v>
       </c>
@@ -11032,7 +11200,7 @@
         <v>2.7471447517498498E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13">
       <c r="A65" t="s">
         <v>124</v>
       </c>
@@ -11073,7 +11241,7 @@
         <v>2.7471447517498498E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13">
       <c r="A66" t="s">
         <v>124</v>
       </c>
@@ -11114,7 +11282,7 @@
         <v>2.7471447517498498E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13">
       <c r="A67" t="s">
         <v>124</v>
       </c>
@@ -11155,7 +11323,7 @@
         <v>2.7471447517498498E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13">
       <c r="A68" t="s">
         <v>124</v>
       </c>
@@ -11196,7 +11364,7 @@
         <v>2.4447220258868901E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13">
       <c r="A69" t="s">
         <v>124</v>
       </c>
@@ -11237,7 +11405,7 @@
         <v>2.4447220258868901E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13">
       <c r="A70" t="s">
         <v>124</v>
       </c>
@@ -11278,7 +11446,7 @@
         <v>2.4447220258868901E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13">
       <c r="A71" t="s">
         <v>124</v>
       </c>
@@ -11319,7 +11487,7 @@
         <v>2.4447220258868901E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13">
       <c r="A72" t="s">
         <v>124</v>
       </c>
@@ -11360,7 +11528,7 @@
         <v>2.4447220258868901E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13">
       <c r="A73" t="s">
         <v>124</v>
       </c>
@@ -11401,7 +11569,7 @@
         <v>2.4447220258868901E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13">
       <c r="A74" t="s">
         <v>124</v>
       </c>
@@ -11442,7 +11610,7 @@
         <v>2.4447220258868901E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13">
       <c r="A75" t="s">
         <v>124</v>
       </c>
@@ -11483,7 +11651,7 @@
         <v>2.4447220258868901E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13">
       <c r="A76" t="s">
         <v>124</v>
       </c>
@@ -11524,7 +11692,7 @@
         <v>2.4447220258868901E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13">
       <c r="A77" t="s">
         <v>124</v>
       </c>
@@ -11565,7 +11733,7 @@
         <v>2.4447220258868901E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13">
       <c r="A78" t="s">
         <v>124</v>
       </c>
@@ -11606,7 +11774,7 @@
         <v>2.4447220258868901E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13">
       <c r="A79" t="s">
         <v>124</v>
       </c>
@@ -11647,7 +11815,7 @@
         <v>2.4447220258868901E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13">
       <c r="A80" t="s">
         <v>124</v>
       </c>
@@ -11688,7 +11856,7 @@
         <v>9.5642043609248301E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13">
       <c r="A81" t="s">
         <v>124</v>
       </c>
@@ -11729,7 +11897,7 @@
         <v>9.5642043609248301E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13">
       <c r="A82" t="s">
         <v>124</v>
       </c>
@@ -11770,7 +11938,7 @@
         <v>9.5642043609248301E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13">
       <c r="A83" t="s">
         <v>124</v>
       </c>
@@ -11811,7 +11979,7 @@
         <v>9.5642043609248301E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13">
       <c r="A84" t="s">
         <v>124</v>
       </c>
@@ -11852,7 +12020,7 @@
         <v>3.0079476421251201E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13">
       <c r="A85" t="s">
         <v>124</v>
       </c>
@@ -11893,7 +12061,7 @@
         <v>3.0079476421251201E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13">
       <c r="A86" t="s">
         <v>124</v>
       </c>
@@ -11934,7 +12102,7 @@
         <v>3.0079476421251201E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13">
       <c r="A87" t="s">
         <v>124</v>
       </c>
@@ -11975,7 +12143,7 @@
         <v>3.0079476421251201E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13">
       <c r="A88" t="s">
         <v>124</v>
       </c>
@@ -12016,7 +12184,7 @@
         <v>3.0079476421251201E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13">
       <c r="A89" t="s">
         <v>124</v>
       </c>
@@ -12057,7 +12225,7 @@
         <v>3.0079476421251201E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13">
       <c r="A90" t="s">
         <v>124</v>
       </c>
@@ -12098,7 +12266,7 @@
         <v>4.21939695625516E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13">
       <c r="A91" t="s">
         <v>124</v>
       </c>
@@ -12139,7 +12307,7 @@
         <v>4.21939695625516E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13">
       <c r="A92" t="s">
         <v>124</v>
       </c>
@@ -12180,7 +12348,7 @@
         <v>5.2867897077308497E-2</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13">
       <c r="A93" t="s">
         <v>124</v>
       </c>

</xml_diff>

<commit_message>
Update solar PV bounds
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_Temporary_Fixes.xlsx
+++ b/SuppXLS/Scen_B_Temporary_Fixes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4124E791-F4A8-43E4-B0DF-C7EAB753B312}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B469948-7089-4775-9006-2F71B86B689B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3233" yWindow="8002" windowWidth="20716" windowHeight="13276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="15" r:id="rId1"/>
@@ -1406,6 +1406,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1415,15 +1424,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3893,8 +3893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE79BAD-EA44-47F0-A194-320DE6C9FB50}">
   <dimension ref="B2:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M33" sqref="M33"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4181,13 +4181,13 @@
       </c>
     </row>
     <row r="27" spans="2:15">
-      <c r="C27" s="44" t="str">
+      <c r="C27" s="41" t="str">
         <f>_xlfn.TEXTJOIN(" ",TRUE,"~UC_Sets: R_E:",_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,"")))</f>
         <v>~UC_Sets: R_E: IE,National</v>
       </c>
     </row>
     <row r="28" spans="2:15">
-      <c r="C28" s="44" t="s">
+      <c r="C28" s="41" t="s">
         <v>10</v>
       </c>
     </row>
@@ -4197,43 +4197,43 @@
       </c>
     </row>
     <row r="30" spans="2:15">
-      <c r="C30" s="45" t="s">
+      <c r="C30" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="D30" s="46" t="s">
+      <c r="D30" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="E30" s="46" t="s">
+      <c r="E30" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="F30" s="46" t="s">
+      <c r="F30" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="G30" s="46" t="s">
+      <c r="G30" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="H30" s="47" t="s">
+      <c r="H30" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="I30" s="47" t="s">
+      <c r="I30" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="J30" s="47" t="s">
+      <c r="J30" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="K30" s="47" t="s">
+      <c r="K30" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="L30" s="48" t="s">
+      <c r="L30" s="45" t="s">
         <v>253</v>
       </c>
-      <c r="M30" s="48" t="s">
+      <c r="M30" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="N30" s="48" t="s">
+      <c r="N30" s="45" t="s">
         <v>254</v>
       </c>
-      <c r="O30" s="49" t="s">
+      <c r="O30" s="46" t="s">
         <v>11</v>
       </c>
     </row>
@@ -4241,7 +4241,7 @@
       <c r="C31" t="s">
         <v>255</v>
       </c>
-      <c r="E31" s="50" t="s">
+      <c r="E31" s="47" t="s">
         <v>256</v>
       </c>
       <c r="H31" t="s">
@@ -4267,7 +4267,7 @@
       </c>
     </row>
     <row r="32" spans="2:15">
-      <c r="E32" s="50" t="s">
+      <c r="E32" s="47" t="s">
         <v>256</v>
       </c>
       <c r="H32" t="s">
@@ -4283,11 +4283,11 @@
         <v>1</v>
       </c>
       <c r="M32">
-        <v>9.4499999999999993</v>
+        <v>10.3</v>
       </c>
     </row>
     <row r="33" spans="5:14">
-      <c r="E33" s="50" t="s">
+      <c r="E33" s="47" t="s">
         <v>256</v>
       </c>
       <c r="H33" t="s">
@@ -4305,7 +4305,7 @@
       <c r="M33">
         <v>11.03</v>
       </c>
-      <c r="N33" s="48"/>
+      <c r="N33" s="45"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5269,16 +5269,16 @@
       <c r="L17" s="37"/>
     </row>
     <row r="18" spans="2:19" ht="15.75" thickBot="1">
-      <c r="N18" s="41">
-        <v>2018</v>
-      </c>
-      <c r="O18" s="42"/>
-      <c r="P18" s="43"/>
-      <c r="Q18" s="41">
+      <c r="N18" s="48">
+        <v>2018</v>
+      </c>
+      <c r="O18" s="49"/>
+      <c r="P18" s="50"/>
+      <c r="Q18" s="48">
         <v>2070</v>
       </c>
-      <c r="R18" s="42"/>
-      <c r="S18" s="43"/>
+      <c r="R18" s="49"/>
+      <c r="S18" s="50"/>
     </row>
     <row r="19" spans="2:19">
       <c r="N19" s="29" t="s">

</xml_diff>

<commit_message>
Let loose DH expansion
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_Temporary_Fixes.xlsx
+++ b/SuppXLS/Scen_B_Temporary_Fixes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B469948-7089-4775-9006-2F71B86B689B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{333B76F9-6BD5-4C17-B542-074D3AA5063B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3233" yWindow="8002" windowWidth="20716" windowHeight="13276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="15" r:id="rId1"/>
@@ -882,9 +882,6 @@
     <t>HETC</t>
   </si>
   <si>
-    <t>*GRID*</t>
-  </si>
-  <si>
     <t>IMPBIO*1G*2,IMPBIO*1G*3,IMPBIO*1G*4</t>
   </si>
   <si>
@@ -959,6 +956,9 @@
   </si>
   <si>
     <t>Solar PV potenatial</t>
+  </si>
+  <si>
+    <t>*GRID</t>
   </si>
 </sst>
 </file>
@@ -3893,7 +3893,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE79BAD-EA44-47F0-A194-320DE6C9FB50}">
   <dimension ref="B2:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
@@ -4058,7 +4058,7 @@
         <v>20.6</v>
       </c>
       <c r="I12" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="13" spans="2:13">
@@ -4079,7 +4079,7 @@
         <v>22.7</v>
       </c>
       <c r="I13" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="14" spans="2:13">
@@ -4100,7 +4100,7 @@
         <v>105</v>
       </c>
       <c r="I14" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="15" spans="2:13">
@@ -4121,7 +4121,7 @@
         <v>108</v>
       </c>
       <c r="I15" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="20" spans="2:15">
@@ -4172,7 +4172,7 @@
         <v>2035</v>
       </c>
       <c r="I22" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="26" spans="2:15">
@@ -4225,13 +4225,13 @@
         <v>9</v>
       </c>
       <c r="L30" s="45" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="M30" s="45" t="s">
         <v>17</v>
       </c>
       <c r="N30" s="45" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="O30" s="46" t="s">
         <v>11</v>
@@ -4239,13 +4239,13 @@
     </row>
     <row r="31" spans="2:15">
       <c r="C31" t="s">
+        <v>254</v>
+      </c>
+      <c r="E31" s="47" t="s">
         <v>255</v>
       </c>
-      <c r="E31" s="47" t="s">
+      <c r="H31" t="s">
         <v>256</v>
-      </c>
-      <c r="H31" t="s">
-        <v>257</v>
       </c>
       <c r="J31">
         <v>2020</v>
@@ -4263,15 +4263,15 @@
         <v>15</v>
       </c>
       <c r="O31" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="32" spans="2:15">
       <c r="E32" s="47" t="s">
+        <v>255</v>
+      </c>
+      <c r="H32" t="s">
         <v>256</v>
-      </c>
-      <c r="H32" t="s">
-        <v>257</v>
       </c>
       <c r="J32">
         <v>2030</v>
@@ -4288,10 +4288,10 @@
     </row>
     <row r="33" spans="5:14">
       <c r="E33" s="47" t="s">
+        <v>255</v>
+      </c>
+      <c r="H33" t="s">
         <v>256</v>
-      </c>
-      <c r="H33" t="s">
-        <v>257</v>
       </c>
       <c r="J33">
         <v>2050</v>
@@ -4316,8 +4316,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:L16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:I14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4392,7 +4392,7 @@
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="J5">
         <v>0</v>
@@ -4478,7 +4478,7 @@
         <v>232</v>
       </c>
       <c r="I13" t="s">
-        <v>233</v>
+        <v>258</v>
       </c>
     </row>
     <row r="14" spans="2:12">
@@ -4505,7 +4505,7 @@
       </c>
       <c r="I14" t="str">
         <f>I13</f>
-        <v>*GRID*</v>
+        <v>*GRID</v>
       </c>
     </row>
     <row r="15" spans="2:12">
@@ -4526,7 +4526,7 @@
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="16" spans="2:12">
@@ -4801,7 +4801,7 @@
         <v>0.115</v>
       </c>
       <c r="I5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="6" spans="2:9">
@@ -4822,7 +4822,7 @@
         <v>0.115</v>
       </c>
       <c r="I6" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="7" spans="2:9">
@@ -4843,7 +4843,7 @@
         <v>0.115</v>
       </c>
       <c r="I7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="8" spans="2:9">
@@ -4864,7 +4864,7 @@
         <v>0.115</v>
       </c>
       <c r="I8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="9" spans="2:9">
@@ -4885,7 +4885,7 @@
         <v>0.115</v>
       </c>
       <c r="I9" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="10" spans="2:9">
@@ -4906,7 +4906,7 @@
         <v>0.115</v>
       </c>
       <c r="I10" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="11" spans="2:9">
@@ -4927,7 +4927,7 @@
         <v>0.115</v>
       </c>
       <c r="I11" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="12" spans="2:9">
@@ -4948,7 +4948,7 @@
         <v>0.115</v>
       </c>
       <c r="I12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -5437,7 +5437,7 @@
         <v>10.3</v>
       </c>
       <c r="K25" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="M25" s="25">
         <v>0.5</v>
@@ -5460,7 +5460,7 @@
         <v>0</v>
       </c>
       <c r="K26" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="27" spans="2:19">
@@ -5480,7 +5480,7 @@
         <v>5</v>
       </c>
       <c r="K27" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="28" spans="2:19">
@@ -5500,7 +5500,7 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="K28" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="29" spans="2:19">
@@ -5520,7 +5520,7 @@
         <v>0</v>
       </c>
       <c r="K29" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="30" spans="2:19">
@@ -5540,7 +5540,7 @@
         <v>5</v>
       </c>
       <c r="K30" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="31" spans="2:19">
@@ -8414,16 +8414,16 @@
     </row>
     <row r="5" spans="2:11">
       <c r="D5" t="s">
+        <v>246</v>
+      </c>
+      <c r="H5" t="s">
         <v>247</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
+        <v>247</v>
+      </c>
+      <c r="K5" t="s">
         <v>248</v>
-      </c>
-      <c r="I5" t="s">
-        <v>248</v>
-      </c>
-      <c r="K5" t="s">
-        <v>249</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove bounds on FTs from Temporary_Fixes and SRV VT
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_Temporary_Fixes.xlsx
+++ b/SuppXLS/Scen_B_Temporary_Fixes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{333B76F9-6BD5-4C17-B542-074D3AA5063B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C16D90-6D3F-4132-932D-37D61307A508}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3233" yWindow="8002" windowWidth="20716" windowHeight="13276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="15" r:id="rId1"/>
@@ -161,7 +161,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1859" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1847" uniqueCount="256">
   <si>
     <t>UC_N</t>
   </si>
@@ -928,15 +928,6 @@
   </si>
   <si>
     <t>T-CAR*1</t>
-  </si>
-  <si>
-    <t>FT-PWRCOA</t>
-  </si>
-  <si>
-    <t>FT-PWRGAS</t>
-  </si>
-  <si>
-    <t>FT-PWRPEA</t>
   </si>
   <si>
     <t>UC_FLO</t>
@@ -3891,10 +3882,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE79BAD-EA44-47F0-A194-320DE6C9FB50}">
-  <dimension ref="B2:O33"/>
+  <dimension ref="B2:O29"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3985,7 +3976,7 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <f t="shared" ref="G8:G15" si="0">F8</f>
+        <f t="shared" ref="G8:G11" si="0">F8</f>
         <v>0</v>
       </c>
       <c r="H8" t="s">
@@ -4040,272 +4031,188 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="2:13">
-      <c r="C12" t="s">
-        <v>83</v>
-      </c>
-      <c r="D12" t="s">
-        <v>229</v>
-      </c>
-      <c r="E12">
-        <v>2018</v>
-      </c>
-      <c r="F12">
-        <v>20.6</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="0"/>
-        <v>20.6</v>
-      </c>
-      <c r="I12" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="13" spans="2:13">
-      <c r="C13" t="s">
-        <v>83</v>
-      </c>
-      <c r="D13" t="s">
-        <v>229</v>
-      </c>
-      <c r="E13">
-        <v>2018</v>
-      </c>
-      <c r="F13">
-        <v>22.7</v>
-      </c>
-      <c r="G13">
-        <f t="shared" si="0"/>
-        <v>22.7</v>
-      </c>
-      <c r="I13" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="14" spans="2:13">
-      <c r="C14" t="s">
-        <v>83</v>
-      </c>
-      <c r="D14" t="s">
-        <v>229</v>
-      </c>
-      <c r="E14">
-        <v>2018</v>
-      </c>
-      <c r="F14">
-        <v>105</v>
-      </c>
-      <c r="G14">
-        <f t="shared" si="0"/>
-        <v>105</v>
-      </c>
-      <c r="I14" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="15" spans="2:13">
-      <c r="C15" t="s">
-        <v>83</v>
-      </c>
-      <c r="D15" t="s">
-        <v>229</v>
-      </c>
-      <c r="E15">
-        <v>2020</v>
-      </c>
-      <c r="F15">
-        <v>108</v>
-      </c>
-      <c r="G15">
-        <f t="shared" si="0"/>
-        <v>108</v>
-      </c>
-      <c r="I15" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="20" spans="2:15">
-      <c r="B20" s="7" t="s">
+    <row r="16" spans="2:13">
+      <c r="B16" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="2:15" ht="15.75" thickBot="1">
-      <c r="B21" s="10" t="s">
+    <row r="17" spans="2:15" ht="15.75" thickBot="1">
+      <c r="B17" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C17" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D17" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E17" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F21" s="11" t="str">
+      <c r="F17" s="11" t="str">
         <f>IF(Regions!C$3&lt;&gt;"",Regions!C$3,"*")</f>
         <v>IE</v>
       </c>
-      <c r="G21" s="11" t="str">
+      <c r="G17" s="11" t="str">
         <f>IF(Regions!D$3&lt;&gt;"",Regions!D$3,"*")</f>
         <v>National</v>
       </c>
-      <c r="H21" s="12" t="s">
+      <c r="H17" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I21" s="12" t="s">
+      <c r="I17" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="J21" s="12" t="s">
+      <c r="J17" s="12" t="s">
         <v>5</v>
       </c>
     </row>
+    <row r="18" spans="2:15">
+      <c r="D18" t="s">
+        <v>79</v>
+      </c>
+      <c r="F18">
+        <v>2035</v>
+      </c>
+      <c r="G18">
+        <f>F18</f>
+        <v>2035</v>
+      </c>
+      <c r="I18" t="s">
+        <v>235</v>
+      </c>
+    </row>
     <row r="22" spans="2:15">
-      <c r="D22" t="s">
-        <v>79</v>
-      </c>
-      <c r="F22">
-        <v>2035</v>
-      </c>
-      <c r="G22">
-        <f>F22</f>
-        <v>2035</v>
-      </c>
-      <c r="I22" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="26" spans="2:15">
-      <c r="B26" t="s">
+      <c r="B22" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="2:15">
-      <c r="C27" s="41" t="str">
+    <row r="23" spans="2:15">
+      <c r="C23" s="41" t="str">
         <f>_xlfn.TEXTJOIN(" ",TRUE,"~UC_Sets: R_E:",_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,"")))</f>
         <v>~UC_Sets: R_E: IE,National</v>
       </c>
     </row>
+    <row r="24" spans="2:15">
+      <c r="C24" s="41" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="2:15">
+      <c r="K25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="2:15">
+      <c r="C26" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="E26" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="F26" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="G26" s="43" t="s">
+        <v>6</v>
+      </c>
+      <c r="H26" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="I26" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="J26" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="K26" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="L26" s="45" t="s">
+        <v>249</v>
+      </c>
+      <c r="M26" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="N26" s="45" t="s">
+        <v>250</v>
+      </c>
+      <c r="O26" s="46" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="2:15">
+      <c r="C27" t="s">
+        <v>251</v>
+      </c>
+      <c r="E27" s="47" t="s">
+        <v>252</v>
+      </c>
+      <c r="H27" t="s">
+        <v>253</v>
+      </c>
+      <c r="J27">
+        <v>2020</v>
+      </c>
+      <c r="K27" t="s">
+        <v>83</v>
+      </c>
+      <c r="L27">
+        <v>1</v>
+      </c>
+      <c r="M27">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="N27">
+        <v>15</v>
+      </c>
+      <c r="O27" t="s">
+        <v>254</v>
+      </c>
+    </row>
     <row r="28" spans="2:15">
-      <c r="C28" s="41" t="s">
-        <v>10</v>
+      <c r="E28" s="47" t="s">
+        <v>252</v>
+      </c>
+      <c r="H28" t="s">
+        <v>253</v>
+      </c>
+      <c r="J28">
+        <v>2030</v>
+      </c>
+      <c r="K28" t="s">
+        <v>83</v>
+      </c>
+      <c r="L28">
+        <v>1</v>
+      </c>
+      <c r="M28">
+        <v>10.3</v>
       </c>
     </row>
     <row r="29" spans="2:15">
+      <c r="E29" s="47" t="s">
+        <v>252</v>
+      </c>
+      <c r="H29" t="s">
+        <v>253</v>
+      </c>
+      <c r="J29">
+        <v>2050</v>
+      </c>
       <c r="K29" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="2:15">
-      <c r="C30" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="D30" s="43" t="s">
-        <v>4</v>
-      </c>
-      <c r="E30" s="43" t="s">
-        <v>3</v>
-      </c>
-      <c r="F30" s="43" t="s">
+        <v>83</v>
+      </c>
+      <c r="L29">
         <v>1</v>
       </c>
-      <c r="G30" s="43" t="s">
-        <v>6</v>
-      </c>
-      <c r="H30" s="44" t="s">
-        <v>5</v>
-      </c>
-      <c r="I30" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="J30" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="K30" s="44" t="s">
-        <v>9</v>
-      </c>
-      <c r="L30" s="45" t="s">
-        <v>252</v>
-      </c>
-      <c r="M30" s="45" t="s">
-        <v>17</v>
-      </c>
-      <c r="N30" s="45" t="s">
-        <v>253</v>
-      </c>
-      <c r="O30" s="46" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="31" spans="2:15">
-      <c r="C31" t="s">
-        <v>254</v>
-      </c>
-      <c r="E31" s="47" t="s">
-        <v>255</v>
-      </c>
-      <c r="H31" t="s">
-        <v>256</v>
-      </c>
-      <c r="J31">
-        <v>2020</v>
-      </c>
-      <c r="K31" t="s">
-        <v>83</v>
-      </c>
-      <c r="L31">
-        <v>1</v>
-      </c>
-      <c r="M31">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="N31">
-        <v>15</v>
-      </c>
-      <c r="O31" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="32" spans="2:15">
-      <c r="E32" s="47" t="s">
-        <v>255</v>
-      </c>
-      <c r="H32" t="s">
-        <v>256</v>
-      </c>
-      <c r="J32">
-        <v>2030</v>
-      </c>
-      <c r="K32" t="s">
-        <v>83</v>
-      </c>
-      <c r="L32">
-        <v>1</v>
-      </c>
-      <c r="M32">
-        <v>10.3</v>
-      </c>
-    </row>
-    <row r="33" spans="5:14">
-      <c r="E33" s="47" t="s">
-        <v>255</v>
-      </c>
-      <c r="H33" t="s">
-        <v>256</v>
-      </c>
-      <c r="J33">
-        <v>2050</v>
-      </c>
-      <c r="K33" t="s">
-        <v>83</v>
-      </c>
-      <c r="L33">
-        <v>1</v>
-      </c>
-      <c r="M33">
+      <c r="M29">
         <v>11.03</v>
       </c>
-      <c r="N33" s="45"/>
+      <c r="N29" s="45"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4316,7 +4223,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
@@ -4478,7 +4385,7 @@
         <v>232</v>
       </c>
       <c r="I13" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="14" spans="2:12">

</xml_diff>

<commit_message>
Activate early retirement for new detached houses
- to avoid dummy imports in 2040 which is caused by a drop in demand in 2041 (combined with NCAP_AF~FX and inability to overproduce the demand)
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_Temporary_Fixes.xlsx
+++ b/SuppXLS/Scen_B_Temporary_Fixes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E7085FA-7D6C-4A37-B296-C61CD9FA7A70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D84EE04C-1297-43E1-95C8-D488C1F5A968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4770" yWindow="1455" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="15" r:id="rId1"/>
@@ -162,7 +162,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1857" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1860" uniqueCount="261">
   <si>
     <t>UC_N</t>
   </si>
@@ -957,6 +957,15 @@
   </si>
   <si>
     <t>val_cond</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>RCAP_BND</t>
+  </si>
+  <si>
+    <t>R-BLD_Det-N1</t>
   </si>
 </sst>
 </file>
@@ -1337,7 +1346,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1422,6 +1431,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8064,7 +8074,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DE4666E-C19A-4073-8183-3ACBB585B13C}">
   <dimension ref="B2:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
@@ -8783,8 +8793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{209CF89D-3AC9-4E2E-BCF6-79A710F8BD8A}">
   <dimension ref="A1:S183"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23:K24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9367,8 +9377,21 @@
       </c>
     </row>
     <row r="31" spans="2:19">
-      <c r="H31" s="26"/>
-      <c r="I31" s="26"/>
+      <c r="C31" t="s">
+        <v>258</v>
+      </c>
+      <c r="D31" t="s">
+        <v>259</v>
+      </c>
+      <c r="H31" s="51">
+        <v>0</v>
+      </c>
+      <c r="I31" s="51">
+        <v>0</v>
+      </c>
+      <c r="K31" t="s">
+        <v>260</v>
+      </c>
     </row>
     <row r="32" spans="2:19">
       <c r="H32" s="26"/>

</xml_diff>